<commit_message>
simplify IG / remove yaml
not yet stabilised, remove yaml
</commit_message>
<xml_diff>
--- a/tools/excel/anssi/anssi-mon-aide-cyber.xlsx
+++ b/tools/excel/anssi/anssi-mon-aide-cyber.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/excel/anssi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5155AF71-4DCD-244D-86C0-7144CAE4BDB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{119939E8-C715-4C49-8740-26B3E1EA366A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="34560" windowHeight="20500" tabRatio="882" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="34560" windowHeight="20500" tabRatio="882" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_meta" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="562">
   <si>
     <t>type</t>
   </si>
@@ -203,16 +203,10 @@
     <t>contexte-cyber-attaque-subie-oui-tiroir-type</t>
   </si>
   <si>
-    <t>_Q8.1_DEPENDS_ON_contexte-cyber-attaque-subie</t>
-  </si>
-  <si>
     <t>Si oui, de quel type ?</t>
   </si>
   <si>
     <t>contexte-cyber-attaque-subie-tiroir-plainte</t>
-  </si>
-  <si>
-    <t>_Q8.2_DEPENDS_ON_contexte-cyber-attaque-subie</t>
   </si>
   <si>
     <t>Si Oui : avez-vous déposé plainte ou réalisé un signalement auprès d'un service judiciaire ?</t>
@@ -253,10 +247,6 @@
     <t>SYSTÈME INDUSTRIEL</t>
   </si>
   <si>
-    <t>SYSTEME-INDUSTRIEL,
-_DEPENDS_ON_contexte-opere-systemes-information-industriels</t>
-  </si>
-  <si>
     <t>Existe-t-il un plan et un inventaire des systèmes d'informations industriels de l'entité ?</t>
   </si>
   <si>
@@ -306,10 +296,6 @@
     <t>acces-outil-gestion-des-comptes</t>
   </si>
   <si>
-    <t>_DEPENDS_ON_contexte-nombre-postes-travail-dans-entite,
-_DEPENDS_ON_contexte-nombre-postes-travail-dans-organisation</t>
-  </si>
-  <si>
     <t>Un outil de gestion des comptes et des politiques de sécurité centralisé (ex : Active Directory, Samba-AD, Entra ID, scripts d'administration automatisés, etc.) est-il mis en œuvre ?</t>
   </si>
   <si>
@@ -323,10 +309,6 @@
     <t>ATTAQUE CIBLÉE</t>
   </si>
   <si>
-    <t>ATTAQUE-CIBLEE,
-_DEPENDS_ON_contexte-activites-recherche-et-developpement</t>
-  </si>
-  <si>
     <t>La liste des comptes utilisateurs (prestataires inclus) est-elle maintenue à jour ?</t>
   </si>
   <si>
@@ -518,9 +500,6 @@
     <t>securite-infrastructure-pare-feu-deploye-oui-tiroir-interconnexions-protegees</t>
   </si>
   <si>
-    <t>_Q33.1_DEPENDS_ON_securite-infrastructure-pare-feu-deploye</t>
-  </si>
-  <si>
     <t>Est-ce que seuls les flux entrants et sortants strictement nécessaires entre Internet et le système d'information (ou autres réseaux externes) sont autorisés ?</t>
   </si>
   <si>
@@ -529,9 +508,6 @@
   </si>
   <si>
     <t>securite-infrastructure-pare-feu-deploye-oui-tiroir-logs-stockes</t>
-  </si>
-  <si>
-    <t>_Q33.2_DEPENDS_ON_securite-infrastructure-pare-feu-deploye</t>
   </si>
   <si>
     <t>Les journaux des flux entrants, sortants et bloqués (générés par le pare-feu) sont-ils stockés ?</t>
@@ -670,9 +646,6 @@
     <t>reaction-sauvegardes-donnees-realisees-oui-ponctuellement-tiroir-environnement-isole</t>
   </si>
   <si>
-    <t>_Q44.1_DEPENDS_ON_reaction-sauvegardes-donnees-realisees</t>
-  </si>
-  <si>
     <t>Existe-t-il au moins un jeu de sauvegarde des données critiques stockées dans un environnement isolé du réseau bureautique interne ou "hors ligne" ?</t>
   </si>
   <si>
@@ -682,9 +655,6 @@
     <t>reaction-sauvegardes-donnees-realisees-oui-ponctuellement-tiroir-sauvegarde-testee-regulierement</t>
   </si>
   <si>
-    <t>_Q44.2_DEPENDS_ON_reaction-sauvegardes-donnees-realisees</t>
-  </si>
-  <si>
     <t>Si "Oui" : La restauration des sauvegardes de toutes vos données critiques est-elle testée régulièrement ?</t>
   </si>
   <si>
@@ -694,9 +664,6 @@
     <t>reaction-sauvegardes-donnees-realisees-oui-automatique-et-reguliere-tiroir-environnement-isole</t>
   </si>
   <si>
-    <t>_Q44.3_DEPENDS_ON_reaction-sauvegardes-donnees-realisees</t>
-  </si>
-  <si>
     <t>Existe-t-il au moins un jeu de sauvegarde des données critiques stockées dans un environnement isolé du réseau bureautique interne ou "hors ligne"</t>
   </si>
   <si>
@@ -704,9 +671,6 @@
   </si>
   <si>
     <t>reaction-sauvegardes-donnees-realisees-oui-automatique-et-reguliere-tiroir-sauvegarde-testee-regulierement</t>
-  </si>
-  <si>
-    <t>_Q44.4_DEPENDS_ON_reaction-sauvegardes-donnees-realisees</t>
   </si>
   <si>
     <t>La restauration des sauvegardes de toutes vos données critiques est-elle testée régulièrement ?</t>
@@ -889,30 +853,9 @@
 Plus de 250</t>
   </si>
   <si>
-    <t>/
-_DEPENDS_ON_contexte-nombre-postes-travail-dans-entite
-_DEPENDS_ON_contexte-nombre-postes-travail-dans-entite
-_DEPENDS_ON_contexte-nombre-postes-travail-dans-entite</t>
-  </si>
-  <si>
     <t>Je ne sais pas
 Non
 Oui</t>
-  </si>
-  <si>
-    <t>_DEPENDS_ON_contexte-activites-recherche-et-developpement
-/
-_DEPENDS_ON_contexte-activites-recherche-et-developpement</t>
-  </si>
-  <si>
-    <t>_DEPENDS_ON_contexte-opere-systemes-information-industriels
-/
-_DEPENDS_ON_contexte-opere-systemes-information-industriels</t>
-  </si>
-  <si>
-    <t>/
-/
-_Q8.1_DEPENDS_ON_contexte-cyber-attaque-subie, _Q8.2_DEPENDS_ON_contexte-cyber-attaque-subie</t>
   </si>
   <si>
     <t>multiple_choice</t>
@@ -1068,11 +1011,6 @@
 Oui, un outil de type EDR a été mis en place et ses alertes sont systématiquement traitées</t>
   </si>
   <si>
-    <t>/
-/
-_Q33.1_DEPENDS_ON_securite-infrastructure-pare-feu-deploye, _Q33.2_DEPENDS_ON_securite-infrastructure-pare-feu-deploye</t>
-  </si>
-  <si>
     <t>Je ne sais pas
 Non
 Oui
@@ -1143,12 +1081,6 @@
 Des sauvegardes des données sont réalisées de manière automatique et régulière</t>
   </si>
   <si>
-    <t>/
-/
-_Q44.1_DEPENDS_ON_reaction-sauvegardes-donnees-realisees, _Q44.2_DEPENDS_ON_reaction-sauvegardes-donnees-realisees
-_Q44.3_DEPENDS_ON_reaction-sauvegardes-donnees-realisees, _Q44.4_DEPENDS_ON_reaction-sauvegardes-donnees-realisees</t>
-  </si>
-  <si>
     <t>Je ne sais pas
 Non
 Oui, nous avons formalisé une fiche réflexe dédiée
@@ -1165,18 +1097,6 @@
   </si>
   <si>
     <t>ATTAQUE-CIBLEE</t>
-  </si>
-  <si>
-    <t>_DEPENDS_ON_contexte-opere-systemes-information-industriels</t>
-  </si>
-  <si>
-    <t>_DEPENDS_ON_contexte-activites-recherche-et-developpement</t>
-  </si>
-  <si>
-    <t>_DEPENDS_ON_contexte-nombre-postes-travail-dans-entite</t>
-  </si>
-  <si>
-    <t>_DEPENDS_ON_contexte-nombre-postes-travail-dans-organisation</t>
   </si>
   <si>
     <t>urn:intuitem:risk:function:anssi-monaidecyber</t>
@@ -2639,6 +2559,74 @@
   <si>
     <t>## Organisation de gestion de crise
 Une organisation de gestion de crise doit à minima identifier les priorités métier à rétablir en cas de crise, des fiches réflexes opérationnelles garantissant la continuité d'activité au travers de modes dégradés défini avec les métiers (ex : assurer la paie, poursuivre la production, gestion des agendas, etc.), des moyens et modalités de communication de crise.</t>
+  </si>
+  <si>
+    <t>DEPENDS_ON_contexte-cyber-attaque-subie</t>
+  </si>
+  <si>
+    <t>DEPENDS_ON_securite-infrastructure-pare-feu-deploye</t>
+  </si>
+  <si>
+    <t>SYSTEME-INDUSTRIEL,
+DEPENDS_ON_contexte-opere-systemes-information-industriels</t>
+  </si>
+  <si>
+    <t>DEPENDS_ON_contexte-nombre-postes-travail-dans-entite,
+DEPENDS_ON_contexte-nombre-postes-travail-dans-organisation</t>
+  </si>
+  <si>
+    <t>ATTAQUE-CIBLEE,
+DEPENDS_ON_contexte-activites-recherche-et-developpement</t>
+  </si>
+  <si>
+    <t>/
+DEPENDS_ON_contexte-nombre-postes-travail-dans-entite
+DEPENDS_ON_contexte-nombre-postes-travail-dans-entite
+DEPENDS_ON_contexte-nombre-postes-travail-dans-entite</t>
+  </si>
+  <si>
+    <t>DEPENDS_ON_contexte-activites-recherche-et-developpement
+/
+DEPENDS_ON_contexte-activites-recherche-et-developpement</t>
+  </si>
+  <si>
+    <t>DEPENDS_ON_contexte-opere-systemes-information-industriels
+/
+DEPENDS_ON_contexte-opere-systemes-information-industriels</t>
+  </si>
+  <si>
+    <t>DEPENDS_ON_contexte-opere-systemes-information-industriels</t>
+  </si>
+  <si>
+    <t>DEPENDS_ON_contexte-activites-recherche-et-developpement</t>
+  </si>
+  <si>
+    <t>DEPENDS_ON_contexte-nombre-postes-travail-dans-entite</t>
+  </si>
+  <si>
+    <t>DEPENDS_ON_contexte-nombre-postes-travail-dans-organisation</t>
+  </si>
+  <si>
+    <t>/
+/
+DEPENDS_ON_contexte-cyber-attaque-subie</t>
+  </si>
+  <si>
+    <t>/
+/
+DEPENDS_ON_securite-infrastructure-pare-feu-deploye</t>
+  </si>
+  <si>
+    <t>DEPENDS_ON_reaction-sauvegardes-donnees-realisees-ponctuellement</t>
+  </si>
+  <si>
+    <t>DEPENDS_ON_reaction-sauvegardes-donnees-realisees-regulierement</t>
+  </si>
+  <si>
+    <t>/
+/
+DEPENDS_ON_reaction-sauvegardes-donnees-realisees-ponctuellement
+DEPENDS_ON_reaction-sauvegardes-donnees-realisees-regulierement</t>
   </si>
 </sst>
 </file>
@@ -2987,7 +2975,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="212" workbookViewId="0">
+    <sheetView zoomScale="212" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -3018,7 +3006,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -3050,7 +3038,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>524</v>
+        <v>503</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="224" x14ac:dyDescent="0.2">
@@ -3058,7 +3046,7 @@
         <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>526</v>
+        <v>505</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -3100,7 +3088,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>496</v>
+        <v>475</v>
       </c>
     </row>
   </sheetData>
@@ -3123,10 +3111,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>497</v>
+        <v>476</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>498</v>
+        <v>477</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -3134,7 +3122,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>281</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -3201,7 +3189,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>524</v>
+        <v>503</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -3229,8 +3217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="186" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="186" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="J60" sqref="J60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3256,7 +3244,7 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>525</v>
+        <v>504</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>10</v>
@@ -3317,7 +3305,7 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
-        <v>527</v>
+        <v>506</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2" t="s">
@@ -3344,7 +3332,7 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
-        <v>528</v>
+        <v>507</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2" t="s">
@@ -3421,7 +3409,7 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
-        <v>529</v>
+        <v>508</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2" t="s">
@@ -3448,7 +3436,7 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2" t="s">
-        <v>530</v>
+        <v>509</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2" t="s">
@@ -3475,7 +3463,7 @@
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2" t="s">
-        <v>531</v>
+        <v>510</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2" t="s">
@@ -3502,7 +3490,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2" t="s">
-        <v>532</v>
+        <v>511</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2" t="s">
@@ -3531,10 +3519,10 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>56</v>
@@ -3549,20 +3537,20 @@
         <v>38</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2" t="s">
-        <v>60</v>
+        <v>545</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K12" s="2"/>
     </row>
@@ -3572,13 +3560,13 @@
         <v>5</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -3595,25 +3583,25 @@
         <v>38</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
-        <v>533</v>
+        <v>512</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2" t="s">
         <v>40</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J14" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K14" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="128" x14ac:dyDescent="0.2">
@@ -3624,25 +3612,25 @@
         <v>38</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
-        <v>534</v>
+        <v>513</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2" t="s">
         <v>40</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J15" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="K15" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="96" x14ac:dyDescent="0.2">
@@ -3653,25 +3641,25 @@
         <v>38</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
-        <v>535</v>
+        <v>514</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2" t="s">
-        <v>73</v>
+        <v>547</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="192" x14ac:dyDescent="0.2">
@@ -3682,25 +3670,25 @@
         <v>38</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
-        <v>536</v>
+        <v>515</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2" t="s">
         <v>40</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="64" x14ac:dyDescent="0.2">
@@ -3711,25 +3699,25 @@
         <v>38</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2" t="s">
-        <v>537</v>
+        <v>516</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2" t="s">
         <v>40</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="176" x14ac:dyDescent="0.2">
@@ -3740,25 +3728,25 @@
         <v>38</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2" t="s">
-        <v>538</v>
+        <v>517</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2" t="s">
         <v>40</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="48" x14ac:dyDescent="0.2">
@@ -3767,13 +3755,13 @@
         <v>5</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -3790,25 +3778,25 @@
         <v>38</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2" t="s">
-        <v>539</v>
+        <v>518</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2" t="s">
-        <v>89</v>
+        <v>548</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="96" x14ac:dyDescent="0.2">
@@ -3819,25 +3807,25 @@
         <v>38</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2" t="s">
-        <v>540</v>
+        <v>519</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2" t="s">
-        <v>94</v>
+        <v>549</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="96" x14ac:dyDescent="0.2">
@@ -3848,25 +3836,25 @@
         <v>38</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2" t="s">
-        <v>540</v>
+        <v>519</v>
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K23" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="112" x14ac:dyDescent="0.2">
@@ -3877,25 +3865,25 @@
         <v>38</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2" t="s">
-        <v>541</v>
+        <v>520</v>
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2" t="s">
         <v>40</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="112" x14ac:dyDescent="0.2">
@@ -3906,25 +3894,25 @@
         <v>38</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2" t="s">
-        <v>542</v>
+        <v>521</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2" t="s">
         <v>40</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="64" x14ac:dyDescent="0.2">
@@ -3935,25 +3923,25 @@
         <v>38</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2" t="s">
-        <v>543</v>
+        <v>522</v>
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2" t="s">
         <v>40</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="160" x14ac:dyDescent="0.2">
@@ -3964,25 +3952,25 @@
         <v>38</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2" t="s">
-        <v>544</v>
+        <v>523</v>
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2" t="s">
         <v>40</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="176" x14ac:dyDescent="0.2">
@@ -3993,25 +3981,25 @@
         <v>38</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2" t="s">
-        <v>545</v>
+        <v>524</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2" t="s">
-        <v>94</v>
+        <v>549</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="112" x14ac:dyDescent="0.2">
@@ -4022,25 +4010,25 @@
         <v>38</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2" t="s">
-        <v>546</v>
+        <v>525</v>
       </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2" t="s">
         <v>40</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="32" x14ac:dyDescent="0.2">
@@ -4051,25 +4039,25 @@
         <v>38</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2" t="s">
-        <v>547</v>
+        <v>526</v>
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2" t="s">
-        <v>73</v>
+        <v>547</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="128" x14ac:dyDescent="0.2">
@@ -4080,25 +4068,25 @@
         <v>38</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2" t="s">
-        <v>548</v>
+        <v>527</v>
       </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2" t="s">
         <v>40</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="48" x14ac:dyDescent="0.2">
@@ -4107,11 +4095,11 @@
         <v>5</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
@@ -4128,25 +4116,25 @@
         <v>38</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2" t="s">
-        <v>549</v>
+        <v>528</v>
       </c>
       <c r="G33" s="2"/>
       <c r="H33" s="2" t="s">
         <v>40</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="32" x14ac:dyDescent="0.2">
@@ -4157,25 +4145,25 @@
         <v>38</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2" t="s">
-        <v>547</v>
+        <v>526</v>
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2" t="s">
-        <v>73</v>
+        <v>547</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="112" x14ac:dyDescent="0.2">
@@ -4186,25 +4174,25 @@
         <v>38</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2" t="s">
-        <v>550</v>
+        <v>529</v>
       </c>
       <c r="G35" s="2"/>
       <c r="H35" s="2" t="s">
         <v>40</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="32" x14ac:dyDescent="0.2">
@@ -4215,25 +4203,25 @@
         <v>38</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2" t="s">
-        <v>547</v>
+        <v>526</v>
       </c>
       <c r="G36" s="2"/>
       <c r="H36" s="2" t="s">
-        <v>73</v>
+        <v>547</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="96" x14ac:dyDescent="0.2">
@@ -4244,25 +4232,25 @@
         <v>38</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2" t="s">
-        <v>551</v>
+        <v>530</v>
       </c>
       <c r="G37" s="2"/>
       <c r="H37" s="2" t="s">
         <v>40</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="48" x14ac:dyDescent="0.2">
@@ -4273,25 +4261,25 @@
         <v>38</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2" t="s">
-        <v>552</v>
+        <v>531</v>
       </c>
       <c r="G38" s="2"/>
       <c r="H38" s="2" t="s">
         <v>40</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="240" x14ac:dyDescent="0.2">
@@ -4302,25 +4290,25 @@
         <v>38</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2" t="s">
-        <v>553</v>
+        <v>532</v>
       </c>
       <c r="G39" s="2"/>
       <c r="H39" s="2" t="s">
-        <v>94</v>
+        <v>549</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="48" x14ac:dyDescent="0.2">
@@ -4329,13 +4317,13 @@
         <v>5</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
@@ -4352,25 +4340,25 @@
         <v>38</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2" t="s">
-        <v>554</v>
+        <v>533</v>
       </c>
       <c r="G41" s="2"/>
       <c r="H41" s="2" t="s">
         <v>40</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="32" x14ac:dyDescent="0.2">
@@ -4381,23 +4369,23 @@
         <v>38</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2" t="s">
-        <v>155</v>
+        <v>546</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -4408,23 +4396,23 @@
         <v>38</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2" t="s">
-        <v>159</v>
+        <v>546</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="112" x14ac:dyDescent="0.2">
@@ -4435,25 +4423,25 @@
         <v>38</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
       <c r="F44" s="2" t="s">
-        <v>555</v>
+        <v>534</v>
       </c>
       <c r="G44" s="2"/>
       <c r="H44" s="2" t="s">
-        <v>73</v>
+        <v>547</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="96" x14ac:dyDescent="0.2">
@@ -4464,25 +4452,25 @@
         <v>38</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
       <c r="F45" s="2" t="s">
-        <v>556</v>
+        <v>535</v>
       </c>
       <c r="G45" s="2"/>
       <c r="H45" s="2" t="s">
         <v>40</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="208" x14ac:dyDescent="0.2">
@@ -4493,25 +4481,25 @@
         <v>38</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2" t="s">
-        <v>557</v>
+        <v>536</v>
       </c>
       <c r="G46" s="2"/>
       <c r="H46" s="2" t="s">
         <v>40</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="144" x14ac:dyDescent="0.2">
@@ -4522,25 +4510,25 @@
         <v>38</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
       <c r="F47" s="2" t="s">
-        <v>558</v>
+        <v>537</v>
       </c>
       <c r="G47" s="2"/>
       <c r="H47" s="2" t="s">
         <v>40</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="128" x14ac:dyDescent="0.2">
@@ -4551,25 +4539,25 @@
         <v>38</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
       <c r="F48" s="2" t="s">
-        <v>559</v>
+        <v>538</v>
       </c>
       <c r="G48" s="2"/>
       <c r="H48" s="2" t="s">
-        <v>94</v>
+        <v>549</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="144" x14ac:dyDescent="0.2">
@@ -4580,25 +4568,25 @@
         <v>38</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
       <c r="F49" s="2" t="s">
-        <v>560</v>
+        <v>539</v>
       </c>
       <c r="G49" s="2"/>
       <c r="H49" s="2" t="s">
-        <v>94</v>
+        <v>549</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="64" x14ac:dyDescent="0.2">
@@ -4607,13 +4595,13 @@
         <v>5</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
@@ -4630,25 +4618,25 @@
         <v>38</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
       <c r="F51" s="2" t="s">
-        <v>561</v>
+        <v>540</v>
       </c>
       <c r="G51" s="2"/>
       <c r="H51" s="2" t="s">
         <v>40</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="96" x14ac:dyDescent="0.2">
@@ -4659,25 +4647,25 @@
         <v>38</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
       <c r="F52" s="2" t="s">
-        <v>562</v>
+        <v>541</v>
       </c>
       <c r="G52" s="2"/>
       <c r="H52" s="2" t="s">
-        <v>94</v>
+        <v>549</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="32" x14ac:dyDescent="0.2">
@@ -4688,23 +4676,23 @@
         <v>38</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
       <c r="H53" s="2" t="s">
-        <v>89</v>
+        <v>548</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="48" x14ac:dyDescent="0.2">
@@ -4713,13 +4701,13 @@
         <v>5</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
@@ -4736,25 +4724,25 @@
         <v>38</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
       <c r="F55" s="2" t="s">
-        <v>563</v>
+        <v>542</v>
       </c>
       <c r="G55" s="2"/>
       <c r="H55" s="2" t="s">
         <v>40</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="208" x14ac:dyDescent="0.2">
@@ -4765,25 +4753,25 @@
         <v>38</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
       <c r="F56" s="2" t="s">
-        <v>564</v>
+        <v>543</v>
       </c>
       <c r="G56" s="2"/>
       <c r="H56" s="2" t="s">
         <v>40</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
     <row r="57" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -4794,23 +4782,23 @@
         <v>38</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
       <c r="H57" s="2" t="s">
-        <v>202</v>
+        <v>559</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
     </row>
     <row r="58" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -4821,23 +4809,23 @@
         <v>38</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
       <c r="H58" s="2" t="s">
-        <v>206</v>
+        <v>559</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="59" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -4848,23 +4836,23 @@
         <v>38</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
       <c r="H59" s="2" t="s">
-        <v>210</v>
+        <v>560</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
     </row>
     <row r="60" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -4875,23 +4863,23 @@
         <v>38</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
       <c r="H60" s="2" t="s">
-        <v>214</v>
+        <v>560</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="J60" s="2" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
     </row>
     <row r="61" spans="1:11" ht="80" x14ac:dyDescent="0.2">
@@ -4902,25 +4890,25 @@
         <v>38</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
       <c r="F61" s="2" t="s">
-        <v>565</v>
+        <v>544</v>
       </c>
       <c r="G61" s="2"/>
       <c r="H61" s="2" t="s">
         <v>40</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="J61" s="2" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -4943,7 +4931,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -4963,8 +4951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A41" zoomScale="176" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4979,22 +4967,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>499</v>
+        <v>478</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -5002,10 +4990,10 @@
         <v>39</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -5016,10 +5004,10 @@
         <v>42</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -5030,10 +5018,10 @@
         <v>44</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -5044,10 +5032,10 @@
         <v>46</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -5058,14 +5046,14 @@
         <v>48</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>230</v>
+        <v>550</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -5074,17 +5062,17 @@
         <v>50</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>232</v>
+        <v>551</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>500</v>
+        <v>479</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -5092,17 +5080,17 @@
         <v>52</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>233</v>
+        <v>552</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>500</v>
+        <v>479</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -5110,17 +5098,17 @@
         <v>54</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>234</v>
+        <v>557</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>500</v>
+        <v>479</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="144" x14ac:dyDescent="0.2">
@@ -5128,10 +5116,10 @@
         <v>56</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -5139,710 +5127,710 @@
     </row>
     <row r="11" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
-        <v>500</v>
+        <v>479</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
-        <v>501</v>
+        <v>480</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
-        <v>502</v>
+        <v>481</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
-        <v>503</v>
+        <v>482</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>225</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>240</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
-        <v>504</v>
+        <v>483</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
-        <v>504</v>
+        <v>483</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
-        <v>505</v>
+        <v>484</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2" t="s">
-        <v>506</v>
+        <v>485</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2" t="s">
-        <v>503</v>
+        <v>482</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2" t="s">
-        <v>503</v>
+        <v>482</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2" t="s">
-        <v>507</v>
+        <v>486</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2" t="s">
-        <v>508</v>
+        <v>487</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2" t="s">
-        <v>501</v>
+        <v>480</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2" t="s">
-        <v>509</v>
+        <v>488</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2" t="s">
-        <v>510</v>
+        <v>489</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2" t="s">
-        <v>503</v>
+        <v>482</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2" t="s">
-        <v>503</v>
+        <v>482</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2" t="s">
-        <v>504</v>
+        <v>483</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2" t="s">
-        <v>501</v>
+        <v>480</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2" t="s">
-        <v>503</v>
+        <v>482</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2" t="s">
-        <v>504</v>
+        <v>483</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2" t="s">
-        <v>510</v>
+        <v>489</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2" t="s">
-        <v>500</v>
+        <v>479</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2" t="s">
-        <v>504</v>
+        <v>483</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2" t="s">
-        <v>506</v>
+        <v>485</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2" t="s">
-        <v>259</v>
+        <v>558</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>500</v>
+        <v>479</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>260</v>
+        <v>244</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2" t="s">
-        <v>504</v>
+        <v>483</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>261</v>
+        <v>245</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2" t="s">
-        <v>504</v>
+        <v>483</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>262</v>
+        <v>246</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2" t="s">
-        <v>510</v>
+        <v>489</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>263</v>
+        <v>247</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2" t="s">
-        <v>511</v>
+        <v>490</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2" t="s">
-        <v>503</v>
+        <v>482</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>264</v>
+        <v>248</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
       <c r="F42" s="2" t="s">
-        <v>510</v>
+        <v>489</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>265</v>
+        <v>249</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
       <c r="F43" s="2" t="s">
-        <v>510</v>
+        <v>489</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>266</v>
+        <v>250</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
       <c r="F44" s="2" t="s">
-        <v>510</v>
+        <v>489</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>267</v>
+        <v>251</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
       <c r="F45" s="2" t="s">
-        <v>504</v>
+        <v>483</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2" t="s">
-        <v>506</v>
+        <v>485</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>268</v>
+        <v>252</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
       <c r="F47" s="2" t="s">
-        <v>504</v>
+        <v>483</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>269</v>
+        <v>253</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
       <c r="F48" s="2" t="s">
-        <v>501</v>
+        <v>480</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2" t="s">
-        <v>271</v>
+        <v>561</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>501</v>
+        <v>480</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
       <c r="F50" s="2" t="s">
-        <v>506</v>
+        <v>485</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
       <c r="F51" s="2" t="s">
-        <v>506</v>
+        <v>485</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
       <c r="F52" s="2" t="s">
-        <v>506</v>
+        <v>485</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
       <c r="F53" s="2" t="s">
-        <v>506</v>
+        <v>485</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>272</v>
+        <v>255</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
       <c r="F54" s="2" t="s">
-        <v>504</v>
+        <v>483</v>
       </c>
     </row>
   </sheetData>
@@ -5888,8 +5876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView zoomScale="179" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5911,7 +5899,7 @@
         <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>273</v>
+        <v>256</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5919,7 +5907,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>274</v>
+        <v>257</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
@@ -5928,140 +5916,140 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>57</v>
+        <v>545</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>518</v>
+        <v>497</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>60</v>
+        <v>545</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>519</v>
+        <v>498</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>275</v>
+        <v>258</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>276</v>
+        <v>259</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>155</v>
+        <v>546</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>512</v>
+        <v>491</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>159</v>
+        <v>546</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>513</v>
+        <v>492</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>202</v>
+        <v>559</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>514</v>
+        <v>493</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>206</v>
+        <v>559</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>515</v>
+        <v>494</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>210</v>
+        <v>560</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>516</v>
+        <v>495</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>214</v>
+        <v>560</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>517</v>
+        <v>496</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>277</v>
+        <v>553</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>520</v>
+        <v>499</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>278</v>
+        <v>554</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>521</v>
+        <v>500</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>279</v>
+        <v>555</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>522</v>
+        <v>501</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>280</v>
+        <v>556</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>523</v>
+        <v>502</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -6097,7 +6085,7 @@
         <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>281</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -6109,7 +6097,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -6131,10 +6119,10 @@
         <v>10</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>282</v>
+        <v>261</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>283</v>
+        <v>262</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>12</v>
@@ -6145,1037 +6133,1037 @@
     </row>
     <row r="2" spans="1:6" ht="192" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>284</v>
+        <v>263</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>285</v>
+        <v>264</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>286</v>
+        <v>265</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>287</v>
+        <v>266</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>288</v>
+        <v>267</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>289</v>
+        <v>268</v>
       </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="240" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>290</v>
+        <v>269</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>291</v>
+        <v>270</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>292</v>
+        <v>271</v>
       </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" ht="144" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>293</v>
+        <v>272</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>294</v>
+        <v>273</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>295</v>
+        <v>274</v>
       </c>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" ht="272" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>296</v>
+        <v>275</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>297</v>
+        <v>276</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>298</v>
+        <v>277</v>
       </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" ht="160" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>299</v>
+        <v>278</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>300</v>
+        <v>279</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>301</v>
+        <v>280</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" ht="176" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>302</v>
+        <v>281</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>303</v>
+        <v>282</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>304</v>
+        <v>283</v>
       </c>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" ht="176" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>305</v>
+        <v>284</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>306</v>
+        <v>285</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>304</v>
+        <v>283</v>
       </c>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" ht="144" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>307</v>
+        <v>286</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>308</v>
+        <v>287</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>309</v>
+        <v>288</v>
       </c>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" ht="144" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>310</v>
+        <v>289</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>311</v>
+        <v>290</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>309</v>
+        <v>288</v>
       </c>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" ht="288" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>312</v>
+        <v>291</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>313</v>
+        <v>292</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
-        <v>314</v>
+        <v>293</v>
       </c>
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" ht="176" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>315</v>
+        <v>294</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>316</v>
+        <v>295</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
-        <v>317</v>
+        <v>296</v>
       </c>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" ht="128" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>318</v>
+        <v>297</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>319</v>
+        <v>298</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
-        <v>320</v>
+        <v>299</v>
       </c>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>321</v>
+        <v>300</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>322</v>
+        <v>301</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
-        <v>323</v>
+        <v>302</v>
       </c>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>324</v>
+        <v>303</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>325</v>
+        <v>304</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>326</v>
+        <v>305</v>
       </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>327</v>
+        <v>306</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>328</v>
+        <v>307</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>329</v>
+        <v>308</v>
       </c>
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>330</v>
+        <v>309</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>331</v>
+        <v>310</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2" t="s">
-        <v>332</v>
+        <v>311</v>
       </c>
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>333</v>
+        <v>312</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>334</v>
+        <v>313</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2" t="s">
-        <v>335</v>
+        <v>314</v>
       </c>
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" ht="128" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>336</v>
+        <v>315</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>337</v>
+        <v>316</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2" t="s">
-        <v>338</v>
+        <v>317</v>
       </c>
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" ht="128" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>339</v>
+        <v>318</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>340</v>
+        <v>319</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2" t="s">
-        <v>341</v>
+        <v>320</v>
       </c>
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" ht="365" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>342</v>
+        <v>321</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>343</v>
+        <v>322</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2" t="s">
-        <v>344</v>
+        <v>323</v>
       </c>
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" ht="144" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>345</v>
+        <v>324</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>346</v>
+        <v>325</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2" t="s">
-        <v>347</v>
+        <v>326</v>
       </c>
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" ht="395" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>348</v>
+        <v>327</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>349</v>
+        <v>328</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2" t="s">
-        <v>350</v>
+        <v>329</v>
       </c>
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6" ht="224" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>351</v>
+        <v>330</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>352</v>
+        <v>331</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2" t="s">
-        <v>353</v>
+        <v>332</v>
       </c>
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" ht="272" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>354</v>
+        <v>333</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>355</v>
+        <v>334</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6" ht="160" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>358</v>
+        <v>337</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2" t="s">
-        <v>359</v>
+        <v>338</v>
       </c>
       <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6" ht="144" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>360</v>
+        <v>339</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>361</v>
+        <v>340</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2" t="s">
-        <v>362</v>
+        <v>341</v>
       </c>
       <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:6" ht="128" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>363</v>
+        <v>342</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>364</v>
+        <v>343</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2" t="s">
-        <v>365</v>
+        <v>344</v>
       </c>
       <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:6" ht="192" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>366</v>
+        <v>345</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>367</v>
+        <v>346</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2" t="s">
-        <v>368</v>
+        <v>347</v>
       </c>
       <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6" ht="128" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>369</v>
+        <v>348</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>370</v>
+        <v>349</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2" t="s">
-        <v>371</v>
+        <v>350</v>
       </c>
       <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:6" ht="192" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>372</v>
+        <v>351</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>373</v>
+        <v>352</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2" t="s">
-        <v>374</v>
+        <v>353</v>
       </c>
       <c r="F32" s="1"/>
     </row>
     <row r="33" spans="1:6" ht="208" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>375</v>
+        <v>354</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>376</v>
+        <v>355</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2" t="s">
-        <v>377</v>
+        <v>356</v>
       </c>
       <c r="F33" s="1"/>
     </row>
     <row r="34" spans="1:6" ht="224" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>378</v>
+        <v>357</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>379</v>
+        <v>358</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2" t="s">
-        <v>380</v>
+        <v>359</v>
       </c>
       <c r="F34" s="1"/>
     </row>
     <row r="35" spans="1:6" ht="192" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>381</v>
+        <v>360</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>382</v>
+        <v>361</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2" t="s">
-        <v>383</v>
+        <v>362</v>
       </c>
       <c r="F35" s="1"/>
     </row>
     <row r="36" spans="1:6" ht="144" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>384</v>
+        <v>363</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>385</v>
+        <v>364</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2" t="s">
-        <v>386</v>
+        <v>365</v>
       </c>
       <c r="F36" s="1"/>
     </row>
     <row r="37" spans="1:6" ht="192" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>387</v>
+        <v>366</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>388</v>
+        <v>367</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2" t="s">
-        <v>383</v>
+        <v>362</v>
       </c>
       <c r="F37" s="1"/>
     </row>
     <row r="38" spans="1:6" ht="144" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>389</v>
+        <v>368</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>390</v>
+        <v>369</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2" t="s">
-        <v>386</v>
+        <v>365</v>
       </c>
       <c r="F38" s="1"/>
     </row>
     <row r="39" spans="1:6" ht="192" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>391</v>
+        <v>370</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>392</v>
+        <v>371</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2" t="s">
-        <v>393</v>
+        <v>372</v>
       </c>
       <c r="F39" s="1"/>
     </row>
     <row r="40" spans="1:6" ht="208" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>394</v>
+        <v>373</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>395</v>
+        <v>374</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2" t="s">
-        <v>396</v>
+        <v>375</v>
       </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="1:6" ht="192" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>397</v>
+        <v>376</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>398</v>
+        <v>377</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2" t="s">
-        <v>393</v>
+        <v>372</v>
       </c>
       <c r="F41" s="1"/>
     </row>
     <row r="42" spans="1:6" ht="208" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>399</v>
+        <v>378</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>400</v>
+        <v>379</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2" t="s">
-        <v>396</v>
+        <v>375</v>
       </c>
       <c r="F42" s="1"/>
     </row>
     <row r="43" spans="1:6" ht="256" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>401</v>
+        <v>380</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>402</v>
+        <v>381</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2" t="s">
-        <v>403</v>
+        <v>382</v>
       </c>
       <c r="F43" s="1"/>
     </row>
     <row r="44" spans="1:6" ht="144" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>404</v>
+        <v>383</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>405</v>
+        <v>384</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2" t="s">
-        <v>406</v>
+        <v>385</v>
       </c>
       <c r="F44" s="1"/>
     </row>
     <row r="45" spans="1:6" ht="192" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>407</v>
+        <v>386</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>408</v>
+        <v>387</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2" t="s">
-        <v>409</v>
+        <v>388</v>
       </c>
       <c r="F45" s="1"/>
     </row>
     <row r="46" spans="1:6" ht="192" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>410</v>
+        <v>389</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>411</v>
+        <v>390</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2" t="s">
-        <v>412</v>
+        <v>391</v>
       </c>
       <c r="F46" s="1"/>
     </row>
     <row r="47" spans="1:6" ht="240" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>413</v>
+        <v>392</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>414</v>
+        <v>393</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2" t="s">
-        <v>415</v>
+        <v>394</v>
       </c>
       <c r="F47" s="1"/>
     </row>
     <row r="48" spans="1:6" ht="160" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>416</v>
+        <v>395</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>417</v>
+        <v>396</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2" t="s">
-        <v>418</v>
+        <v>397</v>
       </c>
       <c r="F48" s="1"/>
     </row>
     <row r="49" spans="1:6" ht="192" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>419</v>
+        <v>398</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>420</v>
+        <v>399</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2" t="s">
-        <v>421</v>
+        <v>400</v>
       </c>
       <c r="F49" s="1"/>
     </row>
     <row r="50" spans="1:6" ht="176" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>422</v>
+        <v>401</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>423</v>
+        <v>402</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
       <c r="E50" s="2" t="s">
-        <v>424</v>
+        <v>403</v>
       </c>
       <c r="F50" s="1"/>
     </row>
     <row r="51" spans="1:6" ht="224" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>425</v>
+        <v>404</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>426</v>
+        <v>405</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
       <c r="E51" s="2" t="s">
-        <v>427</v>
+        <v>406</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="1:6" ht="144" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>428</v>
+        <v>407</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>429</v>
+        <v>408</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
       <c r="E52" s="2" t="s">
-        <v>430</v>
+        <v>409</v>
       </c>
       <c r="F52" s="1"/>
     </row>
     <row r="53" spans="1:6" ht="240" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>431</v>
+        <v>410</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>432</v>
+        <v>411</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
       <c r="E53" s="2" t="s">
-        <v>433</v>
+        <v>412</v>
       </c>
       <c r="F53" s="1"/>
     </row>
     <row r="54" spans="1:6" ht="272" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>434</v>
+        <v>413</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>435</v>
+        <v>414</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
       <c r="E54" s="2" t="s">
-        <v>436</v>
+        <v>415</v>
       </c>
       <c r="F54" s="1"/>
     </row>
     <row r="55" spans="1:6" ht="320" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>437</v>
+        <v>416</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>438</v>
+        <v>417</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
       <c r="E55" s="2" t="s">
-        <v>439</v>
+        <v>418</v>
       </c>
       <c r="F55" s="1"/>
     </row>
     <row r="56" spans="1:6" ht="192" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>440</v>
+        <v>419</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>441</v>
+        <v>420</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
       <c r="E56" s="2" t="s">
-        <v>442</v>
+        <v>421</v>
       </c>
       <c r="F56" s="1"/>
     </row>
     <row r="57" spans="1:6" ht="240" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>443</v>
+        <v>422</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>444</v>
+        <v>423</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
       <c r="E57" s="2" t="s">
-        <v>445</v>
+        <v>424</v>
       </c>
       <c r="F57" s="1"/>
     </row>
     <row r="58" spans="1:6" ht="144" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>446</v>
+        <v>425</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>447</v>
+        <v>426</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
       <c r="E58" s="2" t="s">
-        <v>448</v>
+        <v>427</v>
       </c>
       <c r="F58" s="1"/>
     </row>
     <row r="59" spans="1:6" ht="128" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>449</v>
+        <v>428</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>450</v>
+        <v>429</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
       <c r="E59" s="2" t="s">
-        <v>451</v>
+        <v>430</v>
       </c>
       <c r="F59" s="1"/>
     </row>
     <row r="60" spans="1:6" ht="288" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>452</v>
+        <v>431</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>453</v>
+        <v>432</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
       <c r="E60" s="2" t="s">
-        <v>454</v>
+        <v>433</v>
       </c>
       <c r="F60" s="1"/>
     </row>
     <row r="61" spans="1:6" ht="208" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>455</v>
+        <v>434</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>456</v>
+        <v>435</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
       <c r="E61" s="2" t="s">
-        <v>457</v>
+        <v>436</v>
       </c>
       <c r="F61" s="1"/>
     </row>
     <row r="62" spans="1:6" ht="304" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>458</v>
+        <v>437</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>459</v>
+        <v>438</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
       <c r="E62" s="2" t="s">
-        <v>460</v>
+        <v>439</v>
       </c>
       <c r="F62" s="1"/>
     </row>
     <row r="63" spans="1:6" ht="240" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>461</v>
+        <v>440</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>462</v>
+        <v>441</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
       <c r="E63" s="2" t="s">
-        <v>463</v>
+        <v>442</v>
       </c>
       <c r="F63" s="1"/>
     </row>
     <row r="64" spans="1:6" ht="160" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>464</v>
+        <v>443</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>465</v>
+        <v>444</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
       <c r="E64" s="2" t="s">
-        <v>466</v>
+        <v>445</v>
       </c>
       <c r="F64" s="1"/>
     </row>
     <row r="65" spans="1:6" ht="192" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>467</v>
+        <v>446</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>468</v>
+        <v>447</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
       <c r="E65" s="2" t="s">
-        <v>469</v>
+        <v>448</v>
       </c>
       <c r="F65" s="1"/>
     </row>
     <row r="66" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>470</v>
+        <v>449</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>471</v>
+        <v>450</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
       <c r="E66" s="2" t="s">
-        <v>472</v>
+        <v>451</v>
       </c>
       <c r="F66" s="1"/>
     </row>
     <row r="67" spans="1:6" ht="176" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>473</v>
+        <v>452</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>474</v>
+        <v>453</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
       <c r="E67" s="2" t="s">
-        <v>475</v>
+        <v>454</v>
       </c>
       <c r="F67" s="1"/>
     </row>
     <row r="68" spans="1:6" ht="272" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>476</v>
+        <v>455</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>477</v>
+        <v>456</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
       <c r="E68" s="2" t="s">
-        <v>478</v>
+        <v>457</v>
       </c>
       <c r="F68" s="1"/>
     </row>
     <row r="69" spans="1:6" ht="160" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>479</v>
+        <v>458</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>480</v>
+        <v>459</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
       <c r="E69" s="2" t="s">
-        <v>481</v>
+        <v>460</v>
       </c>
       <c r="F69" s="1"/>
     </row>
     <row r="70" spans="1:6" ht="256" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>482</v>
+        <v>461</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>483</v>
+        <v>462</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
       <c r="E70" s="2" t="s">
-        <v>484</v>
+        <v>463</v>
       </c>
       <c r="F70" s="1"/>
     </row>
     <row r="71" spans="1:6" ht="128" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>485</v>
+        <v>464</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>486</v>
+        <v>465</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
       <c r="E71" s="2" t="s">
-        <v>487</v>
+        <v>466</v>
       </c>
       <c r="F71" s="1"/>
     </row>
     <row r="72" spans="1:6" ht="256" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>488</v>
+        <v>467</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>483</v>
+        <v>462</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
       <c r="E72" s="2" t="s">
-        <v>484</v>
+        <v>463</v>
       </c>
       <c r="F72" s="1"/>
     </row>
     <row r="73" spans="1:6" ht="128" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>489</v>
+        <v>468</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>486</v>
+        <v>465</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
       <c r="E73" s="2" t="s">
-        <v>487</v>
+        <v>466</v>
       </c>
       <c r="F73" s="1"/>
     </row>
     <row r="74" spans="1:6" ht="224" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>490</v>
+        <v>469</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>491</v>
+        <v>470</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
       <c r="E74" s="2" t="s">
-        <v>492</v>
+        <v>471</v>
       </c>
       <c r="F74" s="1"/>
     </row>
     <row r="75" spans="1:6" ht="192" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>493</v>
+        <v>472</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>494</v>
+        <v>473</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
       <c r="E75" s="2" t="s">
-        <v>495</v>
+        <v>474</v>
       </c>
       <c r="F75" s="1"/>
     </row>

</xml_diff>

<commit_message>
[Excel] Replace "#" by "##" in "annotation"
</commit_message>
<xml_diff>
--- a/tools/excel/anssi/anssi-mon-aide-cyber.xlsx
+++ b/tools/excel/anssi/anssi-mon-aide-cyber.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\tarkadia\projects\intuitem\ciso-assistant-community\tools\excel\anssi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E887F5D2-2665-4599-93A5-12E9374BAAE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF74C4E-A543-41A2-A5DE-4994E4DAFA54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4005" yWindow="-13980" windowWidth="20160" windowHeight="11310" tabRatio="882" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1485" yWindow="-15870" windowWidth="25440" windowHeight="15990" tabRatio="882" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_meta" sheetId="1" r:id="rId1"/>
@@ -2483,24 +2483,78 @@
 /</t>
   </si>
   <si>
-    <t># Entités publiques
+    <t>Question 33.1 dépendante de la Question 33</t>
+  </si>
+  <si>
+    <t>Question 33.2 dépendante de la Question 33</t>
+  </si>
+  <si>
+    <t>Question 44.1 dépendante de la Question 44</t>
+  </si>
+  <si>
+    <t>Question 44.2 dépendante de la Question 44</t>
+  </si>
+  <si>
+    <t>Question 44.3 dépendante de la Question 44</t>
+  </si>
+  <si>
+    <t>Question 44.4 dépendante de la Question 44</t>
+  </si>
+  <si>
+    <t>Question 8.1 dépendante de la Question 8</t>
+  </si>
+  <si>
+    <t>Question 8.2 dépendante de la Question 8</t>
+  </si>
+  <si>
+    <t>Questions dépendantes de la Question 7</t>
+  </si>
+  <si>
+    <t>Questions dépendantes de la Question 6</t>
+  </si>
+  <si>
+    <t>Questions dépendantes de la Question 5</t>
+  </si>
+  <si>
+    <t>Questions dépendantes de la Question</t>
+  </si>
+  <si>
+    <t>MonAideCyber aide les entités publiques et privées sensibilisées à la sécurité informatique à passer à l’action. Le dispositif MonAideCyber est développé par l'Agence Nationale de la Sécurité des Systèmes d'Information, en lien avec BetaGouv et la Direction interministérielle du numérique.
+ Sources :
+	• https://github.com/betagouv/mon-aide-cyber 
+	• https://monaide.cyber.gouv.fr/diagnostic-libre-acces</t>
+  </si>
+  <si>
+    <t>node_id</t>
+  </si>
+  <si>
+    <t>## Entités publiques
 Les entités publiques sont invitées à s'orienter vers le service ANSSI https://club.ssi.gouv.fr/ pour bénéficier d'outils gratuits d’audits automatisés.</t>
   </si>
   <si>
-    <t># Moins de 9 postes
+    <t>## Des dispositifs adaptés
+Selon le secteur d’activité et la région sélectionnés, l’entité se verra proposer des dispositifs adhoc.</t>
+  </si>
+  <si>
+    <t>## Moins de 9 postes
 Si l’entité dispose de moins de 9 postes, le questionnaire MonAideCyber se verra légèrement simplifié. Ainsi, les questions 12, 33 et 34 seront facultatives.</t>
   </si>
   <si>
-    <t># Attaque ciblée
+    <t>## Attaque ciblée
 Si oui, des questions additionnelles liées à la maîtrise des accès utilisateurs et à la sécurisation des données jugées sensibles seront abordées.
 Exemples d’informations et de données pouvant être faire l’objet d’une attaque ciblée : secrets industriels, données de R&amp;D, brevets d'invention, données innovantes jugées vitales pour l’activité de l’entité, données clientes confidentielles.</t>
   </si>
   <si>
-    <t># Statistiques anonymes
+    <t>## Systèmes industriels
+Si oui, des questions dédiées à la sécurité des systèmes industriels seront abordées.
+Exemples de systèmes industriels : objet ou machine industrielle connectée, automates programmables, systèmes numériques de contrôle-commande, systèmes instrumentés de sécurité, capteurs et actionneurs,  bus de terrain, logiciels de supervision et de contrôle SCADA, logiciels de gestion de production assistée par ordinateur (GPAO, GMAO, MES), logiciels d’ingénierie et de maintenance, systèmes embarqués, Gestion Technique Centralisée (GTC), Gestion Technique du Bâtiment (GTB), équipements biomédicaux, etc.</t>
+  </si>
+  <si>
+    <t>## Statistiques anonymes
 Attention, bien préciser à l’entité que cette question est utile à des fins de statistiques anonymisées. Aucune action ne sera menée si jamais elle n’a pas déposé plainte suite à une cyberattaque.</t>
   </si>
   <si>
-    <t># À protéger en priorité 
+    <t>## À protéger en priorité 
 Peuvent être jugées prioritaires :
 	• les activités critiques, indispensables à l’activité,
 	• les informations sensibles, confidentielles et/ou ne devant pas être volées et exfiltrées
@@ -2512,54 +2566,54 @@
 	• Courriels, agenda et données bureautiques associées</t>
   </si>
   <si>
-    <t># Interconnexions extérieures
+    <t>## Interconnexions extérieures
 IP publiques, accès distants ouverts aux prestataires et partenaires, etc.
-# Entités publiques
+## Entités publiques
 Les entités publiques sont éligibles au service gratuit SILENE de l’ANSSI qui permet d’identifier la surface d’attaque des services exposés sur Internet.&lt;br /&gt; Pour y accéder, l’entité est invitée à s'orienter vers le service ANSSI https://club.ssi.gouv.fr/.</t>
   </si>
   <si>
-    <t># **SYSTÈME INDUSTRIEL**
-# Composants
+    <t>## **SYSTÈME INDUSTRIEL**
+## Composants
 Équipements réseaux (routeur, switch/commutateur, borne-wifi, pare-feu et autres équipements de sécurité), les serveurs (en précisant leurs fonctionnalités), les infrastructures de sauvegarde, les postes de travail utilisateurs et les supports mobiles interconnectés au réseau.</t>
   </si>
   <si>
-    <t># CNIL
+    <t>## CNIL
 Attention à ne pas tomber dans un contrôle de conformité au RGPD, ces informations ne seront pas partagées à la CNIL. Si nécessaire, rappeler de manière pédagogique que le Règlement Général sur Protection des Données est une obligation réglementaire qui s’applique à toute entité, publique et privée, qui gère et stocke des données personnelles.
-# Données personnelles 
+## Données personnelles 
 Exemples de données personnelles :
 	• Données liées au personnel,
 	• Données des clients ou des usagers,
 	• Données des fournisseurs ou partenaires.</t>
   </si>
   <si>
-    <t># Utilisation des données personnelles
+    <t>## Utilisation des données personnelles
 Il existe une page d’information dédiée à l'utilisation des données personnelles et la gestion des droits d’informations et les moyens de les exercer sur le site de la CNIL : https://www.cnil.fr/fr/respecter-les-droits-des-personnes</t>
   </si>
   <si>
-    <t># Contrats des prestataires
+    <t>## Contrats des prestataires
 Cette question suppose que l’entité ait des contrats avec ses prestataires et sait lesquels ont accès à son système d’information, sinon, nous vous invitons à cocher “Non, aucune exigence ne figure dans nos contrats de prestation.”
 Exemples d’exigences pouvant être intégrées dans un contrat : changement des mots de passe par défaut ; sécurisation des accès distants ; délai de déploiement des mises à jour critiques ; signalement en cas de cyberattaque ; contractualisation d'un plan d'assurance sécurité (PAS).
-# Systèmes industriels
+## Systèmes industriels
 Si l’entité est concernée, cette question s’applique également pour les prestataires disposant d’accès informatiques sur les systèmes industriels</t>
   </si>
   <si>
-    <t># Entités publiques
+    <t>## Entités publiques
 Les entités publiques sont éligibles au service gratuit ADS de l’ANSSI qui permet d’analyser le niveau de sécurité de l’annuaire centralisé. Pour y accéder, l’entité est invitée à s’orienter vers le service ANSSI https://club.ssi.gouv.fr/
-# Active Directory, Samba-AD
+## Active Directory, Samba-AD
 À partir d’un parc informatique d’une dizaine de postes, il est fortement recommandé de s’appuyer sur une solution de type Active Directory ou Samba-AD, et de ne plus s’appuyer sur un réseau en “Workgroup” afin d’homogénéiser le niveau de sécurité des postes de travail.</t>
   </si>
   <si>
-    <t># **ATTAQUE CIBLÉE**
-# Accès et comptes prioritaires
+    <t>## **ATTAQUE CIBLÉE**
+## Accès et comptes prioritaires
 Les accès et comptes utilisateurs à maitriser en priorité sont ceux permettant d’ouvrir une session sur le poste de travail et ceux permettant d’accéder aux données jugées les plus sensibles. Selon les cas, ces accès et comptes sont gérés via un Active Directory et/ou un service Cloud et/ou applicatif(s) métier(s).</t>
   </si>
   <si>
-    <t># Administration locale des postes
+    <t>## Administration locale des postes
 Cette question traite du privilège d'administration local des comptes utilisateurs sur leur poste de travail, il permet par exemple aux utilisateurs d'être autonome dans l'installation d'applications et la configuration de leur machine.
 Si le personnel est autorisé à utiliser son matériel personnel (BYOD) pour travailler et accéder aux systèmes d’information de l’entité, nous vous invitons à cocher “Oui”.</t>
   </si>
   <si>
-    <t># Mots de passe 
+    <t>## Mots de passe 
 Exigences minimales acceptables :
 	• Longueur de mots de passe à minima de 12 caractères si compte non administrateur local
 	• Longueur de mots de passe à minima de 16 caractères si compte administrateur local
@@ -2567,52 +2621,78 @@
 	• 1 renouvellement annuel des mots de passe, et lors d'une suspicion d'une cyberattaque</t>
   </si>
   <si>
-    <t># Comptes d’administration
+    <t>## Comptes d’administration
 NB : cette question traite des comptes d'administration systèmes sur les serveurs, infrastructures etc. L'administration locale des postes de travail est traitée dans la question sur les utilisateurs administrateurs de leurs postes</t>
   </si>
   <si>
-    <t># Authentification multifacteur 
+    <t>## Comptes d’administration
+NB : cette question traite des comptes d'administration systèmes sur les serveurs, infrastructures etc. L'administration locale des postes de travail est traitée dans la question sur les utilisateurs administrateurs de leurs postes. 
+Exemple de restrictions :
+	• Tous les administrateurs utilisent en parallèle un compte utilisateur sans privilèges pour les usages du quotidien (ex : surf sur internet, messagerie, etc.)
+	• 1 seul compte administrateur du domaine
+	• Le compte administrateur du domaine n’est utilisé qu’exceptionnellement
+	• Le compte d’administration de la solution de sauvegarde différent n’est pas géré via l’annuaire centralisé (ex : Active Directory, Samba-AD)</t>
+  </si>
+  <si>
+    <t>## **ATTAQUE CIBLÉE**
+## Données sensibles
+Nous vous invitons à vous focaliser sur les ressources et données qui étaient jugées prioritaires lors de la question sur les informations et activités à protéger. 
+Exemples de mesures acceptables :
+	• Contraintes renforcées de robustesse et de longueur de mots de passe (16 caractères minimum)
+	• Authentification multifacteur
+	• Protection des données dans un conteneur chiffré “à froid” et lors d’un transfert via Internet (ex : mail)
+	• Utilisation d'une solution de Data Loss Prevention permettant de limiter les fuites de données</t>
+  </si>
+  <si>
+    <t>## Authentification multifacteur 
 Exemples de facteur d’authentification :
 	• l’usage d’une carte à puce et d’un code PIN d’authentification ;
 	• l’usage d’un token physique et d’un code PIN d’authentification ;
 	• l’utilisation d’une application dédiée sur un smartphone idéalement professionnel (ex : Windows Authentificator, Twilio Authy, etc.), ou à défaut un code envoyé par sms idéalement sur un téléphone professionnel</t>
   </si>
   <si>
-    <t># **SYSTÈME INDUSTRIEL**</t>
-  </si>
-  <si>
-    <t># Mises à jour installées
+    <t>## **SYSTÈME INDUSTRIEL**</t>
+  </si>
+  <si>
+    <t>## Authentification renforcée
+Pour répondre aux exigences de la réponse “Oui, des mesures renforçant l’authentification ont été mises en œuvre”, l’entité doit appliquer au moins les premières mesures suivantes :
+	• Modification des mots de passe par défaut
+	• Contraintes renforcées de robustesse et de longueur de mots de passe (16 caractères minimum)
+	• Stockage des mots de passes d’administration des services critiques (ex : annuaire centralisé, sauvegarde, messagerie) en dehors du système d’information (ex : feuille papier dans un meuble fermé à clef, coffre-fort, etc)</t>
+  </si>
+  <si>
+    <t>## Mises à jour installées
 Pour cocher la réponse “Toutes les mises à jour sont déployées […]”, l’entité doit s’assurer que les mises à jour sont bien installées.
-# Mesures complémentaires 
+## Mesures complémentaires 
 Mesures complémentaires pouvant être menées pour sécuriser les postes de travail obsolètes :
 	• les isoler et les cloisonner du reste du réseau bureautique (ex : déconnecter de l’annuaire centralisée), une compromission de ces derniers aura ainsi un faible impact
 	• mettre en œuvre un outil de protection de type EDR en complément de l’antivirus intégrant des règles de sécurité spécifiques aux postes obsolètes.
-# Déploiement des logiciels et contrôle des mises à jour 
+## Déploiement des logiciels et contrôle des mises à jour 
 Afin de s’assurer que les mises à jours sont déployées, il peut être nécessaire de :
 	• faire une vérification manuelle sur chaque poste et pour chaque logiciel (à l’aide d’un script/programme exécuté sur chaque poste)
 	• déployer un agent logiciel réalisant la vérification (outil de gestion des vulnérabilités)
 	• utiliser un outil de gestion centralisé des logiciels : un tel outil permet de connaître l’état de déploiement des logiciels (et notamment leur version) de chaque poste de manière centralisée</t>
   </si>
   <si>
-    <t># Mises à jour installées
+    <t>## Mises à jour installées
 Pour cocher la réponse “Oui et ses alertes sont systématiquement traitées […]”, l’entité doit s’assurer que les mises à jour sont bien installées.
-# Windows Defender
+## Windows Defender
 Windows Defender est l’antivirus intégré gratuitement dans tous les systèmes d’exploitation Windows récents.</t>
   </si>
   <si>
-    <t># Pare-feu local
+    <t>## Pare-feu local
 Le pare-feu local est un logiciel qui permet de filtrer le trafic entrant et sortant dans le système d’exploitation du poste de travail. Un pare-feu local est une fonction intégrée à la plupart des systèmes d’exploitation grand public. Par défaut, ce logiciel est désactivé ou d’un niveau de paramétrage insuffisant. Un niveau suffisant serait de restreindre les communications réseaux directes entre les postes de travail et de bloquer toute connexion entrante. Des pare-feux sont également commercialisés en complément de suites logicielles antivirales.</t>
   </si>
   <si>
-    <t># EDR
+    <t>## EDR
 Un EDR, Endpoint Detection Response, détecte et bloque les menaces sur les terminaux en s’appuyant sur l’analyse comportementale et la corrélation d'événements.</t>
   </si>
   <si>
-    <t># **ATTAQUE CIBLÉE**
-# Windows Bitlocker
+    <t>## **ATTAQUE CIBLÉE**
+## Windows Bitlocker
 Windows Bitlocker est un outil de chiffrement intégré gratuitement dans tous les systèmes d’exploitation Windows récents.
 NB : il est indispensable que le déchiffrement au démarrage du poste soit soumis à un mot de passe robuste (ou un token USB).
-# Matériels nomades 
+## Matériels nomades 
 Il s’agit des équipements et matériels numériques transportés durant les déplacements, exemples :
 	• ordinateur portable
 	• tablette
@@ -2620,36 +2700,36 @@
 	• clefs USB et disques durs</t>
   </si>
   <si>
-    <t># Pare-feu
+    <t>## Pare-feu
 Le pare-feu est l’outil permettant de restreindre les services exposés sur Internet, et réalisant le filtrage des communications et des flux réseaux. Afin de réduire au maximum la surface d’attaque disponible pour les attaquants, il est recommandé de réduire au maximum les services et les flux accessibles depuis Internet.
 Par exemple, il est fortement déconseillé d’autoriser l’accès à distance vers des objets connectés (ex : caméra, imprimante, sondes etc.)
 NB : une box Internet n’est pas à considérer comme un pare-feu physique puisqu’elle ne permet pas de filtrer efficacement les flux sortants.</t>
   </si>
   <si>
-    <t># **SYSTÈME INDUSTRIEL**
-# Cloisonnement des systèmes industriels
+    <t>## **SYSTÈME INDUSTRIEL**
+## Cloisonnement des systèmes industriels
 Le plus sécurisé est un cloisonnement strict (pas d’interconnexion). De manière plus fonctionnelle, les flux réseaux entre les réseaux bureautique et industriel sont filtrés strictement (pour ne laisser passer que les flux des applications strictement nécessaires). Il est par ailleurs fortement conseillé de bloquer l’accès à distance vers des objets connectés (ex : caméra, équipements industriels, sondes etc.) sans restriction particulière (adresse IP source) ou sans passer par un VPN.</t>
   </si>
   <si>
-    <t># Équipements de sécurité 
+    <t>## Équipements de sécurité 
 Exemples d’équipements de sécurité à mettre à jour dès que possible :
 	• Pare-feu réseau, pare-feu applicatif (WAF)
 	• Équipement VPN
 	• Proxy</t>
   </si>
   <si>
-    <t># Serveurs et services d’administration 
+    <t>## Serveurs et services d’administration 
 Exemples des serveurs et des services d’administration à mettre à jour dès que possible :
 	• Serveurs d’infrastructures : Windows Server, Active Directory, serveur gestionnaire de mises à jour WSUS, serveur de messagerie (exchange, zimbra, etc.), solution de virtualisation, outil de supervision et de télémaintenance, solution de sauvegarde
 	• Serveurs métiers : base de données, serveur web (Apache, IIS, etc.), serveur d’application, outil de développement et autres applicatifs etc.
-# Mesures complémentaires 
+## Mesures complémentaires 
 Mesures complémentaires pouvant être menées pour sécuriser les serveurs obsolètes :
 	• les isoler et les cloisonner du reste du réseau bureautique (ex : déconnecter de l’annuaire centralisée)
 	• ne pas les interconnecter à Internet
 	• mettre en œuvre un outil de protection de type EDR intégrant des règles de sécurité spécifiques aux serveurs obsolètes.</t>
   </si>
   <si>
-    <t># Mécanismes de protection 
+    <t>## Mécanismes de protection 
 Les mécanismes de protection de mails illégitimes à paramétrer sur le serveur DNS sont :
 	• Sender Policy Framework (SPF) qui permet de spécifier les adresses IP des serveurs autorisés à émettre les mails d’un domaine ;
 	• DomainKeys Identified Mail (DKIM) qui permet l’authentification du domaine de messagerie d’un mail à l’aide d’une signature cryptographique
@@ -2657,22 +2737,22 @@
 Si l’entité (ou son prestataire) ne maitrise pas ces éléments, il est conseillé de se faire accompagner par un prestataire spécialisé.</t>
   </si>
   <si>
-    <t># **ATTAQUE CIBLÉE**
-# Chiffrement de connexion 
+    <t>## **ATTAQUE CIBLÉE**
+## Chiffrement de connexion 
 Minimum attendu pour cocher la 4ème réponse :
 	• Mot de passe de 20 caractères minimum ;
 	• Chiffrement robuste de la connexion wifi, a minima WPA2 ;
 	• Pas d'accès au réseau interne pour les visiteurs via le Wi-Fi (SSID différent, sous-réseau différent ou Wi-Fi non accessible au visiteur).</t>
   </si>
   <si>
-    <t># **ATTAQUE CIBLÉE**
-# Accès aux serveurs
+    <t>## **ATTAQUE CIBLÉE**
+## Accès aux serveurs
 Pour sélectionner “Oui”, l’accès aux serveurs doit être à minima protégé par une porte fermée à clef dont la clef n’est accessible qu’aux personnes légitimes.
-# Référent sûreté de gendarmerie et de police
+## Référent sûreté de gendarmerie et de police
 Si c’est jugé nécessaire, l’entité peut être mise en relation avec un référent sûreté physique de la gendarmerie et de la police.</t>
   </si>
   <si>
-    <t># Actions de sensibilisation 
+    <t>## Actions de sensibilisation 
 Exemple d'actions de sensibilisation :
 	• Campagne d'affichage, mails d'information, conférence de sensibilisation
 	• Sensibilisation ciblée du CODIR, sensibilisation aux risques d'escroquerie au faux ordre de virement et fraude au président
@@ -2682,109 +2762,29 @@
 Ressources de sensibilisation gratuites : https://www.cybermalveillance.gouv.fr/tous-nos-contenus/actualites/liste-des-ressources-mises-a-disposition Des actions de sensibilisation gratuites peuvent être menées en sollicitant la police ou la gendarmerie nationales : https://www.masecurite.interieur.gouv.fr/fr</t>
   </si>
   <si>
-    <t># Organisation de gestion de crise
-Une organisation de gestion de crise doit à minima identifier les priorités métier à rétablir en cas de crise, des fiches réflexes opérationnelles garantissant la continuité d'activité au travers de modes dégradés défini avec les métiers (ex : assurer la paie, poursuivre la production, gestion des agendas, etc.), des moyens et modalités de communication de crise.</t>
-  </si>
-  <si>
-    <t># Systèmes industriels
-Si oui, des questions dédiées à la sécurité des systèmes industriels seront abordées.
-Exemples de systèmes industriels : objet ou machine industrielle connectée, automates programmables, systèmes numériques de contrôle-commande, systèmes instrumentés de sécurité, capteurs et actionneurs,  bus de terrain, logiciels de supervision et de contrôle SCADA, logiciels de gestion de production assistée par ordinateur (GPAO, GMAO, MES), logiciels d’ingénierie et de maintenance, systèmes embarqués, Gestion Technique Centralisée (GTC), Gestion Technique du Bâtiment (GTB), équipements biomédicaux, etc.</t>
-  </si>
-  <si>
-    <t># Des dispositifs adaptés
-Selon le secteur d’activité et la région sélectionnés, l’entité se verra proposer des dispositifs adhoc.</t>
-  </si>
-  <si>
-    <t>Question 33.1 dépendante de la Question 33</t>
-  </si>
-  <si>
-    <t>Question 33.2 dépendante de la Question 33</t>
-  </si>
-  <si>
-    <t>Question 44.1 dépendante de la Question 44</t>
-  </si>
-  <si>
-    <t>Question 44.2 dépendante de la Question 44</t>
-  </si>
-  <si>
-    <t>Question 44.3 dépendante de la Question 44</t>
-  </si>
-  <si>
-    <t>Question 44.4 dépendante de la Question 44</t>
-  </si>
-  <si>
-    <t>Question 8.1 dépendante de la Question 8</t>
-  </si>
-  <si>
-    <t>Question 8.2 dépendante de la Question 8</t>
-  </si>
-  <si>
-    <t>Questions dépendantes de la Question 7</t>
-  </si>
-  <si>
-    <t>Questions dépendantes de la Question 6</t>
-  </si>
-  <si>
-    <t>Questions dépendantes de la Question 5</t>
-  </si>
-  <si>
-    <t>Questions dépendantes de la Question</t>
-  </si>
-  <si>
-    <t># Comptes d’administration
-NB : cette question traite des comptes d'administration systèmes sur les serveurs, infrastructures etc. L'administration locale des postes de travail est traitée dans la question sur les utilisateurs administrateurs de leurs postes. 
-Exemple de restrictions :
-	• Tous les administrateurs utilisent en parallèle un compte utilisateur sans privilèges pour les usages du quotidien (ex : surf sur internet, messagerie, etc.)
-	• 1 seul compte administrateur du domaine
-	• Le compte administrateur du domaine n’est utilisé qu’exceptionnellement
-	• Le compte d’administration de la solution de sauvegarde différent n’est pas géré via l’annuaire centralisé (ex : Active Directory, Samba-AD)</t>
-  </si>
-  <si>
-    <t># **ATTAQUE CIBLÉE**
-# Données sensibles
-Nous vous invitons à vous focaliser sur les ressources et données qui étaient jugées prioritaires lors de la question sur les informations et activités à protéger. 
-Exemples de mesures acceptables :
-	• Contraintes renforcées de robustesse et de longueur de mots de passe (16 caractères minimum)
-	• Authentification multifacteur
-	• Protection des données dans un conteneur chiffré “à froid” et lors d’un transfert via Internet (ex : mail)
-	• Utilisation d'une solution de Data Loss Prevention permettant de limiter les fuites de données</t>
-  </si>
-  <si>
-    <t># Authentification renforcée
-Pour répondre aux exigences de la réponse “Oui, des mesures renforçant l’authentification ont été mises en œuvre”, l’entité doit appliquer au moins les premières mesures suivantes :
-	• Modification des mots de passe par défaut
-	• Contraintes renforcées de robustesse et de longueur de mots de passe (16 caractères minimum)
-	• Stockage des mots de passes d’administration des services critiques (ex : annuaire centralisé, sauvegarde, messagerie) en dehors du système d’information (ex : feuille papier dans un meuble fermé à clef, coffre-fort, etc)</t>
-  </si>
-  <si>
-    <t># **ATTAQUE CIBLÉE**
-# Passeport de conseils cyber aux voyageurs
+    <t>## **ATTAQUE CIBLÉE**
+## Passeport de conseils cyber aux voyageurs
 L’ANSSI a publié un guide pour sensibiliser les collaborateurs aux bonnes pratiques de cybersécurité durant les déplacements : https://cyber.gouv.fr/publications/bonnes-pratiques-lusage-des-professionnels-en-deplacement</t>
   </si>
   <si>
-    <t># Entités publiques
+    <t>## Entités publiques
 Les entités publiques sont éligibles au service gratuit SILENE de l’ANSSI qui permet d’identifier la surface d’attaque des services exposés sur Internet. Pour y accéder, l’entité est invitée à s'orienter vers le service ANSSI https://club.ssi.gouv.fr/.
-# Suivi des alertes et des vulnérabilités
+## Suivi des alertes et des vulnérabilités
 Le suivi des alertes et des vulnérabilités consiste à se tenir informé des vulnérabilités techniques de cybersécurité critiques pouvant affecter son système d’information (selon les équipements et les systèmes utilisés). Des services gratuits centralisent et répertorient ces vulnérabilités, par exemple le site du [CERT-FR de l'ANSSI.](https://www.cert.ssi.gouv.fr/)</t>
   </si>
   <si>
-    <t># Jeu de sauvegarde isolé 
+    <t>## Jeu de sauvegarde isolé 
 Le jeu de sauvegarde isolé (ou sanctuarisé) peut être réalisé de plusieurs manières :
 	• sur un périphérique de stockage déconnecté du réseau (bandes, disques durs externes, clefs usb),
 	• dans un cloud externe privé, non interconnecté à l'environnement bureautique, via une authentification spécifique,
 	• sur un serveur ou média déconnecté physiquement et/ou logiquement à l’issue de chaque sauvegarde.
 Ce jeu de sauvegarde ne doit donc pas être accessible via l’Active Directory (ou autre service d'annuaire centralisé).
-# Sauvegarde des ressources hébergées en cloud
+## Sauvegarde des ressources hébergées en cloud
 Il convient aussi de s’assurer que les mécanismes de sauvegarde mis en œuvre par l’entité (ou par son prestataire) / prennent également en compte les ressources bureautiques et/ou métiers qui sont seulement hébergées dans des environnements cloud.</t>
   </si>
   <si>
-    <t>MonAideCyber aide les entités publiques et privées sensibilisées à la sécurité informatique à passer à l’action. Le dispositif MonAideCyber est développé par l'Agence Nationale de la Sécurité des Systèmes d'Information, en lien avec BetaGouv et la Direction interministérielle du numérique.
- Sources :
-	• https://github.com/betagouv/mon-aide-cyber 
-	• https://monaide.cyber.gouv.fr/diagnostic-libre-acces</t>
-  </si>
-  <si>
-    <t>node_id</t>
+    <t>## Organisation de gestion de crise
+Une organisation de gestion de crise doit à minima identifier les priorités métier à rétablir en cas de crise, des fiches réflexes opérationnelles garantissant la continuité d'activité au travers de modes dégradés défini avec les métiers (ex : assurer la paie, poursuivre la production, gestion des agendas, etc.), des moyens et modalités de communication de crise.</t>
   </si>
 </sst>
 </file>
@@ -3196,7 +3196,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>616</v>
+        <v>577</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -3347,7 +3347,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>616</v>
+        <v>577</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -3402,7 +3402,7 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>617</v>
+        <v>578</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>10</v>
@@ -3465,7 +3465,7 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
-        <v>565</v>
+        <v>579</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2" t="s">
@@ -3494,7 +3494,7 @@
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
-        <v>597</v>
+        <v>580</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2" t="s">
@@ -3577,7 +3577,7 @@
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
-        <v>566</v>
+        <v>581</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2" t="s">
@@ -3606,7 +3606,7 @@
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2" t="s">
-        <v>567</v>
+        <v>582</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2" t="s">
@@ -3635,7 +3635,7 @@
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2" t="s">
-        <v>596</v>
+        <v>583</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2" t="s">
@@ -3664,7 +3664,7 @@
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2" t="s">
-        <v>568</v>
+        <v>584</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2" t="s">
@@ -3768,7 +3768,7 @@
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
-        <v>569</v>
+        <v>585</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2" t="s">
@@ -3799,7 +3799,7 @@
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
-        <v>570</v>
+        <v>586</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2" t="s">
@@ -3830,7 +3830,7 @@
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
-        <v>571</v>
+        <v>587</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2" t="s">
@@ -3861,7 +3861,7 @@
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
-        <v>572</v>
+        <v>588</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2" t="s">
@@ -3892,7 +3892,7 @@
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2" t="s">
-        <v>573</v>
+        <v>589</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2" t="s">
@@ -3923,7 +3923,7 @@
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2" t="s">
-        <v>574</v>
+        <v>590</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2" t="s">
@@ -3975,7 +3975,7 @@
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2" t="s">
-        <v>575</v>
+        <v>591</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2" t="s">
@@ -4006,7 +4006,7 @@
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2" t="s">
-        <v>576</v>
+        <v>592</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2" t="s">
@@ -4037,7 +4037,7 @@
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2" t="s">
-        <v>576</v>
+        <v>592</v>
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2" t="s">
@@ -4068,7 +4068,7 @@
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2" t="s">
-        <v>577</v>
+        <v>593</v>
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2" t="s">
@@ -4099,7 +4099,7 @@
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2" t="s">
-        <v>578</v>
+        <v>594</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2" t="s">
@@ -4130,7 +4130,7 @@
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2" t="s">
-        <v>579</v>
+        <v>595</v>
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2" t="s">
@@ -4161,7 +4161,7 @@
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2" t="s">
-        <v>610</v>
+        <v>596</v>
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2" t="s">
@@ -4192,7 +4192,7 @@
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2" t="s">
-        <v>611</v>
+        <v>597</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2" t="s">
@@ -4223,7 +4223,7 @@
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2" t="s">
-        <v>580</v>
+        <v>598</v>
       </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2" t="s">
@@ -4254,7 +4254,7 @@
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2" t="s">
-        <v>581</v>
+        <v>599</v>
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2" t="s">
@@ -4285,7 +4285,7 @@
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="2" t="s">
-        <v>612</v>
+        <v>600</v>
       </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2" t="s">
@@ -4337,7 +4337,7 @@
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2" t="s">
-        <v>582</v>
+        <v>601</v>
       </c>
       <c r="G33" s="2"/>
       <c r="H33" s="2" t="s">
@@ -4368,7 +4368,7 @@
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2" t="s">
-        <v>581</v>
+        <v>599</v>
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2" t="s">
@@ -4399,7 +4399,7 @@
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="2" t="s">
-        <v>583</v>
+        <v>602</v>
       </c>
       <c r="G35" s="2"/>
       <c r="H35" s="2" t="s">
@@ -4430,7 +4430,7 @@
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2" t="s">
-        <v>581</v>
+        <v>599</v>
       </c>
       <c r="G36" s="2"/>
       <c r="H36" s="2" t="s">
@@ -4461,7 +4461,7 @@
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="2" t="s">
-        <v>584</v>
+        <v>603</v>
       </c>
       <c r="G37" s="2"/>
       <c r="H37" s="2" t="s">
@@ -4492,7 +4492,7 @@
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2" t="s">
-        <v>585</v>
+        <v>604</v>
       </c>
       <c r="G38" s="2"/>
       <c r="H38" s="2" t="s">
@@ -4523,7 +4523,7 @@
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="2" t="s">
-        <v>586</v>
+        <v>605</v>
       </c>
       <c r="G39" s="2"/>
       <c r="H39" s="2" t="s">
@@ -4575,7 +4575,7 @@
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="2" t="s">
-        <v>587</v>
+        <v>606</v>
       </c>
       <c r="G41" s="2"/>
       <c r="H41" s="2" t="s">
@@ -4664,7 +4664,7 @@
       </c>
       <c r="E44" s="2"/>
       <c r="F44" s="2" t="s">
-        <v>588</v>
+        <v>607</v>
       </c>
       <c r="G44" s="2"/>
       <c r="H44" s="2" t="s">
@@ -4695,7 +4695,7 @@
       </c>
       <c r="E45" s="2"/>
       <c r="F45" s="2" t="s">
-        <v>589</v>
+        <v>608</v>
       </c>
       <c r="G45" s="2"/>
       <c r="H45" s="2" t="s">
@@ -4726,7 +4726,7 @@
       </c>
       <c r="E46" s="2"/>
       <c r="F46" s="2" t="s">
-        <v>590</v>
+        <v>609</v>
       </c>
       <c r="G46" s="2"/>
       <c r="H46" s="2" t="s">
@@ -4757,7 +4757,7 @@
       </c>
       <c r="E47" s="2"/>
       <c r="F47" s="2" t="s">
-        <v>591</v>
+        <v>610</v>
       </c>
       <c r="G47" s="2"/>
       <c r="H47" s="2" t="s">
@@ -4788,7 +4788,7 @@
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="2" t="s">
-        <v>592</v>
+        <v>611</v>
       </c>
       <c r="G48" s="2"/>
       <c r="H48" s="2" t="s">
@@ -4819,7 +4819,7 @@
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="2" t="s">
-        <v>593</v>
+        <v>612</v>
       </c>
       <c r="G49" s="2"/>
       <c r="H49" s="2" t="s">
@@ -4871,7 +4871,7 @@
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="2" t="s">
-        <v>594</v>
+        <v>613</v>
       </c>
       <c r="G51" s="2"/>
       <c r="H51" s="2" t="s">
@@ -4902,7 +4902,7 @@
       </c>
       <c r="E52" s="2"/>
       <c r="F52" s="2" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="G52" s="2"/>
       <c r="H52" s="2" t="s">
@@ -4983,7 +4983,7 @@
       </c>
       <c r="E55" s="2"/>
       <c r="F55" s="2" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="G55" s="2"/>
       <c r="H55" s="2" t="s">
@@ -5014,7 +5014,7 @@
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="2" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="G56" s="2"/>
       <c r="H56" s="2" t="s">
@@ -5161,7 +5161,7 @@
       </c>
       <c r="E61" s="2"/>
       <c r="F61" s="2" t="s">
-        <v>595</v>
+        <v>617</v>
       </c>
       <c r="G61" s="2"/>
       <c r="H61" s="2" t="s">
@@ -6185,7 +6185,7 @@
         <v>66</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>604</v>
+        <v>571</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -6195,7 +6195,7 @@
         <v>70</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>605</v>
+        <v>572</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -6225,7 +6225,7 @@
         <v>191</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>598</v>
+        <v>565</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -6235,7 +6235,7 @@
         <v>196</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>599</v>
+        <v>566</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -6245,7 +6245,7 @@
         <v>251</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>600</v>
+        <v>567</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -6255,7 +6255,7 @@
         <v>256</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>601</v>
+        <v>568</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -6265,7 +6265,7 @@
         <v>261</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>602</v>
+        <v>569</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -6275,7 +6275,7 @@
         <v>266</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>603</v>
+        <v>570</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -6285,7 +6285,7 @@
         <v>330</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>606</v>
+        <v>573</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -6295,7 +6295,7 @@
         <v>331</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>607</v>
+        <v>574</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -6305,7 +6305,7 @@
         <v>332</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>608</v>
+        <v>575</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -6315,7 +6315,7 @@
         <v>333</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>609</v>
+        <v>576</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>

</xml_diff>

<commit_message>
[Excel] Replace "#" by "##" in "description" (ref_ctrl_content)
</commit_message>
<xml_diff>
--- a/tools/excel/anssi/anssi-mon-aide-cyber.xlsx
+++ b/tools/excel/anssi/anssi-mon-aide-cyber.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\tarkadia\projects\intuitem\ciso-assistant-community\tools\excel\anssi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF74C4E-A543-41A2-A5DE-4994E4DAFA54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2DE5D89-BE09-498E-98BD-0A4A761E5125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1485" yWindow="-15870" windowWidth="25440" windowHeight="15990" tabRatio="882" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1353,9 +1353,831 @@
     <t>Établir la liste des activités et des données à protéger en priorité</t>
   </si>
   <si>
-    <t># Pourquoi ?
+    <t>gouvernance-infos-et-activites-a-proteger_niveau2</t>
+  </si>
+  <si>
+    <t>Établir la liste exhaustive et à jour des activités métiers et des informations à protéger en priorité</t>
+  </si>
+  <si>
+    <t>gouvernance-schema-si-a-jour_niveau1</t>
+  </si>
+  <si>
+    <t>Disposer d’un schéma global du réseau informatique et de la liste des interconnexions vers l’extérieur à jour</t>
+  </si>
+  <si>
+    <t>gouvernance-schema-si-a-jour_niveau2</t>
+  </si>
+  <si>
+    <t>Disposer de la liste des équipements et applicatifs concourant au fonctionnement du système d’information</t>
+  </si>
+  <si>
+    <t>gouvernance-schema-si-industriel-a-jour_niveau1</t>
+  </si>
+  <si>
+    <t>Disposer d’un schéma global du réseau industriel et de la liste des interconnexions vers l’extérieur à jour</t>
+  </si>
+  <si>
+    <t>gouvernance-schema-si-industriel-a-jour_niveau2</t>
+  </si>
+  <si>
+    <t>Disposer de la liste des équipements et applicatifs concourant au fonctionnement des systèmes industriels</t>
+  </si>
+  <si>
+    <t>gouvernance-connaissance-rgpd-1_niveau1</t>
+  </si>
+  <si>
+    <t>Établir la liste des données personnelles traitées au sein de votre entité</t>
+  </si>
+  <si>
+    <t>gouvernance-connaissance-rgpd-1_niveau2</t>
+  </si>
+  <si>
+    <t>Établir votre registre des activités de traitement de données personnelles et le tenir à jour</t>
+  </si>
+  <si>
+    <t>gouvernance-connaissance-rgpd-2_niveau1</t>
+  </si>
+  <si>
+    <t>Fournir des informations aux personnes concernées sur l'utilisation de leurs données personnelles</t>
+  </si>
+  <si>
+    <t>gouvernance-connaissance-rgpd-2_niveau2</t>
+  </si>
+  <si>
+    <t>Mettre en place les modalités permettant aux personnes d'exercer de leurs droits</t>
+  </si>
+  <si>
+    <t>gouvernance-exigence-cyber-securite-presta_niveau1</t>
+  </si>
+  <si>
+    <t>Fixer des exigences de cybersécurité aux prestataires</t>
+  </si>
+  <si>
+    <t>gouvernance-exigence-cyber-securite-presta_niveau2</t>
+  </si>
+  <si>
+    <t>Vérifier l'application et imposer des pénalités aux prestataires en cas de non-respect des exigences de cybersécurité</t>
+  </si>
+  <si>
+    <t>acces-outil-gestion-des-comptes_niveau1</t>
+  </si>
+  <si>
+    <t>Mettre en œuvre un outil de gestion des politiques de sécurité centralisées (ex : Active Directory, Samba-AD) et en évaluer/améliorer son niveau de sécurité annuellement</t>
+  </si>
+  <si>
+    <t>acces-outil-gestion-des-comptes_niveau2</t>
+  </si>
+  <si>
+    <t>Contrôler régulièrement le niveau de sécurité de son outil de gestion de politiques de sécurité centralisé</t>
+  </si>
+  <si>
+    <t>acces-liste-compte-utilisateurs_niveau1</t>
+  </si>
+  <si>
+    <t>Réaliser annuellement une revue des accès utilisateurs en les comparant avec les informations détenues par le service RH</t>
+  </si>
+  <si>
+    <t>acces-liste-compte-utilisateurs_niveau2</t>
+  </si>
+  <si>
+    <t>Définir avec le service RH des processus de « circuit arrivée » et « circuit départ » assurant les créations et les désactivations des comptes utilisateurs</t>
+  </si>
+  <si>
+    <t>acces-droits-acces-utilisateurs-limites_niveau1</t>
+  </si>
+  <si>
+    <t>Restreindre l'accès aux données à protéger en priorité aux seules personnes autorisées à y accéder</t>
+  </si>
+  <si>
+    <t>acces-droits-acces-utilisateurs-limites_niveau2</t>
+  </si>
+  <si>
+    <t>Pour les systèmes et applications à protéger en priorité, définir et gérer les utilisateurs selon 2 niveaux de privilèges distincts : 1 niveau "accès complet" et 1 niveau "accès restreint"</t>
+  </si>
+  <si>
+    <t>acces-administrateurs-informatiques-suivie-et-limitee_niveau1</t>
+  </si>
+  <si>
+    <t>Réaliser tous les 6 mois une revue des accès administrateurs en les comparant avec les informations détenues par le service RH</t>
+  </si>
+  <si>
+    <t>acces-administrateurs-informatiques-suivie-et-limitee_niveau2</t>
+  </si>
+  <si>
+    <t>Définir avec les administrateurs des processus de « circuit arrivée » et « circuit départ » assurant les créations et les désactivations des comptes administrateurs</t>
+  </si>
+  <si>
+    <t>acces-utilisation-comptes-administrateurs-droits-limitee_niveau1</t>
+  </si>
+  <si>
+    <t>Utiliser des comptes d'administration dédiés à cet usage</t>
+  </si>
+  <si>
+    <t>acces-utilisation-comptes-administrateurs-droits-limitee_niveau2</t>
+  </si>
+  <si>
+    <t>Utiliser des comptes d'administration distincts selon les périmètres d’administration</t>
+  </si>
+  <si>
+    <t>acces-utilisateurs-administrateurs-poste_niveau1</t>
+  </si>
+  <si>
+    <t>Limiter drastiquement le nombre d’utilisateurs disposant du privilège d’administration local sur leur machine</t>
+  </si>
+  <si>
+    <t>acces-mesures-securite-robustesse-mdp_niveau1</t>
+  </si>
+  <si>
+    <t>Fixer des critères de longueur et complexité des mots de passe et encourager l’usage d’un coffre-fort de mots de passe</t>
+  </si>
+  <si>
+    <t>acces-mesures-securite-robustesse-mdp_niveau2</t>
+  </si>
+  <si>
+    <t>Mettre à disposition des utilisateurs une coffre fort de mots de passe et les former régulièrement à la création de mots de passe robustes</t>
+  </si>
+  <si>
+    <t>acces-utilisateurs-donnees-sensibles-mesures-securite-additionnelles_niveau1</t>
+  </si>
+  <si>
+    <t>Protéger de manière spéficique les données jugées sensibles</t>
+  </si>
+  <si>
+    <t>acces-utilisateurs-donnees-sensibles-mesures-securite-additionnelles_niveau2</t>
+  </si>
+  <si>
+    <t>Mettre en place des mesures additionnelles de sécurisation des données jugées sensibles</t>
+  </si>
+  <si>
+    <t>acces-teletravail-acces-distants-mesures-particulieres_niveau1</t>
+  </si>
+  <si>
+    <t>Mettre en place pour tous les accès distants des mécanismes de double authentification à minima</t>
+  </si>
+  <si>
+    <t>acces-teletravail-acces-distants-mesures-particulieres_niveau2</t>
+  </si>
+  <si>
+    <t>Gérer tous les accès distants via un VPN, lui même authentifié à double facteur</t>
+  </si>
+  <si>
+    <t>acces-si-industriel-teletravail-acces-distants-mesures-particulieres_niveau1</t>
+  </si>
+  <si>
+    <t>Mettre en place pour tous les accès distants des systèmes industriels des mécanismes de double authentification</t>
+  </si>
+  <si>
+    <t>acces-si-industriel-teletravail-acces-distants-mesures-particulieres_niveau2</t>
+  </si>
+  <si>
+    <t>Gérer tous les accès distants des systèmes industriels via un VPN, lui même authentifié à double facteur</t>
+  </si>
+  <si>
+    <t>acces-administrateurs-si-mesures-specifiques_niveau1</t>
+  </si>
+  <si>
+    <t>Protéger de manière spécifique les accès des admininistrateurs</t>
+  </si>
+  <si>
+    <t>acces-administrateurs-si-mesures-specifiques_niveau2</t>
+  </si>
+  <si>
+    <t>Compléter les mesures de sécurisation des accès d’administration</t>
+  </si>
+  <si>
+    <t>securite-poste-maj-fonctionnelles-et-securite-deployees_niveau1</t>
+  </si>
+  <si>
+    <t>Déployer systématiquement toutes les mises à jour sur les postes de travail dès que celles-ci sont disponibles</t>
+  </si>
+  <si>
+    <t>securite-poste-maj-fonctionnelles-et-securite-deployees_niveau2</t>
+  </si>
+  <si>
+    <t>Mettre en œuvre des mesures de sécurité supplémentaires sur les systèmes ne pouvant pas bénéficier des mises à jour</t>
+  </si>
+  <si>
+    <t>securite-poste-si-industriel-maj-fonctionnelles-et-securite-deployees_niveau1</t>
+  </si>
+  <si>
+    <t>Déployer systématiquement toutes les mises à jour sur les postes de travail dédiés aux systèmes industriels dès que celles-ci sont disponibles</t>
+  </si>
+  <si>
+    <t>securite-poste-si-industriel-maj-fonctionnelles-et-securite-deployees_niveau2</t>
+  </si>
+  <si>
+    <t>Mettre en œuvre des mesures de sécurité supplémentaires sur les systèmes industriels ne pouvant pas bénéficier des mises à jour</t>
+  </si>
+  <si>
+    <t>securite-poste-antivirus-deploye_niveau1</t>
+  </si>
+  <si>
+    <t>Installer de manière systématique un antivirus sur les postes de travail</t>
+  </si>
+  <si>
+    <t>securite-poste-antivirus-deploye_niveau2</t>
+  </si>
+  <si>
+    <t>Traiter systématiquement les alertes générées par l'antivirus</t>
+  </si>
+  <si>
+    <t>securite-poste-si-industriel-antivirus-deploye_niveau1</t>
+  </si>
+  <si>
+    <t>Installer de manière systématique un antivirus sur les postes de travail des systèmes industriels, vérifier régulièrement leur bon fonctionnement et leurs mises à jour</t>
+  </si>
+  <si>
+    <t>securite-poste-si-industriel-antivirus-deploye_niveau2</t>
+  </si>
+  <si>
+    <t>Traiter systématiquement les alertes générées par l'antivirus des postes de travail des systèmes industriels</t>
+  </si>
+  <si>
+    <t>securite-poste-pare-feu-local-active_niveau1</t>
+  </si>
+  <si>
+    <t>Activer systématiquement le pare-feu local sur les postes de travail</t>
+  </si>
+  <si>
+    <t>securite-poste-outils-complementaires-securisation_niveau1</t>
+  </si>
+  <si>
+    <t>Mettre en œuvre une solution de type EDR (Endpoint Detection &amp; Response)</t>
+  </si>
+  <si>
+    <t>securite-poste-outils-complementaires-securisation_niveau2</t>
+  </si>
+  <si>
+    <t>Traiter systématiquement les alertes générées par l'EDR</t>
+  </si>
+  <si>
+    <t>securite-poste-r-et-d-disques-chiffres_niveau1</t>
+  </si>
+  <si>
+    <t>Chiffrer les disques durs des matériels nomades</t>
+  </si>
+  <si>
+    <t>securite-infrastructure-pare-feu-deploye_niveau1</t>
+  </si>
+  <si>
+    <t>Déployer un pare-feu physique pour protéger l’interconnexion du SI à Internet</t>
+  </si>
+  <si>
+    <t>securite-infrastructure-pare-feu-deploye-interconnexions-protegees_niveau1</t>
+  </si>
+  <si>
+    <t>Fermer tous les flux et les ports non strictement nécessaires</t>
+  </si>
+  <si>
+    <t>securite-infrastructure-pare-feu-deploye-interconnexions-protegees_niveau2</t>
+  </si>
+  <si>
+    <t>Mettre en œuvre autant que possible un tunnel VPN pour tous les flux entrants</t>
+  </si>
+  <si>
+    <t>securite-infrastructure-pare-feu-deploye-logs-stockes_niveau1</t>
+  </si>
+  <si>
+    <t>Activer et conserver l'historique de l’ensemble des flux bloqués et des flux entrants et sortants identifiés par le pare-feu</t>
+  </si>
+  <si>
+    <t>securite-infrastructure-si-industriel-pare-feu-deploye_niveau1</t>
+  </si>
+  <si>
+    <t>Fermer tous les flux et les ports non strictement nécessaires aux systèmes industriels</t>
+  </si>
+  <si>
+    <t>securite-infrastructure-si-industriel-pare-feu-deploye_niveau2</t>
+  </si>
+  <si>
+    <t>Dans la mesure du possible et si non nécessaire, séparer le réseau industriel du réseau bureautique interne</t>
+  </si>
+  <si>
+    <t>securite-infrastructure-mises-a-jour-fonctionnelles-securite-equipements-securite-deployees_niveau1</t>
+  </si>
+  <si>
+    <t>Déployer systématiquement toutes les mises à jour sur les équipements de sécurité dès que celles-ci sont disponibles</t>
+  </si>
+  <si>
+    <t>securite-infrastructure-mises-a-jour-fonctionnelles-securite-systemes-exploitation-securite-deployees_niveau1</t>
+  </si>
+  <si>
+    <t>Déployer systématiquement toutes les mises à jour sur les serveurs, services et logiciels d'administration dès que celles-ci sont disponibles</t>
+  </si>
+  <si>
+    <t>securite-infrastructure-mises-a-jour-fonctionnelles-securite-systemes-exploitation-securite-deployees_niveau2</t>
+  </si>
+  <si>
+    <t>Mettre en œuvre des mesures de sécurité supplémentaires sur les serveurs, services et logiciels d'administration ne pouvant pas bénéficier des mises à jour</t>
+  </si>
+  <si>
+    <t>securite-infrastructure-outils-securisation-systeme-messagerie_niveau1</t>
+  </si>
+  <si>
+    <t>Mettre en œuvre une solution d'anti-spam et d'anti-hameçonnage</t>
+  </si>
+  <si>
+    <t>securite-infrastructure-outils-securisation-systeme-messagerie_niveau2</t>
+  </si>
+  <si>
+    <t>Mettre en œuvre des mécanismes complémentaires de protection contre les mails illégitimes</t>
+  </si>
+  <si>
+    <t>securite-infrastructure-acces-wifi-securises_niveau1</t>
+  </si>
+  <si>
+    <t>Mettre en place des mesures de sécurisation wifi</t>
+  </si>
+  <si>
+    <t>securite-infrastructure-acces-wifi-securises_niveau2</t>
+  </si>
+  <si>
+    <t>Créer un sous-réseau wifi dédié aux visiteurs</t>
+  </si>
+  <si>
+    <t>securite-infrastructure-espace-stockage-serveurs_niveau1</t>
+  </si>
+  <si>
+    <t>Protéger les informations et les systèmes contre des atteintes physiques</t>
+  </si>
+  <si>
+    <t>securite-infrastructure-espace-stockage-serveurs_niveau2</t>
+  </si>
+  <si>
+    <t>Mettre en place un système de vidéoprotection</t>
+  </si>
+  <si>
+    <t>sensibilisation-actions-sensibilisation-menace-et-bonnes-pratiques_niveau1</t>
+  </si>
+  <si>
+    <t>Mettre en œuvre des bonnes pratiques de sensibilisation</t>
+  </si>
+  <si>
+    <t>sensibilisation-actions-sensibilisation-menace-et-bonnes-pratiques_niveau2</t>
+  </si>
+  <si>
+    <t>En complément des pratiques déjà en œuvre, mettre en place des actions de sensibilisation additionnelles</t>
+  </si>
+  <si>
+    <t>sensibilisation-risque-espionnage-industriel-r-et-d_niveau1</t>
+  </si>
+  <si>
+    <t>Mener des actions de sensibilisation ciblée auprès du personnel effectuant des déplacements</t>
+  </si>
+  <si>
+    <t>sensibilisation-collaborateurs-soumis-obligations-usages-securises_niveau1</t>
+  </si>
+  <si>
+    <t>Établir une charte informatique</t>
+  </si>
+  <si>
+    <t>sensibilisation-collaborateurs-soumis-obligations-usages-securises_niveau2</t>
+  </si>
+  <si>
+    <t>S'assurer que la charte informatique est annexée au contrat de travail et est signée par les salariés</t>
+  </si>
+  <si>
+    <t>reaction-surveillance-veille-vulnerabilites-potentielles_niveau1</t>
+  </si>
+  <si>
+    <t>S’abonner aux alertes de sécurité publiées par le centre gouvernemental de veille, d'alerte et de réponses aux cyberattaques</t>
+  </si>
+  <si>
+    <t>reaction-surveillance-veille-vulnerabilites-potentielles_niveau2</t>
+  </si>
+  <si>
+    <t>Réaliser une veille proactive des vulnérabilités informatiques</t>
+  </si>
+  <si>
+    <t>reaction-sauvegardes-donnees-realisees_niveau1</t>
+  </si>
+  <si>
+    <t>Réaliser des sauvegardes régulièrement</t>
+  </si>
+  <si>
+    <t>reaction-sauvegardes-donnees-realisees-oui-ponctuellement-tiroir-environnement-isole_niveau1</t>
+  </si>
+  <si>
+    <t>Disposer d'une copie de sauvegarde des données critiques “hors ligne”, isolé de l'environnement bureautique</t>
+  </si>
+  <si>
+    <t>reaction-sauvegardes-donnees-realisees-oui-ponctuellement-tiroir-sauvegarde-testee-regulierement_niveau1</t>
+  </si>
+  <si>
+    <t>Procéder à des tests de restauration des sauvegardes</t>
+  </si>
+  <si>
+    <t>reaction-sauvegardes-donnees-realisees-oui-automatique-et-reguliere-tiroir-environnement-isole_niveau1</t>
+  </si>
+  <si>
+    <t>reaction-sauvegardes-donnees-realisees-oui-automatique-et-reguliere-tiroir-sauvegarde-testee-regulierement_niveau1</t>
+  </si>
+  <si>
+    <t>reaction-dispositif-gestion-crise-adapte-defini_niveau1</t>
+  </si>
+  <si>
+    <t>Lister les personnes à contacter en cas de cyberattaque</t>
+  </si>
+  <si>
+    <t>reaction-dispositif-gestion-crise-adapte-defini_niveau2</t>
+  </si>
+  <si>
+    <t>Définir un dispositif de gestion de crise d'origine cyber</t>
+  </si>
+  <si>
+    <t>urn_prefix</t>
+  </si>
+  <si>
+    <t>prefix_id</t>
+  </si>
+  <si>
+    <t>prefix_value</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>#555555
+#8B0000
+#209226</t>
+  </si>
+  <si>
+    <t>#555555
+#8B0000
+/
+/</t>
+  </si>
+  <si>
+    <t>#555555
+#8B0000
+/
+/
+/</t>
+  </si>
+  <si>
+    <t>#000000
+#555555
+#8B0000
+/
+/</t>
+  </si>
+  <si>
+    <t>#555555
+#8B0000
+#209226
+#209226</t>
+  </si>
+  <si>
+    <t>#000000
+#555555
+/
+#209226
+#209226</t>
+  </si>
+  <si>
+    <t>#000000
+#555555
+#8B0000
+#209226</t>
+  </si>
+  <si>
+    <t>#555555
+#209226
+/
+/</t>
+  </si>
+  <si>
+    <t>#555555
+#8B0000
+/</t>
+  </si>
+  <si>
+    <t>#555555
+/
+/
+/</t>
+  </si>
+  <si>
+    <t>#000000
+#555555
+#8B0000
+#209226
+#209226</t>
+  </si>
+  <si>
+    <t>#000000
+#555555
+#8B0000
+/</t>
+  </si>
+  <si>
+    <t>Question 33.1 dépendante de la Question 33</t>
+  </si>
+  <si>
+    <t>Question 33.2 dépendante de la Question 33</t>
+  </si>
+  <si>
+    <t>Question 44.1 dépendante de la Question 44</t>
+  </si>
+  <si>
+    <t>Question 44.2 dépendante de la Question 44</t>
+  </si>
+  <si>
+    <t>Question 44.3 dépendante de la Question 44</t>
+  </si>
+  <si>
+    <t>Question 44.4 dépendante de la Question 44</t>
+  </si>
+  <si>
+    <t>Question 8.1 dépendante de la Question 8</t>
+  </si>
+  <si>
+    <t>Question 8.2 dépendante de la Question 8</t>
+  </si>
+  <si>
+    <t>Questions dépendantes de la Question 7</t>
+  </si>
+  <si>
+    <t>Questions dépendantes de la Question 6</t>
+  </si>
+  <si>
+    <t>Questions dépendantes de la Question 5</t>
+  </si>
+  <si>
+    <t>Questions dépendantes de la Question</t>
+  </si>
+  <si>
+    <t>MonAideCyber aide les entités publiques et privées sensibilisées à la sécurité informatique à passer à l’action. Le dispositif MonAideCyber est développé par l'Agence Nationale de la Sécurité des Systèmes d'Information, en lien avec BetaGouv et la Direction interministérielle du numérique.
+ Sources :
+	• https://github.com/betagouv/mon-aide-cyber 
+	• https://monaide.cyber.gouv.fr/diagnostic-libre-acces</t>
+  </si>
+  <si>
+    <t>node_id</t>
+  </si>
+  <si>
+    <t>## Entités publiques
+Les entités publiques sont invitées à s'orienter vers le service ANSSI https://club.ssi.gouv.fr/ pour bénéficier d'outils gratuits d’audits automatisés.</t>
+  </si>
+  <si>
+    <t>## Des dispositifs adaptés
+Selon le secteur d’activité et la région sélectionnés, l’entité se verra proposer des dispositifs adhoc.</t>
+  </si>
+  <si>
+    <t>## Moins de 9 postes
+Si l’entité dispose de moins de 9 postes, le questionnaire MonAideCyber se verra légèrement simplifié. Ainsi, les questions 12, 33 et 34 seront facultatives.</t>
+  </si>
+  <si>
+    <t>## Attaque ciblée
+Si oui, des questions additionnelles liées à la maîtrise des accès utilisateurs et à la sécurisation des données jugées sensibles seront abordées.
+Exemples d’informations et de données pouvant être faire l’objet d’une attaque ciblée : secrets industriels, données de R&amp;D, brevets d'invention, données innovantes jugées vitales pour l’activité de l’entité, données clientes confidentielles.</t>
+  </si>
+  <si>
+    <t>## Systèmes industriels
+Si oui, des questions dédiées à la sécurité des systèmes industriels seront abordées.
+Exemples de systèmes industriels : objet ou machine industrielle connectée, automates programmables, systèmes numériques de contrôle-commande, systèmes instrumentés de sécurité, capteurs et actionneurs,  bus de terrain, logiciels de supervision et de contrôle SCADA, logiciels de gestion de production assistée par ordinateur (GPAO, GMAO, MES), logiciels d’ingénierie et de maintenance, systèmes embarqués, Gestion Technique Centralisée (GTC), Gestion Technique du Bâtiment (GTB), équipements biomédicaux, etc.</t>
+  </si>
+  <si>
+    <t>## Statistiques anonymes
+Attention, bien préciser à l’entité que cette question est utile à des fins de statistiques anonymisées. Aucune action ne sera menée si jamais elle n’a pas déposé plainte suite à une cyberattaque.</t>
+  </si>
+  <si>
+    <t>## À protéger en priorité 
+Peuvent être jugées prioritaires :
+	• les activités critiques, indispensables à l’activité,
+	• les informations sensibles, confidentielles et/ou ne devant pas être volées et exfiltrées
+Exemples d’activités et de données à protéger en priorité, classées par ordre de priorité :
+	• Production et données techniques de production
+	• R&amp;D et données d’industrialisation
+	• Paie des salariés et données bancaires associées
+	• Facturation et données clients
+	• Courriels, agenda et données bureautiques associées</t>
+  </si>
+  <si>
+    <t>## Interconnexions extérieures
+IP publiques, accès distants ouverts aux prestataires et partenaires, etc.
+## Entités publiques
+Les entités publiques sont éligibles au service gratuit SILENE de l’ANSSI qui permet d’identifier la surface d’attaque des services exposés sur Internet.&lt;br /&gt; Pour y accéder, l’entité est invitée à s'orienter vers le service ANSSI https://club.ssi.gouv.fr/.</t>
+  </si>
+  <si>
+    <t>## **SYSTÈME INDUSTRIEL**
+## Composants
+Équipements réseaux (routeur, switch/commutateur, borne-wifi, pare-feu et autres équipements de sécurité), les serveurs (en précisant leurs fonctionnalités), les infrastructures de sauvegarde, les postes de travail utilisateurs et les supports mobiles interconnectés au réseau.</t>
+  </si>
+  <si>
+    <t>## CNIL
+Attention à ne pas tomber dans un contrôle de conformité au RGPD, ces informations ne seront pas partagées à la CNIL. Si nécessaire, rappeler de manière pédagogique que le Règlement Général sur Protection des Données est une obligation réglementaire qui s’applique à toute entité, publique et privée, qui gère et stocke des données personnelles.
+## Données personnelles 
+Exemples de données personnelles :
+	• Données liées au personnel,
+	• Données des clients ou des usagers,
+	• Données des fournisseurs ou partenaires.</t>
+  </si>
+  <si>
+    <t>## Utilisation des données personnelles
+Il existe une page d’information dédiée à l'utilisation des données personnelles et la gestion des droits d’informations et les moyens de les exercer sur le site de la CNIL : https://www.cnil.fr/fr/respecter-les-droits-des-personnes</t>
+  </si>
+  <si>
+    <t>## Contrats des prestataires
+Cette question suppose que l’entité ait des contrats avec ses prestataires et sait lesquels ont accès à son système d’information, sinon, nous vous invitons à cocher “Non, aucune exigence ne figure dans nos contrats de prestation.”
+Exemples d’exigences pouvant être intégrées dans un contrat : changement des mots de passe par défaut ; sécurisation des accès distants ; délai de déploiement des mises à jour critiques ; signalement en cas de cyberattaque ; contractualisation d'un plan d'assurance sécurité (PAS).
+## Systèmes industriels
+Si l’entité est concernée, cette question s’applique également pour les prestataires disposant d’accès informatiques sur les systèmes industriels</t>
+  </si>
+  <si>
+    <t>## Entités publiques
+Les entités publiques sont éligibles au service gratuit ADS de l’ANSSI qui permet d’analyser le niveau de sécurité de l’annuaire centralisé. Pour y accéder, l’entité est invitée à s’orienter vers le service ANSSI https://club.ssi.gouv.fr/
+## Active Directory, Samba-AD
+À partir d’un parc informatique d’une dizaine de postes, il est fortement recommandé de s’appuyer sur une solution de type Active Directory ou Samba-AD, et de ne plus s’appuyer sur un réseau en “Workgroup” afin d’homogénéiser le niveau de sécurité des postes de travail.</t>
+  </si>
+  <si>
+    <t>## **ATTAQUE CIBLÉE**
+## Accès et comptes prioritaires
+Les accès et comptes utilisateurs à maitriser en priorité sont ceux permettant d’ouvrir une session sur le poste de travail et ceux permettant d’accéder aux données jugées les plus sensibles. Selon les cas, ces accès et comptes sont gérés via un Active Directory et/ou un service Cloud et/ou applicatif(s) métier(s).</t>
+  </si>
+  <si>
+    <t>## Administration locale des postes
+Cette question traite du privilège d'administration local des comptes utilisateurs sur leur poste de travail, il permet par exemple aux utilisateurs d'être autonome dans l'installation d'applications et la configuration de leur machine.
+Si le personnel est autorisé à utiliser son matériel personnel (BYOD) pour travailler et accéder aux systèmes d’information de l’entité, nous vous invitons à cocher “Oui”.</t>
+  </si>
+  <si>
+    <t>## Mots de passe 
+Exigences minimales acceptables :
+	• Longueur de mots de passe à minima de 12 caractères si compte non administrateur local
+	• Longueur de mots de passe à minima de 16 caractères si compte administrateur local
+	• Construction complexe avec par ex l’utilisation de minuscules, majuscules, chiffres et caractères spéciaux
+	• 1 renouvellement annuel des mots de passe, et lors d'une suspicion d'une cyberattaque</t>
+  </si>
+  <si>
+    <t>## Comptes d’administration
+NB : cette question traite des comptes d'administration systèmes sur les serveurs, infrastructures etc. L'administration locale des postes de travail est traitée dans la question sur les utilisateurs administrateurs de leurs postes</t>
+  </si>
+  <si>
+    <t>## Comptes d’administration
+NB : cette question traite des comptes d'administration systèmes sur les serveurs, infrastructures etc. L'administration locale des postes de travail est traitée dans la question sur les utilisateurs administrateurs de leurs postes. 
+Exemple de restrictions :
+	• Tous les administrateurs utilisent en parallèle un compte utilisateur sans privilèges pour les usages du quotidien (ex : surf sur internet, messagerie, etc.)
+	• 1 seul compte administrateur du domaine
+	• Le compte administrateur du domaine n’est utilisé qu’exceptionnellement
+	• Le compte d’administration de la solution de sauvegarde différent n’est pas géré via l’annuaire centralisé (ex : Active Directory, Samba-AD)</t>
+  </si>
+  <si>
+    <t>## **ATTAQUE CIBLÉE**
+## Données sensibles
+Nous vous invitons à vous focaliser sur les ressources et données qui étaient jugées prioritaires lors de la question sur les informations et activités à protéger. 
+Exemples de mesures acceptables :
+	• Contraintes renforcées de robustesse et de longueur de mots de passe (16 caractères minimum)
+	• Authentification multifacteur
+	• Protection des données dans un conteneur chiffré “à froid” et lors d’un transfert via Internet (ex : mail)
+	• Utilisation d'une solution de Data Loss Prevention permettant de limiter les fuites de données</t>
+  </si>
+  <si>
+    <t>## Authentification multifacteur 
+Exemples de facteur d’authentification :
+	• l’usage d’une carte à puce et d’un code PIN d’authentification ;
+	• l’usage d’un token physique et d’un code PIN d’authentification ;
+	• l’utilisation d’une application dédiée sur un smartphone idéalement professionnel (ex : Windows Authentificator, Twilio Authy, etc.), ou à défaut un code envoyé par sms idéalement sur un téléphone professionnel</t>
+  </si>
+  <si>
+    <t>## **SYSTÈME INDUSTRIEL**</t>
+  </si>
+  <si>
+    <t>## Authentification renforcée
+Pour répondre aux exigences de la réponse “Oui, des mesures renforçant l’authentification ont été mises en œuvre”, l’entité doit appliquer au moins les premières mesures suivantes :
+	• Modification des mots de passe par défaut
+	• Contraintes renforcées de robustesse et de longueur de mots de passe (16 caractères minimum)
+	• Stockage des mots de passes d’administration des services critiques (ex : annuaire centralisé, sauvegarde, messagerie) en dehors du système d’information (ex : feuille papier dans un meuble fermé à clef, coffre-fort, etc)</t>
+  </si>
+  <si>
+    <t>## Mises à jour installées
+Pour cocher la réponse “Toutes les mises à jour sont déployées […]”, l’entité doit s’assurer que les mises à jour sont bien installées.
+## Mesures complémentaires 
+Mesures complémentaires pouvant être menées pour sécuriser les postes de travail obsolètes :
+	• les isoler et les cloisonner du reste du réseau bureautique (ex : déconnecter de l’annuaire centralisée), une compromission de ces derniers aura ainsi un faible impact
+	• mettre en œuvre un outil de protection de type EDR en complément de l’antivirus intégrant des règles de sécurité spécifiques aux postes obsolètes.
+## Déploiement des logiciels et contrôle des mises à jour 
+Afin de s’assurer que les mises à jours sont déployées, il peut être nécessaire de :
+	• faire une vérification manuelle sur chaque poste et pour chaque logiciel (à l’aide d’un script/programme exécuté sur chaque poste)
+	• déployer un agent logiciel réalisant la vérification (outil de gestion des vulnérabilités)
+	• utiliser un outil de gestion centralisé des logiciels : un tel outil permet de connaître l’état de déploiement des logiciels (et notamment leur version) de chaque poste de manière centralisée</t>
+  </si>
+  <si>
+    <t>## Mises à jour installées
+Pour cocher la réponse “Oui et ses alertes sont systématiquement traitées […]”, l’entité doit s’assurer que les mises à jour sont bien installées.
+## Windows Defender
+Windows Defender est l’antivirus intégré gratuitement dans tous les systèmes d’exploitation Windows récents.</t>
+  </si>
+  <si>
+    <t>## Pare-feu local
+Le pare-feu local est un logiciel qui permet de filtrer le trafic entrant et sortant dans le système d’exploitation du poste de travail. Un pare-feu local est une fonction intégrée à la plupart des systèmes d’exploitation grand public. Par défaut, ce logiciel est désactivé ou d’un niveau de paramétrage insuffisant. Un niveau suffisant serait de restreindre les communications réseaux directes entre les postes de travail et de bloquer toute connexion entrante. Des pare-feux sont également commercialisés en complément de suites logicielles antivirales.</t>
+  </si>
+  <si>
+    <t>## EDR
+Un EDR, Endpoint Detection Response, détecte et bloque les menaces sur les terminaux en s’appuyant sur l’analyse comportementale et la corrélation d'événements.</t>
+  </si>
+  <si>
+    <t>## **ATTAQUE CIBLÉE**
+## Windows Bitlocker
+Windows Bitlocker est un outil de chiffrement intégré gratuitement dans tous les systèmes d’exploitation Windows récents.
+NB : il est indispensable que le déchiffrement au démarrage du poste soit soumis à un mot de passe robuste (ou un token USB).
+## Matériels nomades 
+Il s’agit des équipements et matériels numériques transportés durant les déplacements, exemples :
+	• ordinateur portable
+	• tablette
+	• téléphone
+	• clefs USB et disques durs</t>
+  </si>
+  <si>
+    <t>## Pare-feu
+Le pare-feu est l’outil permettant de restreindre les services exposés sur Internet, et réalisant le filtrage des communications et des flux réseaux. Afin de réduire au maximum la surface d’attaque disponible pour les attaquants, il est recommandé de réduire au maximum les services et les flux accessibles depuis Internet.
+Par exemple, il est fortement déconseillé d’autoriser l’accès à distance vers des objets connectés (ex : caméra, imprimante, sondes etc.)
+NB : une box Internet n’est pas à considérer comme un pare-feu physique puisqu’elle ne permet pas de filtrer efficacement les flux sortants.</t>
+  </si>
+  <si>
+    <t>## **SYSTÈME INDUSTRIEL**
+## Cloisonnement des systèmes industriels
+Le plus sécurisé est un cloisonnement strict (pas d’interconnexion). De manière plus fonctionnelle, les flux réseaux entre les réseaux bureautique et industriel sont filtrés strictement (pour ne laisser passer que les flux des applications strictement nécessaires). Il est par ailleurs fortement conseillé de bloquer l’accès à distance vers des objets connectés (ex : caméra, équipements industriels, sondes etc.) sans restriction particulière (adresse IP source) ou sans passer par un VPN.</t>
+  </si>
+  <si>
+    <t>## Équipements de sécurité 
+Exemples d’équipements de sécurité à mettre à jour dès que possible :
+	• Pare-feu réseau, pare-feu applicatif (WAF)
+	• Équipement VPN
+	• Proxy</t>
+  </si>
+  <si>
+    <t>## Serveurs et services d’administration 
+Exemples des serveurs et des services d’administration à mettre à jour dès que possible :
+	• Serveurs d’infrastructures : Windows Server, Active Directory, serveur gestionnaire de mises à jour WSUS, serveur de messagerie (exchange, zimbra, etc.), solution de virtualisation, outil de supervision et de télémaintenance, solution de sauvegarde
+	• Serveurs métiers : base de données, serveur web (Apache, IIS, etc.), serveur d’application, outil de développement et autres applicatifs etc.
+## Mesures complémentaires 
+Mesures complémentaires pouvant être menées pour sécuriser les serveurs obsolètes :
+	• les isoler et les cloisonner du reste du réseau bureautique (ex : déconnecter de l’annuaire centralisée)
+	• ne pas les interconnecter à Internet
+	• mettre en œuvre un outil de protection de type EDR intégrant des règles de sécurité spécifiques aux serveurs obsolètes.</t>
+  </si>
+  <si>
+    <t>## Mécanismes de protection 
+Les mécanismes de protection de mails illégitimes à paramétrer sur le serveur DNS sont :
+	• Sender Policy Framework (SPF) qui permet de spécifier les adresses IP des serveurs autorisés à émettre les mails d’un domaine ;
+	• DomainKeys Identified Mail (DKIM) qui permet l’authentification du domaine de messagerie d’un mail à l’aide d’une signature cryptographique
+	• Domain-based Message Authentication, Reporting and Conformance (DMARC) qui permet notamment à une entité de définir une politique de traitement de ses mails envoyés en fonction des résultats de conformité SPF et DKIM
+Si l’entité (ou son prestataire) ne maitrise pas ces éléments, il est conseillé de se faire accompagner par un prestataire spécialisé.</t>
+  </si>
+  <si>
+    <t>## **ATTAQUE CIBLÉE**
+## Chiffrement de connexion 
+Minimum attendu pour cocher la 4ème réponse :
+	• Mot de passe de 20 caractères minimum ;
+	• Chiffrement robuste de la connexion wifi, a minima WPA2 ;
+	• Pas d'accès au réseau interne pour les visiteurs via le Wi-Fi (SSID différent, sous-réseau différent ou Wi-Fi non accessible au visiteur).</t>
+  </si>
+  <si>
+    <t>## **ATTAQUE CIBLÉE**
+## Accès aux serveurs
+Pour sélectionner “Oui”, l’accès aux serveurs doit être à minima protégé par une porte fermée à clef dont la clef n’est accessible qu’aux personnes légitimes.
+## Référent sûreté de gendarmerie et de police
+Si c’est jugé nécessaire, l’entité peut être mise en relation avec un référent sûreté physique de la gendarmerie et de la police.</t>
+  </si>
+  <si>
+    <t>## Actions de sensibilisation 
+Exemple d'actions de sensibilisation :
+	• Campagne d'affichage, mails d'information, conférence de sensibilisation
+	• Sensibilisation ciblée du CODIR, sensibilisation aux risques d'escroquerie au faux ordre de virement et fraude au président
+	• Sensibilisation en ligne des utilisateurs, ex : https://www.cybermalveillance.gouv.fr/sens-cyber/apprendre
+	• Campagne de faux phishing
+	• Formation en ligne, ex : [https://secnumacademie.gouv.fr](https://secnumacademie.gouv.fr/) , https://pix.fr/actualites/partenariat-pix-anssi-cybermalveillance
+Ressources de sensibilisation gratuites : https://www.cybermalveillance.gouv.fr/tous-nos-contenus/actualites/liste-des-ressources-mises-a-disposition Des actions de sensibilisation gratuites peuvent être menées en sollicitant la police ou la gendarmerie nationales : https://www.masecurite.interieur.gouv.fr/fr</t>
+  </si>
+  <si>
+    <t>## **ATTAQUE CIBLÉE**
+## Passeport de conseils cyber aux voyageurs
+L’ANSSI a publié un guide pour sensibiliser les collaborateurs aux bonnes pratiques de cybersécurité durant les déplacements : https://cyber.gouv.fr/publications/bonnes-pratiques-lusage-des-professionnels-en-deplacement</t>
+  </si>
+  <si>
+    <t>## Entités publiques
+Les entités publiques sont éligibles au service gratuit SILENE de l’ANSSI qui permet d’identifier la surface d’attaque des services exposés sur Internet. Pour y accéder, l’entité est invitée à s'orienter vers le service ANSSI https://club.ssi.gouv.fr/.
+## Suivi des alertes et des vulnérabilités
+Le suivi des alertes et des vulnérabilités consiste à se tenir informé des vulnérabilités techniques de cybersécurité critiques pouvant affecter son système d’information (selon les équipements et les systèmes utilisés). Des services gratuits centralisent et répertorient ces vulnérabilités, par exemple le site du [CERT-FR de l'ANSSI.](https://www.cert.ssi.gouv.fr/)</t>
+  </si>
+  <si>
+    <t>## Jeu de sauvegarde isolé 
+Le jeu de sauvegarde isolé (ou sanctuarisé) peut être réalisé de plusieurs manières :
+	• sur un périphérique de stockage déconnecté du réseau (bandes, disques durs externes, clefs usb),
+	• dans un cloud externe privé, non interconnecté à l'environnement bureautique, via une authentification spécifique,
+	• sur un serveur ou média déconnecté physiquement et/ou logiquement à l’issue de chaque sauvegarde.
+Ce jeu de sauvegarde ne doit donc pas être accessible via l’Active Directory (ou autre service d'annuaire centralisé).
+## Sauvegarde des ressources hébergées en cloud
+Il convient aussi de s’assurer que les mécanismes de sauvegarde mis en œuvre par l’entité (ou par son prestataire) / prennent également en compte les ressources bureautiques et/ou métiers qui sont seulement hébergées dans des environnements cloud.</t>
+  </si>
+  <si>
+    <t>## Organisation de gestion de crise
+Une organisation de gestion de crise doit à minima identifier les priorités métier à rétablir en cas de crise, des fiches réflexes opérationnelles garantissant la continuité d'activité au travers de modes dégradés défini avec les métiers (ex : assurer la paie, poursuivre la production, gestion des agendas, etc.), des moyens et modalités de communication de crise.</t>
+  </si>
+  <si>
+    <t>## Pourquoi ?
 Cette mesure permet de remettre au centre de la démarche de sécurisation les véritables enjeux de sécurité de l’entité et de prioriser les efforts de sécurisation « au bon endroit ».
-# Comment ?
+## Comment ?
 La liste des activités et des informations doit être établie de manière collective, au cours d’un atelier de réflexion impliquant les directions métiers et/ou les décideurs de l’organisation. Chaque contributeur réfléchi, à son niveau, aux activités et/ou données qui semblent essentielles à la continuité des missions de l’organisation, et qui par conséquent, ne peuvent être indisponibles, altérés ou volées/divulguées. Ces réflexions sont présentés en séance, et font l’objet d’une validation commune (et si nécessaire, d’arbitrages). Cette liste, énumérant 5 activités et données à protéger en priorité, peut ensuite être formalisée sur une fiche A4 sous la forme ci-dessous. Activités et données à protéger en priorité, classées par ordre de priorité :
 	• 1.Production et données techniques de production
 	• 2.R&amp;D et données d’industrialisation
@@ -1364,126 +2186,66 @@
 	• 5.Mail/Agenda et données</t>
   </si>
   <si>
-    <t>gouvernance-infos-et-activites-a-proteger_niveau2</t>
-  </si>
-  <si>
-    <t>Établir la liste exhaustive et à jour des activités métiers et des informations à protéger en priorité</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Cette mesure permet de remettre au centre de la démarche de sécurisation les véritables enjeux de sécurité de l’entité et de prioriser les efforts de sécurisation « au bon endroit ». Une réflexion exhaustive permet d’avoir une vision détaillée de tous les enjeux de sécurité de l’entité.
-# Comment ?
+## Comment ?
 Au sein de chaque service de l’entité, une réflexion doit être menée afin d’établir la liste exhaustive des activités et des données à protéger en priorité au sein de ce service. Après avoir centralisé l’ensemble des listes établies par les services, une réunion de réflexion impliquant les décideurs doit être menée afin de prioriser ces éléments selon par exemple 3 critères : indispensable, important, dispensable. Cette réflexion doit être réactualisée à minima tous les 3 ans avec les décideurs.</t>
   </si>
   <si>
-    <t>gouvernance-schema-si-a-jour_niveau1</t>
-  </si>
-  <si>
-    <t>Disposer d’un schéma global du réseau informatique et de la liste des interconnexions vers l’extérieur à jour</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Pour bien se protéger de manière adaptée et pour faire le point sur les besoins et les capacités numériques actuels, il est nécessaire pour l’entité d’avoir une vision d’ensemble et une lisibilité quasi exhaustive de son réseau informatique et à minima un schéma général. Cette lisibilité est nécessaire pour instaurer un dialogue clair entre les différents interlocuteurs techniques et métiers et à décider des mesures de sécurité prioritaires à mener.
 La liste des interconnexions vers l’extérieur permet de mener des actions de sécurisation sur les adresses IP exposées sur internet ce qui est un aspect fondamental de la sécurité d’un système d’information dans la durée car elles représentent pour les hackers les principaux points d’accès et « portes d’entrée » au réseau informatique. En effet, les services exposés sur internet peuvent être exploités par des acteurs malveillants ou par des robots.
 De mauvaises pratiques, des erreurs de configuration des équipements réseaux ou encore des oublis d’anciens services obsolètes ont souvent comme résultat l’exposition d’interfaces d’administration ou de services internes qui sont autant de points d’entrée dans le système d’information.
 En cas de cyberattaque et de crise, ce schéma et cette liste à d’interconnexions à jour seront les premiers éléments d’information qui seront utilisées par les experts et prestataires à réponses à incident afin d’effectuer un premier point de situation, d’appréhender le potentiel mode opératoire appliqué par le cyberattaquant et de prendre les mesures d’endiguement et de sécurisation adaptées.
-# Comment ?
+## Comment ?
 A l’instar d’un plan d'évacuation, le schéma global du réseau informatique (incluant les systèmes industriels si concerné) doit pouvoir tenir sur une page et représenter les différentes zones d’administration (environnement bureautique centralisant les postes de travail,  serveurs, etc.), le plan d’adressage IP associé, les équipements réseaux et listant toutes les interconnexions vers l’extérieur (Internet, accès distants, réseaux partenaires ou prestataires, etc.). Il est recommandé d’imprimer des versions papiers de ces éléments.</t>
   </si>
   <si>
-    <t>gouvernance-schema-si-a-jour_niveau2</t>
-  </si>
-  <si>
-    <t>Disposer de la liste des équipements et applicatifs concourant au fonctionnement du système d’information</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 En complément d’un schéma global et de la liste des interconnexions vers l’extérieur, la liste des équipements et des applicatifs permet d’avoir une meilleure lisibilité sur le système d’information au sein de l’organisation et de la partager. Ces éléments permettent d’identifier plus facilement les équipements et applicatifs les plus critiques et les plus exposés afin d’en d’anticiper les chemins d’attaque possibles et de mettre en place des mesures de sécurisation adéquates.
-# Comment ?
+## Comment ?
 L’équipe informatique (ou le prestataire) doit lister de manière exhaustive :
 	• tous les équipements physiques composant le système d’information, incluant les équipements réseaux (routeur, switch/commutateur, borne-wifi, pare-feu et autres équipement de sécurité), les serveurs (en précisant leurs fonctionnalités), les infrastructures de sauvegarde, les postes de travail utilisateurs et les supports mobiles interconnectés au réseau
 	• tous les applicatifs et composants logiciels installés, en précisant leur nature et leurs fonctions principales</t>
   </si>
   <si>
-    <t>gouvernance-schema-si-industriel-a-jour_niveau1</t>
-  </si>
-  <si>
-    <t>Disposer d’un schéma global du réseau industriel et de la liste des interconnexions vers l’extérieur à jour</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Pour bien se protéger de manière adaptée et pour faire le point sur les besoins et les capacités numériques actuels, il est nécessaire pour l’entité d’avoir une vision d’ensemble et une lisibilité quasi exhaustive de son réseau informatique et à minima un schéma général. Cette lisibilité est nécessaire pour instaurer un dialogue clair entre les différents interlocuteurs techniques et métiers et à décider des mesures de sécurité prioritaires à mener.
 La liste des interconnexions vers l’extérieur permet de mener des actions de sécurisation sur les adresses IP exposées sur internet ce qui est un aspect fondamental de la sécurité d’un système d’information dans la durée car elles représentent pour les hackers les principaux points d’accès et « portes d’entrée » au réseau informatique. En effet, les services exposés sur internet peuvent être exploités par des acteurs malveillants ou par des robots.
 De mauvaises pratiques, des erreurs de configuration des équipements réseaux ou encore des oublis d’anciens services obsolètes ont souvent comme résultat l’exposition d’interfaces d’administration ou de services internes qui sont autant de points d’entrée dans le système d’information.
 En cas de cyberattaque et de crise, ce schéma et cette liste à d’interconnexions à jour seront les premiers éléments d’information qui seront utilisées par les experts et prestataires à réponses à incident afin d’effectuer un premier point de situation, d’appréhender le potentiel mode opératoire appliqué par le cyberattaquant et de prendre les mesures d’endiguement et de sécurisation adaptées.
 En complément des informations précédentes, le schéma et un inventaire des interconnexions à jour sont d’autant plus nécessaire sur le réseau industriel puisqu’un incident informatique sur ce dernier peut avoir des répercussions grave sur la production.
-# Comment ?
+## Comment ?
 A l’instar d’un plan bâtimentaire, le schéma global du réseau industriel doit pouvoir tenir sur une page et représenter les différentes zones (PLC, capteurs, actionneurs, stations d’ingénierie et de supervision, etc), le plan d’adressage IP associé, les équipements réseaux et listant toutes les interconnexions vers l’extérieur (Internet, accès distants, réseaux partenaires ou prestataires, etc.). Il est recommandé d’imprimer des versions papiers de ces éléments.</t>
   </si>
   <si>
-    <t>gouvernance-schema-si-industriel-a-jour_niveau2</t>
-  </si>
-  <si>
-    <t>Disposer de la liste des équipements et applicatifs concourant au fonctionnement des systèmes industriels</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 En complément d’un schéma global et de la liste des interconnexions vers l’extérieur, la liste des équipements et des applicatifs permet d’avoir une meilleure lisibilité sur le système d’information au sein de l’organisation et de la partager. Ces éléments permettent d’identifier plus facilement les équipements et applicatifs les plus critiques et les plus exposés afin d’en d’anticiper les chemins d’attaque possibles et de mettre en place des mesures de sécurisation adéquates.
-# Comment ?
+## Comment ?
 L’équipe informatique (ou le prestataire) doit lister de manière exhaustive :
 	• tous les équipements physiques composant le système d’information, incluant les équipements réseaux (routeur, switch/commutateur, borne-wifi, pare-feu et autres équipement de sécurité), les serveurs (en précisant leurs fonctionnalités), les infrastructures de sauvegarde, les postes de travail utilisateurs et les supports mobiles interconnectés au réseau
 	• tous les applicatifs et composants logiciels installés, en précisant leur nature, leurs fonctions principales et éventuellement leurs versions
 	• la liste des machines-outils, capteurs ou autres équipements industriels connectés au réseau et/ou à l’internet</t>
   </si>
   <si>
-    <t>gouvernance-connaissance-rgpd-1_niveau1</t>
-  </si>
-  <si>
-    <t>Établir la liste des données personnelles traitées au sein de votre entité</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Le RGPD est une réglementation devant être obligatoirement appliquée par des entités stockant et traitant des données personnelles (cela concerne ainsi quasiment toutes les entités publiques et privées). Le RGPD encadre le traitement des données personnelles sur le territoire de l’Union européenne qui a pour principaux objectifs de protéger les données personnelles et de préserver les libertés individuelles offrant ainsi aux professionnels un cadre juridique unique dans leur démarche d’innovation et le développement des services numériques. Si l’entité ne respecte pas les exigences du RPGD, cette dernière encourt des mises en demeure et des sanctions financières pouvant s’élever au minimum à 5 000€ et jusqu’à 20 millions d’euros (ou 4% du CA mondial si supérieur).
 L’établissement d’un registre de vos traitements de données personnelles est une exigence réglementaire de la CNIL. Au-delà de l’exigence réglementaire, ce registre vous permettra d’établir l’état des lieux exhaustif des données personnelles transitant au sein de votre système d’information et vous permettra d’en avoir une meilleure maitrise. Il s’agit d’une première étape indispensable pour mener sa démarche de conformité RGPD.
-# Comment ?
+## Comment ?
 Le site de la CNIL regroupe en grand nombre de ressources et des modules de formation en ligne pour comprendre la réglementation et mettre en en œuvre les premières de conformité. La CNIL a publié tout particulièrement un modèle prêt à l’emploi via le lien suivant : https://www.cnil.fr/fr/RGDP-le-registre-des-activites-de-traitement</t>
   </si>
   <si>
-    <t>gouvernance-connaissance-rgpd-1_niveau2</t>
-  </si>
-  <si>
-    <t>Établir votre registre des activités de traitement de données personnelles et le tenir à jour</t>
-  </si>
-  <si>
-    <t>gouvernance-connaissance-rgpd-2_niveau1</t>
-  </si>
-  <si>
-    <t>Fournir des informations aux personnes concernées sur l'utilisation de leurs données personnelles</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Il s’agit d’une exigence réglementaire, principe fondateur au cœur du RPGD. Les individus ont des droits sur leurs données : vous devez les en informer et leur permettre de les exercer.
-# Comment ?
+## Comment ?
 Pour la formalisation des mentions d’information, il est conseillé de s’appuyer sur les exemples partagés par la CNIL suivants : https://www.cnil.fr/fr/rgpd-exemples-de-mentions-dinformation
 Pour ce qui est de la mise en place des moyens permettant aux personnes concernées d’exercer et faire valoir leurs droits (droits d’accès, rectification, opposition, suppression, etc.), il est préconisé de s’appuyer sur la page d’information dédiée de la CNIL : https://www.cnil.fr/fr/respecter-les-droits-des-personnes
 Selon les problématiques de ressources humaines au sein de l’entité, il est peut-être envisagé de se faire accompagner par un prestataire pour lancer et mettre en œuvre cette mesure.</t>
   </si>
   <si>
-    <t>gouvernance-connaissance-rgpd-2_niveau2</t>
-  </si>
-  <si>
-    <t>Mettre en place les modalités permettant aux personnes d'exercer de leurs droits</t>
-  </si>
-  <si>
-    <t>gouvernance-exigence-cyber-securite-presta_niveau1</t>
-  </si>
-  <si>
-    <t>Fixer des exigences de cybersécurité aux prestataires</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Par méconnaissance ou par facilité d’exploitation, un prestataire pourrait ne pas mettre en œuvre et appliquer des bonnes pratiques de sécurité numérique générale, ou celles, plus spécifiques que le bénéficiaire aurait choisi de mettre en œuvre. L’ajout d’exigence de sécurité numérique dans les contrats, vis-à-vis d’un prestataire, responsabilise le prestataire et ses personnels vis-à-vis de ses propres comportements (réduisant ainsi directement les risques).
-# Comment ?
+## Comment ?
 Tout d'abord, il est nécessaire de s'assurer que chacune des prestations est liée à un contrat avec le prestataire. Puis, il convient de confirmer si un accès au système d'information est nécessaire. Enfin, il est recommandé de lister les mesures et les bonnes pratiques de sécurité à exiger aux prestataires au travers d’un clausier cyber type. Ces exigences de sécurité doivent être sélectionnés avec prudence, d’une part en fonction des spécificités du système d’information, d’autre part en tenant compte de la nature des prestations externalisées. mesures pourraient par exemple portées sur :
 	• le recensement et justification des dispositifs de télémaintenance
 	• la sécurisation des accès distants (ex : chiffrement et filtrage des flux d’administration, utilisation des comptes d’administration nominatifs avec privilèges limités au strict nécessaire sauf contrainte justifiée, double authentification ou authentification via VPN seulement etc.),
@@ -1497,15 +2259,9 @@
 Pour aller plus loin un exemple de plan d'assurance sécurité a été formalisé par l'ANSSI dans le guide "Maîtriser les risques de l'infogérance" : https://cyber.gouv.fr/sites/default/files/IMG/pdf/2010-12-03_Guide_externalisation.pdf</t>
   </si>
   <si>
-    <t>gouvernance-exigence-cyber-securite-presta_niveau2</t>
-  </si>
-  <si>
-    <t>Vérifier l'application et imposer des pénalités aux prestataires en cas de non-respect des exigences de cybersécurité</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Cette mesure peut permettre d’obtenir une réparation (au moins financier) en cas de cyberattaque touchant le bénéficiaire mais pouvant être attribuée à un non-respect par le prestataire des règles de sécurité fixées par contrat (partage du risque). La mise en œuvre permet également de responsabiliser davantage le prestataire sur l’application des mesures de sécurité fixées dans le contrat.
-# Comment ?
+## Comment ?
 Sur la base des exigences fixées, les pénalités peuvent être du type :
 	• pour un service SaaS / une prestation d’infogérance : pénalité en cas d’indisponibilité du service/des données intègre(s) (en €/heure, €/jour d’indisponibilité) ;
 	• pour une prestation/une fourniture : pénalités de retard (en €/heure, €/jour de retard)
@@ -1513,146 +2269,80 @@
 La cyberattaque doit également être exclue des « cas de forces majeures ».</t>
   </si>
   <si>
-    <t>acces-outil-gestion-des-comptes_niveau1</t>
-  </si>
-  <si>
-    <t>Mettre en œuvre un outil de gestion des politiques de sécurité centralisées (ex : Active Directory, Samba-AD) et en évaluer/améliorer son niveau de sécurité annuellement</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Un outil de ce type permet de faciliter le suivi et la gestion (création, modification, suppressions) des accès utilisateurs et administrateurs au travers d’une console d’administration les centralisant. Ces outils permettent également d’homogénéiser les exigences de sécurité et de les déployer massivement (restriction d’administration, restriction des connexions, gestion des mots de passe, configuration des postes de travail et des navigateurs).
-# Comment ?
+## Comment ?
 Les principaux outils utilisés sont Active Directory (environnement sous Microsoft), Samba-AD (environnement sous Linux). Ces outils sont gratuits mais peuvent nécessiter un accompagnement extérieur, notamment dans l’optique d’en sécuriser leur paramétrage puisque la mise en place d’un tel outil induit de nouveaux risques de cybersécurité tel que la compromission de cet outil par un cyberattaquant pour faciliter son mode opératoire. Pour les entités publiques, l’ANSSI met à disposition gratuitement son outil ADS/ORADAD de recherches de vulnérabilités via le service ANSSI https://club.ssi.gouv.fr/. Pour les entités privées, des outils gratuits tels que Purple Knight et Pingcastle. Les codes sources d’ADS/ORADAD sont également disponibles : https://github.com/ANSSI-FR/ORADAD . Cette analyse doit être à minima menée une fois par an.</t>
   </si>
   <si>
-    <t>acces-outil-gestion-des-comptes_niveau2</t>
-  </si>
-  <si>
-    <t>Contrôler régulièrement le niveau de sécurité de son outil de gestion de politiques de sécurité centralisé</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Si un tel outil est utilisé, il en devient le centre névralgique de la sécurité de l’environnement bureautique. Il induit ainsi de forts risques de cybersécurité tel que la compromission des comptes administrateurs par un cyberattaquant entraînant par conséquent une prise de contrôle instantanée et complète de tout le SI. Il convient donc de s’assurer de son niveau de sécurité, et ce de manière régulièrement, puisque les pratiques et les paramétrages des administrateurs peuvent engendrer l’apparition de nouvelles vulnérabilités.
-# Comment ?
+## Comment ?
 Pour les entités publiques, l’ANSSI met à disposition gratuitement son outil ADS/ORADAD de recherches de vulnérabilités via le service ANSSI https://club.ssi.gouv.fr/. Pour les entités privées, des outils gratuits tels que Purple Knight et Pingcastle. Les codes sources d’ADS/ORADAD sont également disponibles : https://github.com/ANSSI-FR/ORADAD . Cette analyse doit être à minima menée une fois par trimestre. Il est également conseillé de se faire accompagner par un prestataire extérieur pour mener ces analyses et les corrections associées.</t>
   </si>
   <si>
-    <t>acces-liste-compte-utilisateurs_niveau1</t>
-  </si>
-  <si>
-    <t>Réaliser annuellement une revue des accès utilisateurs en les comparant avec les informations détenues par le service RH</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Lors d’une compromission, les cyberattaquants ont tendance à soit utiliser des accès utilisateurs dits « dormants » car inutilisés, soit en se créant un faux compte d’accès. Des revues régulières permettent donc d’assainir la base d’annuaire des accès, désactiver les comptes « dormants » et supprimer les comptes suspicieux.
-# Comment ?
+## Comment ?
 A minima une fois par an, un contrôle peut être réalisé en comparant avec l’inventaire du personnel détenu par le service RH et la liste des comptes informatiques créés dans l’annuaire. Les comptes en écart (ex : comptes en doublons, compte d’un ancien personnel, compte ne pouvant être attribué à aucune personne, etc.) par rapport à la liste fournie par le service RH doivent être désactivés. Une analyse similaire doit être menée sur les comptes fournis aux prestataires et partenaires. Les mots de passes des comptes partagés concernés par un départ sont à renouveler. NB : si un ou plusieurs comptes suspects sont présents, c’est un signe important de compromission et des investigation supplémentaires devraient être menées (afin de déterminer : depuis quand, les activités de ce compte suspect, comment il a été créé)</t>
   </si>
   <si>
-    <t>acces-liste-compte-utilisateurs_niveau2</t>
-  </si>
-  <si>
-    <t>Définir avec le service RH des processus de « circuit arrivée » et « circuit départ » assurant les créations et les désactivations des comptes utilisateurs</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 La définition de tels processus permet d’inclure l’administrateur gérant les comptes lors de l’arrivée d’un nouveau collaborateur (ou prestataire) mais surtout lors de son départ. Ainsi la base des comptes est mise à jour et reste maitrisée de manière permanente.
-# Comment ?
+## Comment ?
 Le processus doit être convenu entre le service RH et celui administrant les comptes (de manière à être le plus efficace pour les deux parties). Il peut s’agir par exemple d’un mail du service RH vers l’administrateur informatique ou d’un RDV obligatoire organisé par les services RH au profit du collaborateur avec l’administrateur. En complément, les revues régulières et comparaison des bases RH et informatiques doivent être maintenues. Un processus similaire doit également être mis en œuvre avec les services en charge des contrats avec les prestataires disposant d'accès au système d'information.</t>
   </si>
   <si>
-    <t>acces-droits-acces-utilisateurs-limites_niveau1</t>
-  </si>
-  <si>
-    <t>Restreindre l'accès aux données à protéger en priorité aux seules personnes autorisées à y accéder</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Il est nécessaire de limiter les autorisations d’accès aux données et applications métiers, notamment celles à protéger en priorité, afin de limiter le risque de vol et de sabotage en cas de compromission sur le système d’information. La probabilité d’un risque d’atteinte à ces données sera donc limitée aux seuls utilisateurs ayant accès à celles-ci, et non à l’ensemble des collaborateurs si aucune restriction n’est mise en place.
-# Comment ?
+## Comment ?
 Avant de paramétrer ces restrictions, il est conseillé d’établir un tableau répertoriant la liste des utilisateurs légitimes nécessitant un accès en fonction des systèmes et/ou applications et/ou données à protéger en priorité. Ce tableau pourra ensuite être communiqué à l’équipe informatique (ou prestataire) pour l’implémenter dans les applications et systèmes concernés.</t>
   </si>
   <si>
-    <t>acces-droits-acces-utilisateurs-limites_niveau2</t>
-  </si>
-  <si>
-    <t>Pour les systèmes et applications à protéger en priorité, définir et gérer les utilisateurs selon 2 niveaux de privilèges distincts : 1 niveau "accès complet" et 1 niveau "accès restreint"</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Il est nécessaire de limiter les autorisations d’accès aux données et applications métiers, notamment celles à protéger en priorité, afin de limiter le risque de vol et de sabotage en cas de compromission sur le système d’information. La probabilité d’un risque d’atteinte à ces données sera donc limitée aux seuls utilisateurs ayant accès à celles-ci, et non à l’ensemble des collaborateurs si aucune restriction n’est mise en place.
-# Comment ?
+## Comment ?
 Avant de paramétrer ces restrictions, il est conseillé d’établir un tableau répertoriant la liste des utilisateurs légitimes nécessitant un accès en fonction des systèmes et/ou applications et/ou données à protéger en priorité. Pour chacun des utilisateurs il devra être préciser s’il doit bénéficier d’un « accès complet » (accès à toutes les données) ou « accès restreint » (accès seulement aux données nécessaires à son activité). Ce tableau pourra ensuite être communiqué à l’équipe informatique (ou prestataire) pour l’implémenter dans les applications et systèmes concernés.</t>
   </si>
   <si>
-    <t>acces-administrateurs-informatiques-suivie-et-limitee_niveau1</t>
-  </si>
-  <si>
-    <t>Réaliser tous les 6 mois une revue des accès administrateurs en les comparant avec les informations détenues par le service RH</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Lors d’une cyberattaque, les cyberattaquants ont tendance à chercher à prendre la main et compromettre un ou plusieurs administrateurs. Soit en compromettant des accès administrateurs dits « dormants » car inutilisés, soit en se créant un faux compte administrateurs suite à la compromission d’un 1er compte administrateur (ex : faible robustesse du mot de passe, compromission d’un poste administrateur, défaut de mise à jour). Des revues régulières permettent de gagner en maitrise sur ses accès administrateurs, assainir et réduire la liste des comptes administrateurs, désactiver les comptes « dormants » et supprimer les comptes suspicieux. NB : si un ou plusieurs comptes suspects sont présents, c’est un signe important de compromission et des investigation supplémentaires devraient être menées (afin de déterminer : depuis quand, les activités de ce compte suspect, comment il a été créé)
-# Comment ?
+## Comment ?
 A minima une fois tous les 6 mois, sur la base d’un inventaire, un contrôle peut être réalisé en établissant la liste des comptes administrateurs (prestataires inclus) en précisant leur périmètre. Pour chacun de ces comptes administrateur, il est nécessaire d’en justifier et confirmer l’intérêt opérationnel, les accès en écart (ex : accès en doublons, accès d’un ancien salarié, accès inutiles) doivent être désactivés et les mots de passes des comptes partagés concernés par un départ sont à renouveler.</t>
   </si>
   <si>
-    <t>acces-administrateurs-informatiques-suivie-et-limitee_niveau2</t>
-  </si>
-  <si>
-    <t>Définir avec les administrateurs des processus de « circuit arrivée » et « circuit départ » assurant les créations et les désactivations des comptes administrateurs</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 La définition de tels processus permet d’inclure l’administrateur gérant des accès lors de l’arrivée d’un nouveau collaborateur mais surtout lors de son départ. Ainsi la base des accès est mise à jour et reste maitrisée de manière permanente.
-# Comment ?
+## Comment ?
 Avant de définir ces processus, il convient d’organiser une réunion entre les administrateurs (prestataire inclus), et si nécessaire les services RH et les services responsables de contrats de prestataires disposant d'accès au systèmes d'informations, pour identifier les modes opératoires et pratiques les plus accessibles et efficaces pour chaque partie prenante ayant pour objectif de maitriser davantage les comptes administrateurs. Il peut s’agir par exemple d’un mail de ces services vers l’administrateur afin d’un mouvement de personnel ou changement de prestataire. En complément, les revues régulières et la justification de chaque compte administrateur administrateurs doivent être maintenues. Si jugé applicable, des profils types métiers « administrateurs », détaillant les accès administrateurs nécessaires, peuvent également être coconstruits entre les services précédemment cités et les équipes informatiques. Pour chaque nouveau projet informatique (application, migration, infrastructures, changement de prestataire), il est nécessaire de confirmer l’intérêt et justifier chacun des nouveaux accès d’administration.</t>
   </si>
   <si>
-    <t>acces-utilisation-comptes-administrateurs-droits-limitee_niveau1</t>
-  </si>
-  <si>
-    <t>Utiliser des comptes d'administration dédiés à cet usage</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Les comptes d’administrations sont des comptes à hauts privilèges c’est pourquoi ils sont très ciblés par les cyberattaquants. Si un de ces comptes est compromis, un cyberattaquant est en mesure de réaliser une compromission massive rapidement. Il convient donc d’en limiter leur usage. Si un administrateur utilise un seul compte pour ses tâches bureautiques et ses tâches d’administration et que ce compte est compromis, l’attaquant dispose directement des privilèges d’administration. Si un administrateur dispose de 2 comptes en séparant ses usages, 1 compte "bureautique" utilisé pour les tâches bureautiques et 1 compte administrateur utilisé pour les tâches d’administration ; alors le compte le plus exposé le compte “bureautique”) pourrait être compromis sans que l’attaquant obtiennent directement les privilèges d’administration. En plus, de la compromission du compte "bureautique", l’attaquant devra réaliser d’autres actions malveillantes pour obtenir les privilèges administrateur de la personne. Il s’agit donc d’une mesure de protection des privilèges d’administration et de réduction de l’impact de la compromission. NB: cette mesure est rendue caduque notamment par situations suivantes :
 	• le compte utilisation est “administrateur local” de son poste : si l’utilisateur est “administrateur local” de son poste de travail, l’attaquant qui a compromis son compte pourra très facilement compromettre aussi ses comptes d'administrations dès qu’ils seront utilisés sur ce même poste de travail.;
 	• le compte administrateur est utilisé pour la consultation Internet et la messagerie électronique : si le compte administrateur est utilisé pour la messagerie électronique et la consultation d’Internet, il devient aussi exposé au risque de compromission qu’un compte utilisateur (l’effet “protection des privilèges d’administration” est annulé).;
 	• les mots de passe des deux comptes sont identiques : si les deux comptes partagent le même mot de passe, l’attaquant qui a compromis le compte utilisateur n’aura aucune difficulté à compromettre le compte administrateur.
 La séparation des comptes d’administration de l’annuaire centralisé (ex: Active Directory, Samba-AD, etc.) et des sauvegardes (ou de la plateforme de virtualisation), relève de la même logique. Elle vise a protéger, en dernier recours, les sauvegardes. En effet, si le système centralisé de gestion des droits d’accès est compromis et que le compte d’administration des sauvegardes est géré par ce système, alors l’attaquant sera en mesure d’obtenir facilement les privilèges d’administration (notamment la suppression) les sauvegardes.
-# Comment ?
+## Comment ?
 Il faut dans un premier temps s’assurer de la création d’un compte utilisateur (sans privilèges d’administration) pour chacun des administrateurs. Ces comptes utilisateurs, via une authentification spécifique, devront être alors utilisés pour l’accès à l’internet, aux boites mails et aux fonctionnalités d’ordre administratif et bureautique.
 Les comptes administrateurs, via une authentification spécifique, seront alors utilisés pour les opérations de maintenance informatique, administration des services, gestion des sauvegardes, gestion des utilisateurs et des accès, de paramétrage des systèmes et des applications, etc.
 Il est également recommandé d’utiliser 2 autres comptes administrateurs distincts (et une authentification spécifique) : 1 seul compte pour gérer l’administration de l’outil de gestion centralisée de politiques de sécurité (exemple : Active Directory, Samba-AD) et 1 seul compte pour gérer la solution de sauvegarde (NB : ce compte ne doit pas être non géré via l’outil de gestion centralisée de politiques de sécurité).
 Par ailleurs le compte d'administrateur du domaine ne doit être utilisé que de manière exceptionnelle (ex: migration, gestion des relations d'approbation, etc.). Le mot de passe de ce compte doit être stocké dans un coffre-fort.</t>
   </si>
   <si>
-    <t>acces-utilisation-comptes-administrateurs-droits-limitee_niveau2</t>
-  </si>
-  <si>
-    <t>Utiliser des comptes d'administration distincts selon les périmètres d’administration</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Les comptes d’administrations sont des comptes à hauts privilèges c’est pourquoi ils sont très ciblés par les cyberattaquants. Si un de ces comptes est compromis, un cyberattaquant est en mesure de réaliser une compromission massive rapidement. Il convient donc d’en limiter leur usage et leur périmètre d’administration pour réduire l’impact d’une compromission d’un de ces comptes.
-# Comment ?
+## Comment ?
 Il convient de créer plusieurs comptes d'administrations distincts (et via des authentifications spécifiques) selon les différents périmètres d’administration, exemple :
 	• 1 compte d'administration des postes de travail
 	• Des comptes d'administration pour chaque systèmes à administrer (1 compte pour le serveur de messagerie, 1 compte pour le serveurs de fichiers, 1 compte pour l’ERP et/ou 1 compte pour chaque serveur d’application à protéger en priorité)
 	• 1 compte pour l'administration de la plateforme de virtualisation</t>
   </si>
   <si>
-    <t>acces-utilisateurs-administrateurs-poste_niveau1</t>
-  </si>
-  <si>
-    <t>Limiter drastiquement le nombre d’utilisateurs disposant du privilège d’administration local sur leur machine</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Lorsqu’un utilisateur est « administrateur » de son poste, il dispose d’un compte lui permettant de modifier la configuration du poste. Ainsi, un logiciel malveillant exécuté par l’utilisateur (par erreur et/ou à son insu) dispose directement de privilèges élevés sur le poste (les privilèges « administrateur » permettant de modifier la configuration). Le logiciel malveillant pourra alors notamment se rendre « persistant » (un logiciel malveillant est persistant quand il est capable de se redémarrer lui-même même après un redémarrage électrique du poste) ou désactiver les fonctions de sécurité du poste afin de se rendre indétectable (désactivation de l’antivirus, de l’EDR, modification des paramètres de journalisation) ou de faciliter la latéralisation (étape d’une attaque au cours de laquelle l’attaquant étend son emprise sur plusieurs équipements) en désactivant par exemple le pare-feu local. Dans certains de cas de compromission, il a aussi été constaté que le mot de passe du compte administrateur local était commun à toutes les machines ce qui facilite la latéralisation (du point de vue de l’attaquant).
 La situation est la même lorsqu’une personne utilise ses périphériques personnels (ordinateurs, smartphone, etc.) pour se connecter aux ressources professionnelles, en ajoutant les risques liés à l’utilisation du poste par les cercles familiaux et amicaux (par exemple: un enfant pourrait faire un usage inconsidéré des privilèges d’administration pour installer une version gratuite d’un jeu vidéo qui contiendrait un cheval de Troie)
-# Comment ?
+## Comment ?
 Par défaut, il est recommandé de créer aux utilisateurs de comptes utilisateurs ne disposant pas de privilège d’administration. Les utilisateurs souhaitant ce privilège doivent les justifier et utiliser un compte distinct dédié à cet usage. Par conséquent, seuls les administrateurs chargés de l’administration des postes doivent disposer de ces droits lors de leurs interventions.
 Dans un environnement Microsoft, il est recommandé d’étudier la mise en œuvre de "Just Enough and Just In Time Administration" https://learn.microsoft.com/fr-fr/shows/windowsserver/just-enough-just-in-time-administration-in-windows-server-2016 et de LAPS : https://learn.microsoft.com/fr-fr/windows-server/identity/laps/laps-overview
 La mise à disposition d’un magasin étoffé d’applications « store d’application » validées par l’entité permettra de répondre à la majorité des besoins d’installation des utilisateurs.
@@ -1663,15 +2353,9 @@
 Il est préconisé de s’appuyer sur les compétences d’un prestataire externe, idéalement labellisé Expert Cyber ou référencé par un Campus Cyber, pour la mise en œuvre de cette mesure.</t>
   </si>
   <si>
-    <t>acces-mesures-securite-robustesse-mdp_niveau1</t>
-  </si>
-  <si>
-    <t>Fixer des critères de longueur et complexité des mots de passe et encourager l’usage d’un coffre-fort de mots de passe</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Cette mesure permet de diminuer le risque de découverte et d'usurpation de mots de passe par des acteurs malveillants, par exemple, en testant de nombreux mots de passe sur la base de mots de dictionnaires, à la recherche de mots de passe simples à découvrir.'
-# Comment ?
+## Comment ?
 Des exigences sur la création des mots de passe peuvent être implémentées via l’outil de gestion centralisée de politiques de sécurité (exemple : Active Directory, Samba-AD). Par défaut, utiliser au moins la règle de force de mot de passe suivante :
 	• Nombre de caractères : 12 caractères minimum, idéalement 16
 	• Caractères spéciaux : au moins une minuscule, au moins une majuscule, au moins un chiffre, au moins un caractère spécial de la liste suivante : #?!@$%^&amp;*-'+_()[]. Au-delà de 20 caractères, il peut être envisageable d’enlever les contraintes sur les caractères spéciaux. Lors de la création d’un mot de passe, éviter les mots du dictionnaire, les suites de lettres, les suites de chiffre, les dates, les informations personnelles (nom, prénom, date de naissance). Un renouvellement trop fréquent n’est pas recommandé. Il vaut mieux privilégier un changement des mots de passe en cas de suspicion ou bien de manière annuelle. Les deux outils suivants peuvent être recommandés aux utilisateurs ou administrateurs :
@@ -1680,15 +2364,9 @@
 Si nécessaire, il est conseillé de poursuivre les actions de communication et de promotion des coffres fort de mot de passe.</t>
   </si>
   <si>
-    <t>acces-mesures-securite-robustesse-mdp_niveau2</t>
-  </si>
-  <si>
-    <t>Mettre à disposition des utilisateurs une coffre fort de mots de passe et les former régulièrement à la création de mots de passe robustes</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Cette mesure permet de diminuer le risque de découverte et d'usurpation de mots de passe par des acteurs malveillants, par exemple, en testant de manière automatique (attaque par force brute) de nombreux mots de passe sur la base de mots de dictionnaires, à la recherche de mots de passe simples à découvrir. Si un attaquant a réussi à compromettre un des ordinateurs du réseau, la mise en œuvre de mots de passe robustes sur l'ensemble des comptes permet de limiter le risque que cet attaquant compromettre d'autres comptes en découvrant leur mots de passe (réduction de l'impact de l'attaque) Les personnes soumises à des contraintes trop fortes (ex : renouvellement fréquent) auront la fâcheuse tendance à utiliser un même mot de passe pour s’authentifier sur plusieurs services ou comptes différents, ce qui représente une pratique à hauts risques. Un coffre-fort de mots de passe permet de stocker des mots de passe sans que l’utilisateur ait besoin de les mémoriser. Les coffres-forts de mots de passe offrent également la possibilité de générer automatiquement des mots de passe robustes. Ces mots de passe sont alors conservés dans une base de données dédiée et chiffrée par un mot de passe dit « maître », le seul qui doit alors être mémorisé par l’utilisateur.
-# Comment ?
+## Comment ?
 Des exigences sur la création des mots de passe peuvent être implémentées via l’outil de gestion centralisée de politiques de sécurité (exemple : Active Directory, Samba-AD). Par défaut, utiliser au moins la règle de force de mot de passe suivante :
 	• Nombre de caractères : 12 caractères minimum, idéalement 16
 	• Caractères spéciaux : au moins une minuscule, au moins une majuscule, au moins un chiffre, au moins un caractère spécial de la liste suivante : #?!@$%^&amp;*-'+_()[]. Au-delà de 20 caractères, il peut être envisageable d’enlever les contraintes sur les caractères spéciaux. Lors de la création d’un mot de passe, éviter les mots du dictionnaire, les suites de lettres, les suites de chiffre, les dates, les informations personnelles (nom, prénom, date de naissance). Un renouvellement trop fréquent n’est pas recommandé. Il vaut mieux privilégier un changement des mots de passe en cas de suspicion ou bien de manière annuelle. Les deux outils suivants peuvent être recommandés aux utilisateurs ou administrateurs :
@@ -1697,15 +2375,9 @@
 Il est recommandé d’installer sur les postes de travail et inciter auprès des collaborateurs l’utilisation un coffre-fort de mots de passe permettant facilement de générer des mots de passe robustes et différents pour chaque accès nécessitant une authentification distincte. Une communication ou une réunion spécifique peut être organisée pour présenter cet outil, ses fonctionnalités et proposer des moyens mnémotechniques pour créer un ou plusieurs mots de passe robustes (cf. [construire un mot de passe sûr et gérer la liste de ses codes d’accès | CNIL](https://www.cnil.fr/fr/les-conseils-de-la-cnil-pour-un-bon-mot-de-passe) )</t>
   </si>
   <si>
-    <t>acces-utilisateurs-donnees-sensibles-mesures-securite-additionnelles_niveau1</t>
-  </si>
-  <si>
-    <t>Protéger de manière spéficique les données jugées sensibles</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 En cas de compromission d’un ou plusieurs postes de travail, la mise en œuvre des mesures supplémentaires de sécurisation des accès aux systèmes, applications et données à protéger en priorité permet d’en limiter les risques d’espionnage et d’exfiltration.
-# Comment ?
+## Comment ?
 Cette mesure peut inclure la mise en oeuvre de plusieurs bonnes pratiques :
 	• Contraintes renforcées de robustesse et de longueur de mots de passe (idéalement 16 caractères)
 	• Utilisation d'un mécanisme d'authentification multifacteur
@@ -1713,83 +2385,47 @@
 Les contraintes renforcées sur les mots de passe peuvent être implémentées via l’outil de gestion centralisée de politiques de sécurité (exemple : Active Directory, Samba-AD).</t>
   </si>
   <si>
-    <t>acces-utilisateurs-donnees-sensibles-mesures-securite-additionnelles_niveau2</t>
-  </si>
-  <si>
-    <t>Mettre en place des mesures additionnelles de sécurisation des données jugées sensibles</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 En cas de compromission d’un ou plusieurs postes de travail, la mise en œuvre des mesures supplémentaires de sécurisation au niveau des données et au niveau des accès aux systèmes, applications et données à protéger en priorité permet d’en limiter les risques d’espionnage et d’exfiltration.
-# Comment ?
+## Comment ?
 Cette mesure peut inclure la mise en oeuvre de plusieurs bonnes pratiques :
 	• Protection des données dans un conteneur chiffré “à froid” et lors d’un transfert via Internet (ex : mail)
 	• Procédure de suppression et mise à rebut des disques Il est préconisé de s’appuyer sur les compétences d’un prestataire externe, idéalement labellisé Expert Cyber, pour la mise en œuvre d’une solution de chiffrement ; d’une solution de Data Loss Prevention ; d’une procédure de suppression et mise à rebut des disques. Pour aller plus loin et si vous êtes éligible à la réglementation liée à la Protection du Potentiel Scientifique et Technique, vous pouvez prendre contact auprès des services du Haut fonctionnaire de défense et de sécurité de votre ministère de rattachement : https://www.sgdsn.gouv.fr/nos-missions/proteger/proteger-le-potentiel-scientifique-et-technique-de-la-nation/foire-aux-questions</t>
   </si>
   <si>
-    <t>acces-teletravail-acces-distants-mesures-particulieres_niveau1</t>
-  </si>
-  <si>
-    <t>Mettre en place pour tous les accès distants des mécanismes de double authentification à minima</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Les points d’accès accessible via Internet représentant la première surface d’attaque éprouvée très régulièrement de manière automatisée par les cyberattaques, il convient donc de les sécuriser davantage
-# Comment ?
+## Comment ?
 En se basant sur les listes exhaustives des accès distants ou dits « télétravaillés », il est recommandé de mettre en place des mécanismes de double authentification (exemple : code OTP reçu par sms, par mail, via application ou clef sécurisée dédiée, par certificat) avec à minima, avec des restrictions via adresses IP légitimes. Des restrictions complémentaires pourraient par exemple mise en œuvre sur la localisation des accès entrants (ex : pays), les plages horaires acceptées (exemple : heures ouvrées seulement), procédure ponctuelle d’ouverture et de fermeture de l’accès durant chaque intervention à distance.
 Il est préconisé de s’appuyer sur les compétences d’un prestataire externe, idéalement labellisé Expert Cyber, pour la mise en œuvre de cette mesure.</t>
   </si>
   <si>
-    <t>acces-teletravail-acces-distants-mesures-particulieres_niveau2</t>
-  </si>
-  <si>
-    <t>Gérer tous les accès distants via un VPN, lui même authentifié à double facteur</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Les points d’accès accessible via Internet représentant la première surface d’attaque éprouvée très régulièrement de manière automatisée par les cyberattaques, il convient donc de les sécuriser davantage. Une solution VPN « full-tunneling » sera une contrainte supplémentaire pour un cyberattaquant et permet de sécuriser davantage les flux d’authentification.
-# Comment ?
+## Comment ?
 En se basant sur les listes exhaustives des accès distants ou dits « télétravaillés », il est recommandé de les rendre accessible seulement au travers d’une solution de VPN « full-tunneling » établissant un tunnel VPN IPsec entre les postes nomades et une passerelle VPN IPsec. Aucun flux distant ne doit pouvoir être transmis en dehors de ce tunnel.
 En complément il est conseillé de mettre en place des mécanismes de double authentification (exemple : code OTP reçu par sms, par mail, via application ou clef sécurisée dédiée, par certificat) avec à minima, avec des restrictions via adresses IP légitimes. Des restrictions complémentaires pourraient par exemple mise en œuvre sur la localisation des accès entrants (ex : pays), les plages horaires acceptées (exemple : heures ouvrées seulement), procédure ponctuelle d’ouverture et de fermeture de l’accès durant chaque intervention à distance.
 Il est préconisé de s’appuyer sur les compétences d’un prestataire externe, idéalement labellisé Expert Cyber ou référencé par un campus cyber régional pour la mise en œuvre de cette mesure.</t>
   </si>
   <si>
-    <t>acces-si-industriel-teletravail-acces-distants-mesures-particulieres_niveau1</t>
-  </si>
-  <si>
-    <t>Mettre en place pour tous les accès distants des systèmes industriels des mécanismes de double authentification</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Les points d’accès accessible via Internet représentant la première surface d’attaque éprouvée très régulièrement de manière automatisée par les cyberattaques, il convient donc de les sécuriser davantage.
-# Comment ?
+## Comment ?
 En se basant sur les listes exhaustives des accès distants ou dits « télétravaillés » des systèmes industriels, il est recommandé de mettre en place des mécanismes de double authentification avec à minima, avec des restrictions via adresses IP légitimes. Des restrictions complémentaires pourraient par exemple mise en œuvre sur la localisation des accès entrants (ex : pays), les plages horaires acceptées (exemple : heures ouvrées seulement), procédure ponctuelle d’ouverture et de fermeture de l’accès durant chaque intervention à distance.
 Il est préconisé de s’appuyer sur les compétences d’un prestataire externe, idéalement labellisé Expert Cyber, pour la mise en œuvre de cette mesure.</t>
   </si>
   <si>
-    <t>acces-si-industriel-teletravail-acces-distants-mesures-particulieres_niveau2</t>
-  </si>
-  <si>
-    <t>Gérer tous les accès distants des systèmes industriels via un VPN, lui même authentifié à double facteur</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Les points d’accès accessible via Internet représentant la première surface d’attaque éprouvée très régulièrement de manière automatisée par les cyberattaques, il convient donc de les sécuriser davantage. Une solution VPN « full-tunneling » sera une contrainte supplémentaire pour un cyberattaquant et permet de sécuriser davantage les flux d’authentification.
-# Comment ?
+## Comment ?
 En se basant sur les listes exhaustives des accès distants ou dits « télétravaillés » des systèmes industriels, il est recommandé de les rendre accessible seulement au travers d’une solution de VPN « full-tunneling » établissant un tunnel VPN IPsec entre les postes nomades et une passerelle VPN IPsec. Aucun flux distant ne doit pouvoir être transmis en dehors de ce tunnel.
 En complément il est conseillé de mettre en place des mécanismes de double authentification avec à minima, avec des restrictions via adresses IP légitimes. Des restrictions complémentaires pourraient par exemple mise en œuvre sur la localisation des accès entrants (ex : pays), les plages horaires acceptées (exemple : heures ouvrées seulement), procédure ponctuelle d’ouverture et de fermeture de l’accès durant chaque intervention à distance.
 Il est préconisé de s’appuyer sur les compétences d’un prestataire externe, idéalement labellisé Expert Cyber, pour la mise en œuvre de cette mesure.</t>
   </si>
   <si>
-    <t>acces-administrateurs-si-mesures-specifiques_niveau1</t>
-  </si>
-  <si>
-    <t>Protéger de manière spécifique les accès des admininistrateurs</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Cette mesure permet de réduire le risque de compromission des comptes d’administration et d'accès illicite aux fonctions d'administration du service par un cyberattaque et d’une compromission totale du système d’information.
-# Comment ?
+## Comment ?
 Cette mesure peut inclure la mise en oeuvre de plusieurs bonnes pratiques :
 	• Contraintes de complexité et de longueur des mots de passe (idéalement 16 caractères)
 	• Modification systématique des mots de passe par défaut et/ou à la première utilisation (admin métiers et admin SI)
@@ -1799,15 +2435,9 @@
 Il est préconisé de s’appuyer sur les compétences d’un prestataire externe, idéalement labellisé Expert Cyber, pour la mise en œuvre d’un coffre-fort de mots de passe ; de l’authentification multifacteur (exemple : code OTP reçu par sms, par mail, via application ou clef sécurisée dédiée, par certificat)</t>
   </si>
   <si>
-    <t>acces-administrateurs-si-mesures-specifiques_niveau2</t>
-  </si>
-  <si>
-    <t>Compléter les mesures de sécurisation des accès d’administration</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Cette mesure permet de réduire le risque de compromission des comptes d’administration et d'accès illicite aux fonctions d'administration du service par un cyberattaque et d’une compromission totale du système d’information.
-# Comment ?
+## Comment ?
 Cette mesure peut inclure la mise en oeuvre de plusieurs bonnes pratiques :
 	• Postes d’administration dédiés aux fonctions d'administration.
 	• Utilisation d'une solution de gestion des accès à privilèges (PAM, bastion, portail d'authentification).
@@ -1816,156 +2446,78 @@
 Il est préconisé de s’appuyer sur les compétences d’un prestataire externe, idéalement labellisé Expert Cyber, pour la mise en œuvre d’un coffre-fort de mots de passe ; d’une solution de gestion à accès à privilèges ; de l’authentification multifacteur on-premise (exemple : code OTP reçu par sms, par mail, via application ou clef sécurisée dédiée, par certificat)</t>
   </si>
   <si>
-    <t>securite-poste-maj-fonctionnelles-et-securite-deployees_niveau1</t>
-  </si>
-  <si>
-    <t>Déployer systématiquement toutes les mises à jour sur les postes de travail dès que celles-ci sont disponibles</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Tous les logiciels peuvent contenir des bugs. Ces bugs peuvent être utilisés par les cyberattaquants afin de déclencher des effets qui leurs sont favorables, on parle alors d'exploitation de vulnérabilités. Par exemple, si un utilisateur qui ne disposait que de privilèges restreints sur son poste, mais que le système d’exploitation de ce poste n’était pas à jour et contenait des vulnérabilités, un attaquant qui aurait réussi à faire ouvrir une pièce jointe d’un courriel malveillant à l’utilisateur pourrait, en utilisant ces vulnérabilités, obtenir les privilèges administrateurs (ce qui annihilerait la mesure de limitation des privilèges de l’utilisateur).
-# Comment ?
+## Comment ?
 Il est recommandé d'activer les fonctions de mise à jour automatique des postes de travail dès qu’elles proposées par les éditeurs.
 La mise à jour d'un produit ou d'un logiciel est une opération délicate qui doit être menée avec prudence. Il est notamment recommandé d'effectuer en amont des tests autant que possible. Des dispositions doivent également être prises pour garantir la continuité de service en cas de difficultés lors de l'application des mises à jour comme des correctifs ou des changements de version.
 Si jugé nécessaire, il peut être envisagé de mettre en œuvre un serveur de gestion des mises à jour centralisant permettant de monitorer et de déployer les mises à jour de manière automatique sur tous les postes. Pour cela, il est préconisé de s’appuyer sur les compétences d’un prestataire externe, idéalement labellisé Expert Cyber ou référencé par un Campus Cyber régional, pour la mise en œuvre de cette recommandation.</t>
   </si>
   <si>
-    <t>securite-poste-maj-fonctionnelles-et-securite-deployees_niveau2</t>
-  </si>
-  <si>
-    <t>Mettre en œuvre des mesures de sécurité supplémentaires sur les systèmes ne pouvant pas bénéficier des mises à jour</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Les postes de travail obsolètes, dont les systèmes ne sont plus supportés et/ou ne pouvant être mis à jour, représentent un haut risque de compromission. Des mesures supplémentaires peuvent être mises à œuvre pour traiter ces cas particuliers et sécuriser ces postes vulnérables.
-# Comment ?
+## Comment ?
 Plusieurs mesures complémentaires peuvent être menés pour sécuriser les postes de travail :
 	• les isoler et les cloisonner du reste du réseau bureautique (ex : déconnecter de l’annuaire centralisée), une compromission de ces derniers aura ainsi un faible impact
 	• mettre en œuvre un outil de protection de type EDR en complément de l’antivirus intégrant des règles de sécurité spécifiques aux postes obsolètes.
 Il est préconisé de s’appuyer sur les compétences d’un prestataire externe, idéalement labellisé Expert Cyber ou référencé par un Campus Cyber régional, pour la mise en œuvre de cette mesure.</t>
   </si>
   <si>
-    <t>securite-poste-si-industriel-maj-fonctionnelles-et-securite-deployees_niveau1</t>
-  </si>
-  <si>
-    <t>Déployer systématiquement toutes les mises à jour sur les postes de travail dédiés aux systèmes industriels dès que celles-ci sont disponibles</t>
-  </si>
-  <si>
-    <t>securite-poste-si-industriel-maj-fonctionnelles-et-securite-deployees_niveau2</t>
-  </si>
-  <si>
-    <t>Mettre en œuvre des mesures de sécurité supplémentaires sur les systèmes industriels ne pouvant pas bénéficier des mises à jour</t>
-  </si>
-  <si>
-    <t>securite-poste-antivirus-deploye_niveau1</t>
-  </si>
-  <si>
-    <t>Installer de manière systématique un antivirus sur les postes de travail</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Les antivirus sont très utiles à la protection des moyens informatiques : ils constituent une première ligne de défense contre les attaquants. Un antivirus protège des menaces connues qui évoluent très rapidement : des centaines de milliers de codes malveillants apparaissent chaque jour. Cet outil s’appuie sur une base de données de signature virale, elle est l’élément qui permet l’identification de programmes et de fichiers malveillants. Sans une mise à jour fréquente de cette base de données, la protection offerte par l'antivirus s'en trouve très rapidement plus restreinte. Il faut donc, pour cette raison, tenir à jour le logiciel en lui-même et sa base de données de signatures, puis en vérifier leurs bonnes mises à jour.
-# Comment ?
+## Comment ?
 Un antivirus doit être déployé sur la majorité des équipements informatiques, en priorité ceux connectés à Internet (postes de travail, serveurs de fichier, etc.). Il est nécessaire d'en vérifier régulièrement leur bon fonctionnement et leurs mises à jour. Les antivirus commerciaux proposent une mise à jour automatique, et un scan automatique des espaces de stockage : il est indispensable de procéder à l’activation de ces mécanismes dans les paramètres.
 Par ailleurs, lors de l’achat d'un antivirus, il peut être intéressant, en fonction des usages, de souscrire aux fonctionnalités complémentaires proposées par de nombreux éditeurs logiciels tels qu'un pare-feu, un filtrage Web, des outils anti-hameçonnage et de renforcement de la sécurité des transactions bancaires
 Il est préconisé de s’appuyer sur les compétences d’un prestataire externe, idéalement labellisé Expert Cyber, pour la mise en œuvre de cette recommandation.</t>
   </si>
   <si>
-    <t>securite-poste-antivirus-deploye_niveau2</t>
-  </si>
-  <si>
-    <t>Traiter systématiquement les alertes générées par l'antivirus</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 D’une part, les alertes générées par l’antivirus peuvent être le signe d’un mésusage des outils informatiques de la part des utilisateurs. D’autre part, sans action de l’utilisateur, une alerte d’antivirus peut être le signe d’une compromission du poste. Par exemple, un attaquant a obtenu un accès initial au poste par un autre moyen (phishing, vulnérabilité) et essaie d’utiliser des outils spécifiques (logiciel malveillant) qui sont détectés par l’antivirus. Sans investigation particulière des alertes, l’attaquant pourra faire autant de test que nécessaires avant de réussir à contourner l’antivirus.
-# Comment ?
+## Comment ?
 Il est nécessaire de traiter systématiquement les alertes générées par l’antivirus.
 Afin de maintenir un niveau de vigilance élevé de la part des utilisateurs (qui ne doivent pas considérer les alertes de l’antivirus comme une chose normale/habituelle), il est recommandé de contacter l’utilisateur du poste sur lequel une alerte antivirus a été générée.
 Très régulièrement (à minima 1 fois par semaine), il est conseillé de surveiller et d’analyser la console d’administration de la solution antivirale. Cette console permet également de s'assurer que les antivirus sont installés sur tous les postes, qu'il est actif et que sa base virale est à jour, et ainsi d'identifier les postes pour lesquels ce n'est pas le cas.
 Il est préconisé de s’appuyer sur les compétences d’un prestataire externe, idéalement labellisé Expert Cyber, pour la mise en œuvre de cette recommandation.</t>
   </si>
   <si>
-    <t>securite-poste-si-industriel-antivirus-deploye_niveau1</t>
-  </si>
-  <si>
-    <t>Installer de manière systématique un antivirus sur les postes de travail des systèmes industriels, vérifier régulièrement leur bon fonctionnement et leurs mises à jour</t>
-  </si>
-  <si>
-    <t>securite-poste-si-industriel-antivirus-deploye_niveau2</t>
-  </si>
-  <si>
-    <t>Traiter systématiquement les alertes générées par l'antivirus des postes de travail des systèmes industriels</t>
-  </si>
-  <si>
-    <t>securite-poste-pare-feu-local-active_niveau1</t>
-  </si>
-  <si>
-    <t>Activer systématiquement le pare-feu local sur les postes de travail</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Sans connaissance informatique particulière, l’activation d’un pare-feu préinstallé sur le poste de travail et son paramétrage par défaut (qui bloque toute connexion entrante), constituent un premier niveau de protection. Un pare-feu local est une fonction intégrée à la plupart des systèmes d’exploitation grand public. En cas de compromission d’un poste utilisateur, et sans pare-feu, un attaquant pourra plus facilement étendre son attaque vers d’autres équipements du réseau (postes, serveurs, imprimantes, etc.). Tant que l’attaquant n’a pas réussi à obtenir les privilèges administrateurs du poste (qui permettent de modifier la configuration du pare-feu, voire le désactiver), le pare-feu local « bien configuré » sera une barrière efficace pour empêcher l’attaquant d’étendre son emprise sur le réseau. Il est aussi nécessaire de s’assurer régulièrement de leur activation car une désactivation du pare-feu peut être un signe d’une compromission et qu’un logiciel malveillant a pris le contrôle du poste. Ce type d’évènement devrait donc donner lieu à une « levée de doute » de la part des informaticiens (quel est l’origine du changement de configuration ? erreur ? malveillance ? bug ?).
-# Comment ?
+## Comment ?
 L’activation d’un pare-feu préinstallé sur le poste de travail et son paramétrage par défaut (qui bloque toute connexion entrante), constituent un premier niveau de protection. Un pare-feu local (qu’il soit intégré au système d’exploitation ou qu’il soit une solution logicielle tierce), doit ainsi être installé sur tous les postes de travail. Il est recommandé d’assurer l’homogénéité des configurations et de la politique de filtrage des flux.
 Certains pare-feux sont également commercialisés en complément de suites logicielles antivirales.
 Il est également recommandé de vérifier régulièrement leur activation sur tous les postes de travail. Selon les résultats des investigations, il pourra alors être nécessaire d’étendre la levée de doute à l’ensemble des équipements qui ont été contactés par le poste en cause afin d’identifier une extension du périmètre de compromission ou simplement de corriger l’erreur ou le bug.
 Enfin, afin de faciliter les investigations numériques en cas de compromission, il est recommandé de stocker localement les journaux d’évènements du pare-feu local en enregistrant les évènements du type « connexion refusée ».</t>
   </si>
   <si>
-    <t>securite-poste-outils-complementaires-securisation_niveau1</t>
-  </si>
-  <si>
-    <t>Mettre en œuvre une solution de type EDR (Endpoint Detection &amp; Response)</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Pour renforcer davantage la sécurité des postes de travail, il peut être envisagé de mettre en œuvre une solution de type EDR (Endpoint Detection &amp; Response) pour renforcer la sécurité sur les postes de travail et réduire fortement les risques de compromission du SI par rançongiciel via les postes de travail attaques. Cet outil complémentaire à un outil anti-virus permet de détecter des attaques qui n’utilisent que des outils légitimement présents sur un ordinateur (ce qu’un antivirus classique ne peut pas faire).
-# Comment ?
+## Comment ?
 Dans la majorité des cas, ce type de solution peut être mis à disposition par le prestataire informatique ou éditeur qui vous met à disposition sur la solution d’anti-virus. Si non, il est préconisé de s’appuyer sur les compétences d’un prestataire externe, idéalement labellisé Expert Cyber ou référence par un Campus Cyber régional, pour la mise en œuvre de cette recommandation.
 Par ailleurs, l’utilisation d’une telle solution nécessite une supervision et un traitement des alertes remontées par l’outil.</t>
   </si>
   <si>
-    <t>securite-poste-outils-complementaires-securisation_niveau2</t>
-  </si>
-  <si>
-    <t>Traiter systématiquement les alertes générées par l'EDR</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 D’une part, les alertes générées par l'EDR peuvent être le signe d’un mésusage des outils informatiques de la part des utilisateurs. D’autre part, sans action de l’utilisateur, une alerte d'EDR peut être le signe d’une compromission du poste. Par exemple, un attaquant a obtenu un accès initial au poste par un autre moyen (phishing, vulnérabilité) et essaie d’utiliser des outils spécifiques (logiciel malveillant) qui sont détectés par l'EDR. Sans investigation particulière des alertes, l’attaquant pourra faire autant de test que nécessaires avant de réussir à contourner l’antivirus.
-# Comment ?
+## Comment ?
 Il est nécessaire de traiter systématiquement les alertes générées par l'EDR.
 Afin de maintenir un niveau de vigilance élevé de la part des utilisateurs (qui ne doivent pas considérer les alertes de l'EDR comme une chose normale/habituelle), il est recommandé de contacter l’utilisateur du poste sur lequel une alerte a été générée.
 Très régulièrement (à minima 1 fois par semaine), il est conseillé de surveiller et d’analyser la console d’administration de la solution EDR. Cette console permet également de s'assurer que les EDR sont installés sur tous les postes, qu'il est actif et à jour, et ainsi d'identifier les postes pour lesquels ce n'est pas le cas.
 Il est préconisé de s’appuyer sur les compétences d’un prestataire externe, idéalement labellisé Expert Cyber ou référencé par un Campus Cyber, pour la mise en œuvre de cette recommandation.</t>
   </si>
   <si>
-    <t>securite-poste-r-et-d-disques-chiffres_niveau1</t>
-  </si>
-  <si>
-    <t>Chiffrer les disques durs des matériels nomades</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Pour les risques de vols de données et d’espionnage industriel, le chiffrement complet du disque dur des terminaux portables (téléphone, ordinateurs) permet de réduire fortement les risques de vols de données suite à la perte ou vol des terminaux. Les données stockées par un terminal chiffré resteraient inaccessibles à une personne qui l’aurait en sa possession.
-# Comment ?
+## Comment ?
 Il convient au préalable d’identifier les terminaux et postes de travail à risque, au regard des données à protéger en priorité et des habitudes de déplacements des collaborateurs concernés.
 Si vous êtes sur un environnement Microsoft, la solution Bitlocker est gratuite et peut-être activée via le panneau de configuration et les paramètres « Système et Sécurité »
 Si la mise en œuvre de BitLocker n’est pas adaptée au contexte de l’entreprise, une autre solution payant de ce type peut être utilisée. Pour cela il est conseillé de s’appuyer sur les compétences d’un prestataire externe, idéalement labellisé Expert Cyber ou référencé par un Campus Cyber régional.
 Il convient de s’assurer que l’accès aux terminaux chiffrés requiert un mot de passe au démarrage (ou un token USB) et que ce mot de passe soit suffisamment complexe (à minima 12 caractères).</t>
   </si>
   <si>
-    <t>securite-infrastructure-pare-feu-deploye_niveau1</t>
-  </si>
-  <si>
-    <t>Déployer un pare-feu physique pour protéger l’interconnexion du SI à Internet</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Le filtrage des flux et des communications réseaux réalisé par un pare-feu est la première fonction de sécurité à mettre en œuvre afin de limiter le risque de compromission directe du réseau interne à partir d’Internet. Les serveurs rendus accessibles depuis l’Internet à des ordinateurs « non maîtrisés » (ordinateurs quelconques sur l’Internet) sont plus exposés à un risque d’attaque informatique que les ordinateurs accessibles uniquement des autres ordinateurs de l’entité.
 Pour que ce filtrage soit efficace, il ne doit pas être configurer pour laisser passer tous les flux et toutes les communications. Au contraire, il est recommandé que seules les communications nécessaires soient autorisées. Par ailleurs, ce type d’équipement permet aussi la journalisation des flux bloqués par le pare-feu et ainsi d’identifier les tentatives d’intrusion.
-# Comment ?
+## Comment ?
 Déployer un pare-feu physique en mettant en place les mesures de cloisonnements suivants :
 	• Protection de l’interconnexion du SI à Internet en bloquant les flux et ports non strictement nécessaires.
 	• Journalisation des flux bloqués par le pare-feu.
@@ -1973,117 +2525,69 @@
 est préconisé de s’appuyer sur les compétences d’un prestataire externe, idéalement labellisé Expert Cyber, pour la mise en œuvre de cette mesure.</t>
   </si>
   <si>
-    <t>securite-infrastructure-pare-feu-deploye-interconnexions-protegees_niveau1</t>
-  </si>
-  <si>
-    <t>Fermer tous les flux et les ports non strictement nécessaires</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Afin d’augmenter le niveau de cloisonnement entre le réseau interne et l’Internet, le filtrage des flux et des communications réseaux peut être mis en œuvre avec un pare-feu afin de limiter le risque de compromission directe du réseau interne à partir d’Internet. Les serveurs rendus accessibles depuis l’Internet à des ordinateurs « non maîtrisés » (ordinateurs quelconques sur l’Internet) sont plus exposés à un risque d’attaque informatique que les ordinateurs accessibles uniquement des autres ordinateurs de l’entité.
 Pour que ce filtrage soit efficace, il ne doit pas être configurer pour laisser passer tous les flux et toutes les communications. Au contraire, il est recommandé que seules les communications nécessaires soient autorisées.
-# Comment ?
+## Comment ?
 En s’appuyant sur la liste des interconnexions extérieur existantes, il convient d’analyser et de fixer les besoins métiers et techniques de connexion envers internet et autres réseaux partenaires. Sur cette base d’analyse, tous les flux et ports non jugés strictement nécessaires doivent être fermés.
 Il est préconisé de s’appuyer sur les compétences d’un prestataire externe, idéalement labellisé Expert Cyber, pour la mise en œuvre de cette mesure.</t>
   </si>
   <si>
-    <t>securite-infrastructure-pare-feu-deploye-interconnexions-protegees_niveau2</t>
-  </si>
-  <si>
-    <t>Mettre en œuvre autant que possible un tunnel VPN pour tous les flux entrants</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Les points d’accès accessible via Internet représentant la première surface d’attaque éprouvée très régulièrement de manière automatisée par les cyberattaques, il convient donc de les sécuriser davantage. Une solution VPN « full-tunneling » sera une contrainte supplémentaire pour un cyberattaquant et permet de sécuriser davantage les flux d’authentification.
-# Comment ?
+## Comment ?
 En se basant sur les listes exhaustives des accès distants ou dits « télétravaillés », il est recommandé de les rendre accessible seulement au travers d’une solution de VPN « full-tunneling » établissant un tunnel VPN IPsec entre les postes nomades et une passerelle VPN IPsec. Aucun flux distant ne doit pouvoir être transmis en dehors de ce tunnel.
 En complément il est conseillé de mettre en place des mécanismes de double authentification (exemple : code OTP reçu par sms, par mail, via application ou clef sécurisée dédiée, par certificat) avec à minima, avec des restrictions via adresses IP légitimes. Des restrictions complémentaires pourraient par exemple être mises en œuvre sur la localisation des accès entrants (ex : pays), les plages horaires acceptées (exemple : heures ouvrées seulement), procédure ponctuelle d’ouverture et de fermeture de l’accès durant chaque intervention à distance.
 Il est préconisé de s’appuyer sur les compétences d’un prestataire externe, idéalement labellisé Expert Cyber ou référencé, par un campus cyber régional, pour la mise en œuvre de cette mesure.</t>
   </si>
   <si>
-    <t>securite-infrastructure-pare-feu-deploye-logs-stockes_niveau1</t>
-  </si>
-  <si>
-    <t>Activer et conserver l'historique de l’ensemble des flux bloqués et des flux entrants et sortants identifiés par le pare-feu</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 L’installation d’un pare-feu permet de stocker des logs et des journaux pour analyser les flux réseaux passant au travers du pare-feu et ainsi pouvoir détecter d’éventuels tentatives d’intrusion. En cas de compromission avérée, ces logs et journaux peuvent être utiliser à des fins de preuves et d’indices dans le cadre de la remédiation et de l’enquête judiciaire.
-# Comment ?
+## Comment ?
 Par défaut, le pare-feu génère un grand nombre de logs et de journaux, il convient d’analyser la configuration des éléments journalisés (format, fréquence de rotation des fichiers, taille maximale des fichiers journaux, catégories d’évènements enregistrés, etc.), de l’adapter en conséquence et de garder les éléments les plus pertinents en fonction de votre système d’information (ex : recensement des flux et paquets internet entrants et sortants, recensement des flux et des paquets bloqués, authentification réussie et rejeté).
 Ces éléments doivent être journalisés et gardés pendant au moins un an (ou plus en fonction des obligations légales du secteur d’activités).
 Il est préconisé de s’appuyer sur les compétences d’un prestataire externe, idéalement labellisé Expert Cyber ou référencé, par un campus cyber régional, pour la mise en œuvre de cette mesure.</t>
   </si>
   <si>
-    <t>securite-infrastructure-si-industriel-pare-feu-deploye_niveau1</t>
-  </si>
-  <si>
-    <t>Fermer tous les flux et les ports non strictement nécessaires aux systèmes industriels</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Si vos systèmes industriels sont interconnectés à l’environnement bureautique et/ou Internet, le filtrage des flux et des communications réseaux réalisé par un pare-feu est la première fonction de sécurité à mettre en œuvre afin de limiter le risque de compromission directe du réseau industriel à partir d’Internet ou de l’environnement bureautique. Les machines-outils, sondes ou équipements industriels rendus accessibles depuis l’Internet à sont très fortement exposés à un risque d’attaque informatique.
 Pour que ce filtrage soit efficace, il ne doit pas être configurer pour laisser passer tous les flux et toutes les communications. Au contraire, il est recommandé que seules les communications nécessaires soient autorisées. Par ailleurs, ce type d’équipement permet aussi la journalisation des flux bloqués par le pare-feu et ainsi d’identifier les tentatives d’intrusion.
-# Comment ?
+## Comment ?
 En s’appuyant sur la liste des interconnexions extérieur existantes, il convient d’analyser et de fixer les besoins métiers et techniques de connexion du SI industriel (machines-outils, sondes, caméras et autres objets connectés) envers Internet et les autres réseaux partenaires. Sur cette base d’analyse, un pare-feu réseau dédié peut être mis en œuvre afin de fermer tous les flux et ports non jugés strictement nécessaires.
 Il est recommandé de déconnecter tous les accès à Internet des systèmes industriels, si les contraintes métiers et opérationnelles le permettent.
 Il est préconisé de s’appuyer sur les compétences d’un prestataire externe, idéalement labellisé Expert Cyber ou référencé, par un campus cyber régional, pour la mise en œuvre de cette mesure.</t>
   </si>
   <si>
-    <t>securite-infrastructure-si-industriel-pare-feu-deploye_niveau2</t>
-  </si>
-  <si>
-    <t>Dans la mesure du possible et si non nécessaire, séparer le réseau industriel du réseau bureautique interne</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 La mise en œuvre de cette mesure a pour objectif de limiter le risque de latéralisation (étape d’une attaque pendant laquelle un attaquant qui aurait pris le contrôle d’un ordinateur du réseau étend sa prise de contrôle à un sous-ensemble plus grand d’ordinateur du réseau, en allant jusqu’à la totalité des ordinateurs et équipements industriels connectés du réseau) d’une attaque. En effet, en l’absence de restrictions d’interconnexions entre le réseau industriel et l’environnement bureautique (appelé également « réseau interne » ou « réseau administratif »), la compromission d’un de ces 2 réseaux pourrait rapidement engendrer la compromission de l’autre et dans certains cas impacter la chaîne de production.
-# Comment ?
+## Comment ?
 Il convient d’abord d’identifier et d’évaluer avec les métiers les besoins d'échange entre le réseau industriel (machines-outils, sondes, caméras et autres objets connectés) et le réseau bureautique interne.
 Sur la base de cette analyse et selon les usages et les besoins, dans la mesure du possible, il peut être envisager de créer 2 réseaux distincts : 1 réseau « administratif » et 1 réseau « industriel ».</t>
   </si>
   <si>
-    <t>securite-infrastructure-mises-a-jour-fonctionnelles-securite-equipements-securite-deployees_niveau1</t>
-  </si>
-  <si>
-    <t>Déployer systématiquement toutes les mises à jour sur les équipements de sécurité dès que celles-ci sont disponibles</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Au-delà des attaques s’appuyant sur la négligence des utilisateurs et sur l’ingénierie sociale, la majorité des attaquants exploitent des vulnérabilités publiques et documentées pour s’introduire sur les systèmes d’information. Ces vulnérabilités concernent principalement des services exposés sur Internet (par exemple un pare-feu, un équipement VPN, un proxy). Qui plus est, les délais entre la publication d’une vulnérabilité et son exploitation par les attaquants ont tendance à diminuer. Certaines campagnes d’attaques ont industrialisé l’exploitation de vulnérabilités seulement quelques jours après leurs révélations sur Internet.
 En mettant à jour les équipements de sécurité, dans les délais les plus courts possibles, ce risque sera significativement réduit.
-# Comment ?
+## Comment ?
 Il est recommandé d’activer les fonctions de mises à jour automatique proposées par les éditeurs. Certaines mises à jours nécessitent un redémarrage des équipements afin d’être effectives. Il est donc nécessaire de vérifier périodiquement que les équipements ne sont pas en attente de redémarrage et de planifier les redémarrages d’équipements ayant un impact sur la disponibilité des systèmes.
 Certains équipements peuvent être configurés pour notifier les administrateurs d’une mise à jour en attente de redémarrage. Par exemple, le redémarrage d’un pare-feu pour l’application d’une mise à jour peut interrompre l’accès à Internet ou encore les communications entre les différentes zones cloisonnées du réseau. De manière à permettre ces mises à jours au fur et à mesure, dans les meilleurs délais (et qu’elles ne nécessitent pas systématiquement une autorisation hiérarchique), un créneau hebdomadaire ou quotidien peut être consacré à ces courtes interruptions de service de maintenance, et une procédure d’information des utilisateurs instaurée. Sinon, la mise en place de systèmes de tolérance aux pannes (souvent plus coûteux) permet généralement aux équipements de rédémarrer sans interrompre le service.
 Les équipements de sécurité doivent être strictement maintenus à jour : si un équipement de sécurité n’est plus maintenu par l’éditeur, alors il doit être remplacé dans les meilleurs délais.</t>
   </si>
   <si>
-    <t>securite-infrastructure-mises-a-jour-fonctionnelles-securite-systemes-exploitation-securite-deployees_niveau1</t>
-  </si>
-  <si>
-    <t>Déployer systématiquement toutes les mises à jour sur les serveurs, services et logiciels d'administration dès que celles-ci sont disponibles</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Au-delà des attaques s’appuyant sur la négligence des utilisateurs et sur l’ingénierie sociale, la majorité des attaquants exploitent des vulnérabilités publiques et documentées pour s’introduire sur les systèmes d’information. Ces vulnérabilités concernent principalement des services exposés sur Internet (par exemple un pare-feu, un serveur de messagerie, un service d’accès nomade, etc.). Qui plus est, les délais entre la publication d’une vulnérabilité et son exploitation par les attaquants ont tendance à diminuer. Certaines campagnes d’attaques ont industrialisé l’exploitation de vulnérabilités seulement quelques jours après leurs révélations sur Internet.
-# Comment ?
+## Comment ?
 Il est recommandé d'activer les fonctions de mises à jour automatique proposées par les éditeurs. Certaines mises à jours nécessitent un redémarrage des équipements afin d’être effectives. Il est donc nécessaire de vérifier périodiquement que les équipements ne sont pas en attente de redémarrage et de planifier les redémarrages d’équipements ayant un impact sur la disponibilité des systèmes.
 Certains équipements peuvent être configurés pour notifier les administrateurs d’une mise à jour en attente de redémarrage. Par exemple, le redémarrage d’un serveur applicatif pour l’application d’une mise à jour peut interrompre l’accès à cette application. De manière à permettre ces mises à jours au fur et à mesure, dans les meilleurs délais (et qu’elles ne nécessitent pas systématiquement une autorisation hiérarchique), un créneau hebdomadaire ou quotidien peut être consacré à ces courtes interruptions de service de maintenance, et une procédure d’information des utilisateurs instaurée. Sinon, la mise en place de systèmes de tolérance aux pannes permet généralement aux équipements de redémarrer sans que le service soit interrompu.
 Pour certaines mises à jour importantes (systèmes d’exploitation serveurs, base de données, etc.) un délai de qualification interne peut être nécessaire pour s’assurer que la mise à jour n’impacte pas le bon fonctionnement du système. L’état de l’art exigerait d’ailleurs de mettre en place un réseau de “pré-production” permettant que qualifier le bon fonctionnement des systèmes avec les nouvelles versions logicielles avant un déploiement “en production”.
 Des exceptions peuvent être rencontrées (exemple : applications métiers ne fonctionnant qu’avec composant obsolète), mais il convient alors de bien les identifier : à ce niveau de sécurité, l’entité doit être consciente que les systèmes métiers obsolètes représentent un risque de compromission (ou d’extension de compromission) accru.</t>
   </si>
   <si>
-    <t>securite-infrastructure-mises-a-jour-fonctionnelles-securite-systemes-exploitation-securite-deployees_niveau2</t>
-  </si>
-  <si>
-    <t>Mettre en œuvre des mesures de sécurité supplémentaires sur les serveurs, services et logiciels d'administration ne pouvant pas bénéficier des mises à jour</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Au-delà des attaques s’appuyant sur la négligence des utilisateurs et sur l’ingénierie sociale, la majorité des attaquants exploitent des vulnérabilités publiques et documentées pour s’introduire sur les systèmes d’information. Ces vulnérabilités concernent principalement des services exposés sur Internet (par exemple un pare-feu, un équipement VPN, un proxy). Qui plus est, les délais entre la publication d’une vulnérabilité et son exploitation par les attaquants ont tendance à diminuer. Certaines campagnes d’attaques ont industrialisé l’exploitation de vulnérabilités seulement quelques jours après leurs révélations sur Internet.
 En mettant à jour les équipements de sécurité, dans les délais les plus courts possibles, ce risque sera significativement réduit.
 Quand les systèmes ne peuvent pas être mis à jour, il est possible de réduire le risque de compromission de ces systèmes obsolètes par des mesures de sécurité supplémentaires.
-# Comment ?
+## Comment ?
 Des mesures de protection supplémentaires, permettant de limiter le risque d’une compromission des systèmes obsolètes et le risque de latéralisation à partir d’un système obsolète devraient être mis en place.
 Les mesures de protection supplémentaires peuvent être (liste non exhaustive):
 	• cloisonnement réseau dans une zone spécifique isolée de l’environnement bureautique et des services critiques ;
@@ -2096,30 +2600,18 @@
 	• surveillance accrue des journaux d’évènements du système et procédure d’urgence de mise en quarantaine en cas de suspicion de compromission</t>
   </si>
   <si>
-    <t>securite-infrastructure-outils-securisation-systeme-messagerie_niveau1</t>
-  </si>
-  <si>
-    <t>Mettre en œuvre une solution d'anti-spam et d'anti-hameçonnage</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Les systèmes de messagerie sont un des principaux vecteurs d’attaques puisque très largement utilisés et exposés sur internet. Qu’il s’agisse de la compromission d’un poste au travers de l’ouverture de pièces jointes contenant un code malveillant, d’un clic malencontreux sur un lien redirigeant vers un site lui-même malveillant (phishing ou hameçonnage) ou de l’exploitation d’une vulnérabilité et d’un défaut de paramétrage du service de messagerie.
 Des solutions de protection contre l’hameçonnage ou phishing permette de réduire le risque qu’un utilisateur se fasse piéger par un message malveillant. Cependant, les utilisateurs doivent rester vigilants car certains messages pourraient ne pas être détectés par cet outils (et apparaître comme « légitime » bien qu’ils soient malveillants).
-# Comment ?
+## Comment ?
 Il est recommandé de mettre en œuvre d’une solution d'anti-spam et d'anti-hameçonnage permettent de détecter et de bloquer les mails malveillants (malware) ou non sollicités (spam). Certaines solutions traitent également le phishing et le spear phishing parfois grâce à l’intelligence artificielle, d’autres intègrent des fonctionnalités de sensibilisation (simulation d’attaque par phishing, programme de  e-learning).
 Il est préconisé de s’appuyer sur les compétences d’un prestataire externe, idéalement labellisé Expert Cyber ou référencé, par un campus cyber régional, pour la mise en œuvre de cette mesure.</t>
   </si>
   <si>
-    <t>securite-infrastructure-outils-securisation-systeme-messagerie_niveau2</t>
-  </si>
-  <si>
-    <t>Mettre en œuvre des mécanismes complémentaires de protection contre les mails illégitimes</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Les systèmes de messagerie sont un des principaux vecteurs d’attaques puisque très largement utilisés et exposés sur internet, il convient donc de les sécuriser davantage. Une solution VPN "full-tunneling" imposera une difficulté supplémentaire à un cyberattaquant car elle permet de sécuriser davantage les flux d'authentification.
 Par ailleurs, les systèmes de messagerie de type « webmail » sont par définition également exposées sur Internet et donc souvent éprouvés par les cyberattaquants. Des vulnérabilités logiciels peuvent régulièrement apparaître et impactées ces systèmes. Elles nécessitent ainsi un suivi assidu et réactif des mises à jour et des correctifs de sécurité, rendant leur maintenance très contraignante.
-# Comment ?
+## Comment ?
 Pour limiter la nuisance de ces courriels, en amont de leur réception par les utilisateurs, certains protocoles ont pour rôle de vérifier l’authenticité et l’intégrité des courriels. Ils nécessitent une configuration, non seulement par l’entité expéditrice sur les enregistrements DNS de ses noms de domaine, mais aussi par l’entité destinataire sur ses serveurs SMTP de réception. protocoles sont :
 	• Sender Policy Framework (SPF) qui permet de spécifier les adresses IP des serveurs autorisés à émettre les courriels d’un domaine ;
 	• DomainKeys Identified Mail (DKIM) qui permet l’authentification du domaine de messagerie d’un courriel à l’aide d’une signature cryptographique ;
@@ -2127,87 +2619,57 @@
 Par ailleurs, si vous ou votre prestataire héberge votre système de messagerie, vous devez vous assurer : de l’activation du chiffrement TLS des échanges entre serveurs de messagerie (de l’entité ou publics) ainsi qu’entre les postes utilisateurs et les serveurs hébergeant les boîtes de messagerie électronique, en particulier pour les phases d’authentification. Il est également souhaitable de ne pas exposer directement les serveurs de messagerie électronique d’entreprise sur Internet. Dans ce cas, un serveur relais dédié à l’envoi et à la réception des messages doit être mis en place en coupure d’Internet.</t>
   </si>
   <si>
-    <t>securite-infrastructure-acces-wifi-securises_niveau1</t>
-  </si>
-  <si>
-    <t>Mettre en place des mesures de sécurisation wifi</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 L’usage du Wi-Fi en milieu professionnel est aujourd’hui démocratisé mais présente toujours des risques de sécurité bien spécifiques : pas de maîtrise de la zone de couverture pouvant mener à une attaque hors du périmètre géographique de l’entité, configuration par défaut des points d’accès peu sécurisée, mise à disposition d’accès aux visiteurs etc.
-# Comment ?
+## Comment ?
 Plusieurs mesures de sécurisation peuvent être menées via la/les box wifi :
 	• Chiffrement robuste de la connexion wifi, à minima WPA2
 	• Mot de passe de connexion de 20 caractères minimum ;
 	• Si concerné, journalisation des logs de connexion des visiteurs</t>
   </si>
   <si>
-    <t>securite-infrastructure-acces-wifi-securises_niveau2</t>
-  </si>
-  <si>
-    <t>Créer un sous-réseau wifi dédié aux visiteurs</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 L’usage du Wi-Fi en milieu professionnel est aujourd’hui démocratisé mais présente toujours des risques de sécurité bien spécifiques : pas de maîtrise de la zone de couverture pouvant mener à une attaque hors du périmètre géographique de l’entité, configuration par défaut des points d’accès peu sécurisée, mise à disposition d’accès aux visiteurs etc.
-# Comment ?
+## Comment ?
 Il est recommandé de créer un sous-réseau dédié au connexion wifi des visiteurs qui ne doit pas permettre d'accéder au réseau interne mais seulement à Internet et avec SSID différent.
 Il est possible de créer des sous-réseaux et d’en paramétrer leurs différentes restrictions via la console d’administration de la box. Seul un accès cablé/filaire devrait par ailleurs permettre l’accès à la console d’administration.</t>
   </si>
   <si>
-    <t>securite-infrastructure-espace-stockage-serveurs_niveau1</t>
-  </si>
-  <si>
-    <t>Protéger les informations et les systèmes contre des atteintes physiques</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Un accès physique aux locaux hébergeant les équipements (postes de travail, serveurs, équipements réseaux) rend certaines attaques possibles (ou plus faciles). Par exemple:
 	• vol d’informations confidentielles en volant des ordinateurs, des périphériques de stockage de masse (clefs USB, disques durs) ou des documents imprimés (sur les bureaux, dans les poubelles, voire les bennes à ordures de l’entité, dans les imprimantes ou les photocopieuses);
 	• attaques triviales sur la disponibilité (déni de service) : section des câbles réseau ou électriques, incendie, etc.
 	• certaines vulnérabilités (notamment logicielles) peuvent n’être exploitable que localement, en étant directement devant le clavier et l’écran de l’ordinateur, une personne malveillante pourrait utiliser un accès local pour installer un implant logiciel lui permettant ultérieurement d’accéder à distance à l’ordinateur;
 	• installation d’un implant physique visant à donner un accès à distance au réseau de la victime (dispositif connecté physiquement au réseau informatique et accessible, par l’attaquant à distance, via le réseau mobile).
 	• compromission du compte d’administration locale: sauf si des mesures de sécurité spécifiques sont mise en œuvre, un accès physique à un ordinateur permet d’obtenir (ou d’installer un logiciel permettant d’obtenir) les privilèges d’administration de l’ordinateur. Sécuriser l’accès physique aux locaux et accompagner les prestataires lors de leur présence permet de limiter ce type de risques.
-# Comment ?
+## Comment ?
 A minima la ou les salles stockant les infrastructures et équipements informatiques doi(ven)t disposer d'une porte pouvant être fermée à clef, avec si possible une protection contre le duplicata, et idéalement un système de déverrouillage par badge.
 Cette clef ou ces badges doivent être seulement accessibles aux seules personnes légitimes.
 Par ailleurs, il est également conseillé d’accompagner les prestataires durant leurs interventions au sein de la salle.
 Il est également recommandé de mettre en place une politique de protection physique des documents et périphériques de stockages confidentiels. En demandant aux personnels de les stocker sous clé (ne pas les laisser “à la vue”, posés sur un bureau). Une protection contre le vol des ordinateurs traitant les informations confidentielles doit également être mise en place. De plus, il est recommandé de mettre en œuvre un processus de destruction des documents confidentiels avant leur mise au rebus : broyage des documents papier, effacement sécurisé ou destruction des périphériques de stockages.</t>
   </si>
   <si>
-    <t>securite-infrastructure-espace-stockage-serveurs_niveau2</t>
-  </si>
-  <si>
-    <t>Mettre en place un système de vidéoprotection</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Un accès physique aux locaux hébergeant les équipements (postes de travail, serveurs, équipements réseaux) rend certaines attaques possibles (ou plus faciles). Par exemple:
 	• vol d’informations confidentielles en volant des ordinateurs, des périphériques de stockage de masse (clefs USB, disques durs) ou des documents imprimés (sur les bureaux, dans les poubelles, voire les bennes à ordures de l’entité, dans les imprimantes ou les photocopieuses);
 	• attaques triviales sur la disponibilité (déni de service) : section des câbles réseau ou électriques, incendie, etc.
 	• certaines vulnérabilités (notamment logicielles) peuvent n’être exploitable que localement, en étant directement devant le clavier et l’écran de l’ordinateur, une personne malveillante pourrait utiliser un accès local pour installer un implant logiciel lui permettant ultérieurement d’accéder à distance à l’ordinateur;
 	• installation d’un implant physique visant à donner un accès à distance au réseau de la victime (dispositif connecté physiquement au réseau informatique et accessible, par l’attaquant à distance, via le réseau mobile).
 	• compromission du compte d’administration locale: sauf si des mesures de sécurité spécifiques sont mise en œuvre, un accès physique à un ordinateur permet d’obtenir (ou d’installer un logiciel permettant d’obtenir) les privilèges d’administration de l’ordinateur. Mettre en oeuvre un système de vidéoprotection permet de limiter ce type de risques, de potentiellement dissuader les personnes malveillantes et de mieux réagir en cas d’intrusion avérée.
-# Comment ?
+## Comment ?
 Selon le niveau de sécurité souhaité, des mesures complémentaires, peuvent être mises en œuvre telles que (liste à corriger en fonction des mesures déjà en place) :
 	• Vidéoprotection
 	• Traçage des entrées et sorties via un outil informatique dédié en s’appuyant sur un système de badge d’accès. Si jugé nécessaire, solliciter la visite d'un référent sûreté, pour plus d'informations : https://www.gendarmerie.interieur.gouv.fr/conseils/elus/le-referent-surete-un-expert-pour-vous-accompagner</t>
   </si>
   <si>
-    <t>sensibilisation-actions-sensibilisation-menace-et-bonnes-pratiques_niveau1</t>
-  </si>
-  <si>
-    <t>Mettre en œuvre des bonnes pratiques de sensibilisation</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 La sécurité numérique repose nécessairement en partie sur les bonnes pratiques de utilisateurs sur leurs postes et dans l’utilisation au quotidien du numérique. Et moins il n’y a de protections techniques, plus la sécurité repose sur les usages des utilisateurs. Ainsi, il est nécessaire que chaque utilisateur du système d’information (bureautique ou industriel) soit sensibilisé aux risques et formé aux bonnes pratiques à mettre en œuvre à son propre niveau. La cible étant que les utilisateurs sachent notamment :
 	• savoir reconnaître un email d’hameçonnage;
 	• savoir gérer correctement ses mots de passe;
 	• protéger ses terminaux lors d’un déplacement;
 	• être davantage vigilant selon le niveau de criticité et de sensibilité des informations manipulées
 	• plus largement comprendre les mesures de sécurité imposées dans l’entité, les respecter et ne pas essayer de les contourner.
-# Comment ?
+## Comment ?
 Il est préconisé de mener plusieurs actions de sensibilisation pouvant inclure :
 	• Campagnes d'affichage sur les risques et les bonnes pratiques.
 	• Envoi de mails d'information sur les risques et les bonnes pratiques
@@ -2218,20 +2680,14 @@
 Pour que les utilisateurs restent vigilants dans la durée, il est nécessaire de renouveler périodiquement les actions de sensibilisation/formation et sous plusieurs formats répartis dans l’année.</t>
   </si>
   <si>
-    <t>sensibilisation-actions-sensibilisation-menace-et-bonnes-pratiques_niveau2</t>
-  </si>
-  <si>
-    <t>En complément des pratiques déjà en œuvre, mettre en place des actions de sensibilisation additionnelles</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 La sécurité numérique repose nécessairement en partie sur les bonnes pratiques de utilisateurs sur leurs postes et dans l’utilisation au quotidien du numérique. Et moins il n’y a de protections techniques, plus la sécurité repose sur les usages des utilisateurs. Ainsi, il est nécessaire que chaque utilisateur du système d’information (bureautique ou industriel) soit sensibilisé aux risques et formé aux bonnes pratiques à mettre en œuvre à son propre niveau. La cible étant que les utilisateurs sachent notamment :
 	• savoir reconnaître un email d’hameçonnage ;
 	• savoir gérer correctement ses mots de passe ;
 	• protéger ses terminaux lors d’un déplacement ;
 	• être davantage vigilant selon le niveau de criticité et de sensibilité des informations manipulées
 	• plus largement comprendre les mesures de sécurité imposées dans l’entité, les respecter et ne pas essayer de les contourner.
-# Comment ?
+## Comment ?
 Il est préconisé de mener des actions de sensibilisation additionnelles pouvant inclure (liste à corriger en fonction des actions déjà réalisées) :
 	• Sensibilisation des nouveaux arrivants
 	• Intervention auprès du CODIR
@@ -2239,29 +2695,17 @@
 	• Campagne de faux phishing qui consiste à « tester » la capacité des utilisateurs à détecter un mail piégé</t>
   </si>
   <si>
-    <t>sensibilisation-risque-espionnage-industriel-r-et-d_niveau1</t>
-  </si>
-  <si>
-    <t>Mener des actions de sensibilisation ciblée auprès du personnel effectuant des déplacements</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 L’emploi de téléphones connectés (ou ordiphones/smartphones), d’ordinateurs portables et de tablettes facilite et accélère le transport et l’échange de données. Parmi les informations stockées sur ces supports, certaines peuvent présenter une sensibilité importante pour l’entité. Leur perte, leur saisie ou leur vol peut avoir des conséquences majeures sur nos activités et sur leur pérennité. Il nous faut donc, dans ce contexte de nomadisme, les protéger face aux risques et aux menaces qui pèsent sur elles, tout particulièrement lors de nos déplacements à l’étranger.
-# Comment ?
+## Comment ?
 Il est préconisé d’identifier les personnels amenés à se déplacer les plus souvent, et plus particulièrement à l’étranger, et de les sensibiliser aux risques particuliers relatifs aux déplacements professionnels et sensibilisation ciblée auprès des agents effectuant des missions à l'étranger.
 Le [passeport de conseils aux voyages de l’ANSSI](https://www.ssi.gouv.fr/uploads/IMG/pdf/passeport_voyageurs_anssi.pdf) peut être un premier élément de communication à leur transmettre, voire à lire avec eux.
 Une session de sensibilisation dédiée peut également être une bonne pratique.</t>
   </si>
   <si>
-    <t>sensibilisation-collaborateurs-soumis-obligations-usages-securises_niveau1</t>
-  </si>
-  <si>
-    <t>Établir une charte informatique</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 La mise en place d’une charte informatique permet de responsabiliser davantage les utilisateurs envers le risque cyber et permet de garantir la connaissance des bonnes pratiques exigées par l’entité et responsabiliser l’utilisateur face à ses propres usages des outils numériques. Elle participe à la sensibilisation/formation des utilisateurs.
-# Comment ?
+## Comment ?
 La charte doit tout à minima contenir les éléments suivants :
 	• répertorier les moyens informatiques mis à disposition
 	• clarifier la gestion des terminaux personnels au sein de l’entité (interdit et/ou accepté selon des modalités bien précisées)
@@ -2271,42 +2715,24 @@
 	• préciser les responsabilités et les sanctions encourues en cas de non-respect de la charte</t>
   </si>
   <si>
-    <t>sensibilisation-collaborateurs-soumis-obligations-usages-securises_niveau2</t>
-  </si>
-  <si>
-    <t>S'assurer que la charte informatique est annexée au contrat de travail et est signée par les salariés</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 La mise en annexe au contrat de travail de la charte informatique permet de la rendre opposable aux salariés, et en dernier recourt de sanctionner un salarié qui ne la respecterait pas.
-# Comment ?
+## Comment ?
 Après validation des représentants du personnel (si nécessaire), il est conseillé d’annexer la charte au contrat de travail. La signature de la signature peut ainsi être réalisé à l’arrivée du collaborateur ou à la suite d’une séance collective de lecture de la charte et/ou session de sensibilisation aux bonnes pratiques.
 Il est préconisé de définir ce process avec les équipes RH.</t>
   </si>
   <si>
-    <t>reaction-surveillance-veille-vulnerabilites-potentielles_niveau1</t>
-  </si>
-  <si>
-    <t>S’abonner aux alertes de sécurité publiées par le centre gouvernemental de veille, d'alerte et de réponses aux cyberattaques</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Il arrive que des vulnérabilités logicielles soient publiées sans que les mises à jour de sécurité correspondantes aient été mises à disposition par les éditeurs. Un suivi régulier des vulnérabilités de sécurité permet de prendre connaissance des dernières failles critiques exploitables par les cyberattaquants afin de les corriger par anticipation. En effet, des outils malveillants exploitant ces vulnérabilités peuvent alors se diffuser rapidement sur Internet. Dans un tel cas, selon la nature de la vulnérabilité et l’impact que pourrait avoir son exploitation dans le/les réseau(x) de l’entité, la mise en œuvre de mesure de protection spécifique permettant d’en empêcher l’exploitation ou d’en détecter les tentative d’exploitation permettent d’améliorer transitoirement (le temps que les éditeurs publient une mise à jour) la sécurité des systèmes.
-# Comment ?
+## Comment ?
 Une personne de l’entité ou un de ses prestataires doit surveiller quotidiennement la publication, par le CERT-FR, des alertes de sécurité. Ces alertes de sécurité sont publiées gratuitement sur le site du CERT-FR : https://www.cert.ssi.gouv.fr/alerte/ et via le flux RSS https://www.cert.ssi.gouv.fr/alerte/feed/ .
 Sur demande à cert-fr@ssi.gouv.fr, il est aussi possible de recevoir ces alertes par messagerie électronique. Si une alerte concernant un produit utilisé dans l’entité est publiée, il faut alors mettre en œuvre les recommandations détaillées dans l’alerte.
 Ces recommandation peuvent notamment concerner la mise en œuvre de mesures d’atténuation du risque ou de détection de compromission.</t>
   </si>
   <si>
-    <t>reaction-surveillance-veille-vulnerabilites-potentielles_niveau2</t>
-  </si>
-  <si>
-    <t>Réaliser une veille proactive des vulnérabilités informatiques</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Il arrive que des vulnérabilités logicielles soient publiées sans que les mises à jour de sécurité correspondantes aient été mises à disposition par les éditeurs. Un suivi régulier des vulnérabilités de sécurité permet de prendre connaissance des dernières failles critiques exploitables par les cyberattaquants afin de les corriger par anticipation. En effet, des outils malveillants exploitant ces vulnérabilités peuvent alors se diffuser rapidement sur Internet. Dans un tel cas, selon la nature de la vulnérabilité et l’impact que pourrait avoir son exploitation dans le/les réseau(x) de l’entité, la mise en œuvre de mesure de protection spécifique permettant d’en empêcher l’exploitation ou d’en détecter les tentative d’exploitation permettent d’améliorer transitoirement (le temps que les éditeurs publient une mise à jour) la sécurité des systèmes.
-# Comment ?
+## Comment ?
 Dans un premier temps, une personne de l’entité doit surveiller quotidiennement la publication, par le CERT-FR, des avis et alertes de sécurité. Ces informations sont publiées sur le site du CERT-FR : https://www.cert.ssi.gouv.fr/ et via les flux RSS https://www.cert.ssi.gouv.fr/alerte/feed/ et https://www.cert.ssi.gouv.fr/avis/feed/ .
 Sur demande à cert-fr@ssi.gouv.fr, il est aussi possible de recevoir ces informations par messagerie électronique.
 Si un avis de sécurité ou une alerte concernant un produit utilisé dans l’entité est publié(e), il faut alors mettre en œuvre les recommandations détaillées dans l’avis. Ces recommandations peuvent notamment concerner la mise en œuvre de mesures d’atténuation du risque ou de détection de compromission.
@@ -2314,29 +2740,17 @@
 Pour aller plus loin, l’entité peut, à la place de surveiller les avis du CERT-FR, suivre directement les avis de sécurité publiés par chacun des éditeurs des systèmes et applications utilisés. Dans ce cas, la surveillance quotidienne des alertes du CERT-FR doit être maintenue. Il est préconisé de s’appuyer sur les compétences d’un prestataire externe, idéalement labellisé Expert Cyber ou référencé, par un campus cyber régional, pour la mise en œuvre de cette mesure.</t>
   </si>
   <si>
-    <t>reaction-sauvegardes-donnees-realisees_niveau1</t>
-  </si>
-  <si>
-    <t>Réaliser des sauvegardes régulièrement</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 En cas de compromission du système d’information, les dispositifs de sauvegarde permettent une restauration plus rapide des activités opérationnelles, notamment en cas d’attaque par rançongiciel.
-# Comment ?
+## Comment ?
 Tout d’abord, il convient de définir, avec les décideurs au travers d’une réunion dédiée, le rythme de sauvegarde à mettre en place selon le type et la criticité des données.
 Puis, il est nécessaire d’identifier les supports et les moyens utilisés pour réaliser les sauvegardes (exemple : serveur de sauvegarde dédié en ligne, serveur de sauvegarde dédiée hors ligne, cartouches, disques externes, cloud privé d’un fournisseur, etc.). Il est fortement recommandé d’appliquer la règle simple « 3-2-1 » : 3 copies de sauvegarde différentes, sur 2 supports différents dont 1 hors ligne.
 Il est préconisé de s’appuyer sur les compétences d’un prestataire externe, idéalement labellisé Expert Cyber ou référencé, par un campus cyber régional, pour la mise en œuvre de cette mesure.</t>
   </si>
   <si>
-    <t>reaction-sauvegardes-donnees-realisees-oui-ponctuellement-tiroir-environnement-isole_niveau1</t>
-  </si>
-  <si>
-    <t>Disposer d'une copie de sauvegarde des données critiques “hors ligne”, isolé de l'environnement bureautique</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 En cas de compromission du système d’information, les dispositifs de sauvegarde permettent une restauration plus rapide des activités opérationnelles, notamment en cas d’attaque par rançongiciel. Un jeu de sauvegarde totalement déconnecté restera alors préservé malgré une attaque de ce type. Le système de sauvegarde principal étant la majorité des cas connecté au réseau, un cyberattaquant sera susceptible de parvenir à y accéder et à le compromettre également.
-# Comment ?
+## Comment ?
 Il est donc nécessaire de compléter le dispositif de sauvegarde existant par des sauvegardes dites « hors ligne » et déconnectées, qui ne seront pas accessibles par un attaquant en cas de compromission totale de l’environnement bureautique et des postes d’administration (non accessible via l’outil de gestion centralisé des politiques de sécurité et l’annuaire centralisé ou via internet directement hors cloud privé).
 Il peut s'agir d'un support physique comme un disque dur externe, à déconnecter impérativement du système d'information à l'issue de la sauvegarde. Ce type de support réduit le risque d'une compromission des données qu’il contient mais n'est pas à l'abri d'un vol, d'une destruction ou d'un dysfonctionnement.
 Certains services de sauvegarde spécialisés via un cloud privé peuvent aussi apporter les garanties de déconnexion recherchées. Mais ceux-ci doivent être explicitement souscrits auprès du fournisseur de service cloud et leur efficacité de cloisonnement doit être vérifiée. Le rythme de cette sauvegarde « hors ligne » doit idéalement être défini avec les décideurs.
@@ -2344,34 +2758,16 @@
 Il est préconisé de s’appuyer sur les compétences d’un prestataire externe, idéalement labellisé Expert Cyber ou référencé, par un campus cyber régional, pour la mise en œuvre de cette mesure.</t>
   </si>
   <si>
-    <t>reaction-sauvegardes-donnees-realisees-oui-ponctuellement-tiroir-sauvegarde-testee-regulierement_niveau1</t>
-  </si>
-  <si>
-    <t>Procéder à des tests de restauration des sauvegardes</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Il s’avère que des bugs et autres aléas informatiques arrivent souvent lors d’opérations de sauvegardes. Il convient donc de s’assurer que le jeu de sauvegarde hors-ligne est bien fonctionnel pour garantir qu’elles seront exploitables le moment venu (et particulièrement après un incident de sécurité majeur de type attaque par rançongiciel).
-# Comment ?
+## Comment ?
 Quel que soit le support utilisé pour le jeu de sauvegarde « hors-ligne, des tests réguliers de restauration doivent être menés, à minima une fois par semestre. En vérifiant, qu’après la restauration que l’intégrité des données à protéger en priorité est bien conforme.
 Il est préconisé de s’appuyer sur les compétences d’un prestataire externe, idéalement labellisé Expert Cyber ou référencé, par un campus cyber régional, pour la mise en œuvre de cette mesure.</t>
   </si>
   <si>
-    <t>reaction-sauvegardes-donnees-realisees-oui-automatique-et-reguliere-tiroir-environnement-isole_niveau1</t>
-  </si>
-  <si>
-    <t>reaction-sauvegardes-donnees-realisees-oui-automatique-et-reguliere-tiroir-sauvegarde-testee-regulierement_niveau1</t>
-  </si>
-  <si>
-    <t>reaction-dispositif-gestion-crise-adapte-defini_niveau1</t>
-  </si>
-  <si>
-    <t>Lister les personnes à contacter en cas de cyberattaque</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Une cyberattaque peut être à l’origine d’une véritable crise d’ordre générale au sein d’une entité, on parle alors de crise d’origine cyber. Les victimes d’une cyberattaque se retrouvent souvent déstabilisées, sidérées et en panique ne savant plus vers qui se retourner, qui contacter pour être accompagné et avoir les bons réflexes pour bien réagir, de manière rapide et limiter les impacts sur l’entité.
-# Comment ?
+## Comment ?
 Il est recommandé d’identifier en amont d’une crise la liste des contacts pouvant inclure par exemple :
 	• L'équipe ou le prestataire informatique de l'organisation
 	• Le contact local cyber de la police ou la gendarmerie, à minima noter le 17
@@ -2382,409 +2778,13 @@
 Il est ensuite conseillé de formaliser et imprimer plusieurs versions papiers de cette liste.</t>
   </si>
   <si>
-    <t>reaction-dispositif-gestion-crise-adapte-defini_niveau2</t>
-  </si>
-  <si>
-    <t>Définir un dispositif de gestion de crise d'origine cyber</t>
-  </si>
-  <si>
-    <t># Pourquoi ?
+    <t>## Pourquoi ?
 Une organisation est davantage jugée résiliente si, en cas de crise cyber, elle est capable de maintenir ses activités les plus critiques (éventuellement en mode dégradé, voire sans services et outils numériques disponibles).
 Pour cela, il est important qu’elle ait anticipé et mis en place des mesures adaptés aux scénarios de crise cyber, qui seront activés pour maintenir ou rétablir ses activités critiques.
-# Comment ?
+## Comment ?
 Il est recommandé de définir lors d’une réunion dédiée avec les décideurs de l’entité et l’informatique : les priorités métier à rétablir en cas   de crise, des fiches réflexes opérationnelles garantissant la continuité d'activité au travers de modes dégradés défini avec les métiers et des moyens et des modalités de communication de crise qui seront utilisables en cas d’indisponibilité des systèmes de messagerie et de téléphonie habituels.
 Il est aussi recommandé d’exercice de crise d’origine cyber pour éprouver le dispositif de gestion de crise et s’assurer que les fiches réflexes et les modes dégradés sont bien adaptés
 Il est ensuite conseillé de formaliser et imprimer plusieurs versions papiers des fiches réflexes et procédures de modes dégradés.</t>
-  </si>
-  <si>
-    <t>urn_prefix</t>
-  </si>
-  <si>
-    <t>prefix_id</t>
-  </si>
-  <si>
-    <t>prefix_value</t>
-  </si>
-  <si>
-    <t>color</t>
-  </si>
-  <si>
-    <t>#555555
-#8B0000
-#209226</t>
-  </si>
-  <si>
-    <t>#555555
-#8B0000
-/
-/</t>
-  </si>
-  <si>
-    <t>#555555
-#8B0000
-/
-/
-/</t>
-  </si>
-  <si>
-    <t>#000000
-#555555
-#8B0000
-/
-/</t>
-  </si>
-  <si>
-    <t>#555555
-#8B0000
-#209226
-#209226</t>
-  </si>
-  <si>
-    <t>#000000
-#555555
-/
-#209226
-#209226</t>
-  </si>
-  <si>
-    <t>#000000
-#555555
-#8B0000
-#209226</t>
-  </si>
-  <si>
-    <t>#555555
-#209226
-/
-/</t>
-  </si>
-  <si>
-    <t>#555555
-#8B0000
-/</t>
-  </si>
-  <si>
-    <t>#555555
-/
-/
-/</t>
-  </si>
-  <si>
-    <t>#000000
-#555555
-#8B0000
-#209226
-#209226</t>
-  </si>
-  <si>
-    <t>#000000
-#555555
-#8B0000
-/</t>
-  </si>
-  <si>
-    <t>Question 33.1 dépendante de la Question 33</t>
-  </si>
-  <si>
-    <t>Question 33.2 dépendante de la Question 33</t>
-  </si>
-  <si>
-    <t>Question 44.1 dépendante de la Question 44</t>
-  </si>
-  <si>
-    <t>Question 44.2 dépendante de la Question 44</t>
-  </si>
-  <si>
-    <t>Question 44.3 dépendante de la Question 44</t>
-  </si>
-  <si>
-    <t>Question 44.4 dépendante de la Question 44</t>
-  </si>
-  <si>
-    <t>Question 8.1 dépendante de la Question 8</t>
-  </si>
-  <si>
-    <t>Question 8.2 dépendante de la Question 8</t>
-  </si>
-  <si>
-    <t>Questions dépendantes de la Question 7</t>
-  </si>
-  <si>
-    <t>Questions dépendantes de la Question 6</t>
-  </si>
-  <si>
-    <t>Questions dépendantes de la Question 5</t>
-  </si>
-  <si>
-    <t>Questions dépendantes de la Question</t>
-  </si>
-  <si>
-    <t>MonAideCyber aide les entités publiques et privées sensibilisées à la sécurité informatique à passer à l’action. Le dispositif MonAideCyber est développé par l'Agence Nationale de la Sécurité des Systèmes d'Information, en lien avec BetaGouv et la Direction interministérielle du numérique.
- Sources :
-	• https://github.com/betagouv/mon-aide-cyber 
-	• https://monaide.cyber.gouv.fr/diagnostic-libre-acces</t>
-  </si>
-  <si>
-    <t>node_id</t>
-  </si>
-  <si>
-    <t>## Entités publiques
-Les entités publiques sont invitées à s'orienter vers le service ANSSI https://club.ssi.gouv.fr/ pour bénéficier d'outils gratuits d’audits automatisés.</t>
-  </si>
-  <si>
-    <t>## Des dispositifs adaptés
-Selon le secteur d’activité et la région sélectionnés, l’entité se verra proposer des dispositifs adhoc.</t>
-  </si>
-  <si>
-    <t>## Moins de 9 postes
-Si l’entité dispose de moins de 9 postes, le questionnaire MonAideCyber se verra légèrement simplifié. Ainsi, les questions 12, 33 et 34 seront facultatives.</t>
-  </si>
-  <si>
-    <t>## Attaque ciblée
-Si oui, des questions additionnelles liées à la maîtrise des accès utilisateurs et à la sécurisation des données jugées sensibles seront abordées.
-Exemples d’informations et de données pouvant être faire l’objet d’une attaque ciblée : secrets industriels, données de R&amp;D, brevets d'invention, données innovantes jugées vitales pour l’activité de l’entité, données clientes confidentielles.</t>
-  </si>
-  <si>
-    <t>## Systèmes industriels
-Si oui, des questions dédiées à la sécurité des systèmes industriels seront abordées.
-Exemples de systèmes industriels : objet ou machine industrielle connectée, automates programmables, systèmes numériques de contrôle-commande, systèmes instrumentés de sécurité, capteurs et actionneurs,  bus de terrain, logiciels de supervision et de contrôle SCADA, logiciels de gestion de production assistée par ordinateur (GPAO, GMAO, MES), logiciels d’ingénierie et de maintenance, systèmes embarqués, Gestion Technique Centralisée (GTC), Gestion Technique du Bâtiment (GTB), équipements biomédicaux, etc.</t>
-  </si>
-  <si>
-    <t>## Statistiques anonymes
-Attention, bien préciser à l’entité que cette question est utile à des fins de statistiques anonymisées. Aucune action ne sera menée si jamais elle n’a pas déposé plainte suite à une cyberattaque.</t>
-  </si>
-  <si>
-    <t>## À protéger en priorité 
-Peuvent être jugées prioritaires :
-	• les activités critiques, indispensables à l’activité,
-	• les informations sensibles, confidentielles et/ou ne devant pas être volées et exfiltrées
-Exemples d’activités et de données à protéger en priorité, classées par ordre de priorité :
-	• Production et données techniques de production
-	• R&amp;D et données d’industrialisation
-	• Paie des salariés et données bancaires associées
-	• Facturation et données clients
-	• Courriels, agenda et données bureautiques associées</t>
-  </si>
-  <si>
-    <t>## Interconnexions extérieures
-IP publiques, accès distants ouverts aux prestataires et partenaires, etc.
-## Entités publiques
-Les entités publiques sont éligibles au service gratuit SILENE de l’ANSSI qui permet d’identifier la surface d’attaque des services exposés sur Internet.&lt;br /&gt; Pour y accéder, l’entité est invitée à s'orienter vers le service ANSSI https://club.ssi.gouv.fr/.</t>
-  </si>
-  <si>
-    <t>## **SYSTÈME INDUSTRIEL**
-## Composants
-Équipements réseaux (routeur, switch/commutateur, borne-wifi, pare-feu et autres équipements de sécurité), les serveurs (en précisant leurs fonctionnalités), les infrastructures de sauvegarde, les postes de travail utilisateurs et les supports mobiles interconnectés au réseau.</t>
-  </si>
-  <si>
-    <t>## CNIL
-Attention à ne pas tomber dans un contrôle de conformité au RGPD, ces informations ne seront pas partagées à la CNIL. Si nécessaire, rappeler de manière pédagogique que le Règlement Général sur Protection des Données est une obligation réglementaire qui s’applique à toute entité, publique et privée, qui gère et stocke des données personnelles.
-## Données personnelles 
-Exemples de données personnelles :
-	• Données liées au personnel,
-	• Données des clients ou des usagers,
-	• Données des fournisseurs ou partenaires.</t>
-  </si>
-  <si>
-    <t>## Utilisation des données personnelles
-Il existe une page d’information dédiée à l'utilisation des données personnelles et la gestion des droits d’informations et les moyens de les exercer sur le site de la CNIL : https://www.cnil.fr/fr/respecter-les-droits-des-personnes</t>
-  </si>
-  <si>
-    <t>## Contrats des prestataires
-Cette question suppose que l’entité ait des contrats avec ses prestataires et sait lesquels ont accès à son système d’information, sinon, nous vous invitons à cocher “Non, aucune exigence ne figure dans nos contrats de prestation.”
-Exemples d’exigences pouvant être intégrées dans un contrat : changement des mots de passe par défaut ; sécurisation des accès distants ; délai de déploiement des mises à jour critiques ; signalement en cas de cyberattaque ; contractualisation d'un plan d'assurance sécurité (PAS).
-## Systèmes industriels
-Si l’entité est concernée, cette question s’applique également pour les prestataires disposant d’accès informatiques sur les systèmes industriels</t>
-  </si>
-  <si>
-    <t>## Entités publiques
-Les entités publiques sont éligibles au service gratuit ADS de l’ANSSI qui permet d’analyser le niveau de sécurité de l’annuaire centralisé. Pour y accéder, l’entité est invitée à s’orienter vers le service ANSSI https://club.ssi.gouv.fr/
-## Active Directory, Samba-AD
-À partir d’un parc informatique d’une dizaine de postes, il est fortement recommandé de s’appuyer sur une solution de type Active Directory ou Samba-AD, et de ne plus s’appuyer sur un réseau en “Workgroup” afin d’homogénéiser le niveau de sécurité des postes de travail.</t>
-  </si>
-  <si>
-    <t>## **ATTAQUE CIBLÉE**
-## Accès et comptes prioritaires
-Les accès et comptes utilisateurs à maitriser en priorité sont ceux permettant d’ouvrir une session sur le poste de travail et ceux permettant d’accéder aux données jugées les plus sensibles. Selon les cas, ces accès et comptes sont gérés via un Active Directory et/ou un service Cloud et/ou applicatif(s) métier(s).</t>
-  </si>
-  <si>
-    <t>## Administration locale des postes
-Cette question traite du privilège d'administration local des comptes utilisateurs sur leur poste de travail, il permet par exemple aux utilisateurs d'être autonome dans l'installation d'applications et la configuration de leur machine.
-Si le personnel est autorisé à utiliser son matériel personnel (BYOD) pour travailler et accéder aux systèmes d’information de l’entité, nous vous invitons à cocher “Oui”.</t>
-  </si>
-  <si>
-    <t>## Mots de passe 
-Exigences minimales acceptables :
-	• Longueur de mots de passe à minima de 12 caractères si compte non administrateur local
-	• Longueur de mots de passe à minima de 16 caractères si compte administrateur local
-	• Construction complexe avec par ex l’utilisation de minuscules, majuscules, chiffres et caractères spéciaux
-	• 1 renouvellement annuel des mots de passe, et lors d'une suspicion d'une cyberattaque</t>
-  </si>
-  <si>
-    <t>## Comptes d’administration
-NB : cette question traite des comptes d'administration systèmes sur les serveurs, infrastructures etc. L'administration locale des postes de travail est traitée dans la question sur les utilisateurs administrateurs de leurs postes</t>
-  </si>
-  <si>
-    <t>## Comptes d’administration
-NB : cette question traite des comptes d'administration systèmes sur les serveurs, infrastructures etc. L'administration locale des postes de travail est traitée dans la question sur les utilisateurs administrateurs de leurs postes. 
-Exemple de restrictions :
-	• Tous les administrateurs utilisent en parallèle un compte utilisateur sans privilèges pour les usages du quotidien (ex : surf sur internet, messagerie, etc.)
-	• 1 seul compte administrateur du domaine
-	• Le compte administrateur du domaine n’est utilisé qu’exceptionnellement
-	• Le compte d’administration de la solution de sauvegarde différent n’est pas géré via l’annuaire centralisé (ex : Active Directory, Samba-AD)</t>
-  </si>
-  <si>
-    <t>## **ATTAQUE CIBLÉE**
-## Données sensibles
-Nous vous invitons à vous focaliser sur les ressources et données qui étaient jugées prioritaires lors de la question sur les informations et activités à protéger. 
-Exemples de mesures acceptables :
-	• Contraintes renforcées de robustesse et de longueur de mots de passe (16 caractères minimum)
-	• Authentification multifacteur
-	• Protection des données dans un conteneur chiffré “à froid” et lors d’un transfert via Internet (ex : mail)
-	• Utilisation d'une solution de Data Loss Prevention permettant de limiter les fuites de données</t>
-  </si>
-  <si>
-    <t>## Authentification multifacteur 
-Exemples de facteur d’authentification :
-	• l’usage d’une carte à puce et d’un code PIN d’authentification ;
-	• l’usage d’un token physique et d’un code PIN d’authentification ;
-	• l’utilisation d’une application dédiée sur un smartphone idéalement professionnel (ex : Windows Authentificator, Twilio Authy, etc.), ou à défaut un code envoyé par sms idéalement sur un téléphone professionnel</t>
-  </si>
-  <si>
-    <t>## **SYSTÈME INDUSTRIEL**</t>
-  </si>
-  <si>
-    <t>## Authentification renforcée
-Pour répondre aux exigences de la réponse “Oui, des mesures renforçant l’authentification ont été mises en œuvre”, l’entité doit appliquer au moins les premières mesures suivantes :
-	• Modification des mots de passe par défaut
-	• Contraintes renforcées de robustesse et de longueur de mots de passe (16 caractères minimum)
-	• Stockage des mots de passes d’administration des services critiques (ex : annuaire centralisé, sauvegarde, messagerie) en dehors du système d’information (ex : feuille papier dans un meuble fermé à clef, coffre-fort, etc)</t>
-  </si>
-  <si>
-    <t>## Mises à jour installées
-Pour cocher la réponse “Toutes les mises à jour sont déployées […]”, l’entité doit s’assurer que les mises à jour sont bien installées.
-## Mesures complémentaires 
-Mesures complémentaires pouvant être menées pour sécuriser les postes de travail obsolètes :
-	• les isoler et les cloisonner du reste du réseau bureautique (ex : déconnecter de l’annuaire centralisée), une compromission de ces derniers aura ainsi un faible impact
-	• mettre en œuvre un outil de protection de type EDR en complément de l’antivirus intégrant des règles de sécurité spécifiques aux postes obsolètes.
-## Déploiement des logiciels et contrôle des mises à jour 
-Afin de s’assurer que les mises à jours sont déployées, il peut être nécessaire de :
-	• faire une vérification manuelle sur chaque poste et pour chaque logiciel (à l’aide d’un script/programme exécuté sur chaque poste)
-	• déployer un agent logiciel réalisant la vérification (outil de gestion des vulnérabilités)
-	• utiliser un outil de gestion centralisé des logiciels : un tel outil permet de connaître l’état de déploiement des logiciels (et notamment leur version) de chaque poste de manière centralisée</t>
-  </si>
-  <si>
-    <t>## Mises à jour installées
-Pour cocher la réponse “Oui et ses alertes sont systématiquement traitées […]”, l’entité doit s’assurer que les mises à jour sont bien installées.
-## Windows Defender
-Windows Defender est l’antivirus intégré gratuitement dans tous les systèmes d’exploitation Windows récents.</t>
-  </si>
-  <si>
-    <t>## Pare-feu local
-Le pare-feu local est un logiciel qui permet de filtrer le trafic entrant et sortant dans le système d’exploitation du poste de travail. Un pare-feu local est une fonction intégrée à la plupart des systèmes d’exploitation grand public. Par défaut, ce logiciel est désactivé ou d’un niveau de paramétrage insuffisant. Un niveau suffisant serait de restreindre les communications réseaux directes entre les postes de travail et de bloquer toute connexion entrante. Des pare-feux sont également commercialisés en complément de suites logicielles antivirales.</t>
-  </si>
-  <si>
-    <t>## EDR
-Un EDR, Endpoint Detection Response, détecte et bloque les menaces sur les terminaux en s’appuyant sur l’analyse comportementale et la corrélation d'événements.</t>
-  </si>
-  <si>
-    <t>## **ATTAQUE CIBLÉE**
-## Windows Bitlocker
-Windows Bitlocker est un outil de chiffrement intégré gratuitement dans tous les systèmes d’exploitation Windows récents.
-NB : il est indispensable que le déchiffrement au démarrage du poste soit soumis à un mot de passe robuste (ou un token USB).
-## Matériels nomades 
-Il s’agit des équipements et matériels numériques transportés durant les déplacements, exemples :
-	• ordinateur portable
-	• tablette
-	• téléphone
-	• clefs USB et disques durs</t>
-  </si>
-  <si>
-    <t>## Pare-feu
-Le pare-feu est l’outil permettant de restreindre les services exposés sur Internet, et réalisant le filtrage des communications et des flux réseaux. Afin de réduire au maximum la surface d’attaque disponible pour les attaquants, il est recommandé de réduire au maximum les services et les flux accessibles depuis Internet.
-Par exemple, il est fortement déconseillé d’autoriser l’accès à distance vers des objets connectés (ex : caméra, imprimante, sondes etc.)
-NB : une box Internet n’est pas à considérer comme un pare-feu physique puisqu’elle ne permet pas de filtrer efficacement les flux sortants.</t>
-  </si>
-  <si>
-    <t>## **SYSTÈME INDUSTRIEL**
-## Cloisonnement des systèmes industriels
-Le plus sécurisé est un cloisonnement strict (pas d’interconnexion). De manière plus fonctionnelle, les flux réseaux entre les réseaux bureautique et industriel sont filtrés strictement (pour ne laisser passer que les flux des applications strictement nécessaires). Il est par ailleurs fortement conseillé de bloquer l’accès à distance vers des objets connectés (ex : caméra, équipements industriels, sondes etc.) sans restriction particulière (adresse IP source) ou sans passer par un VPN.</t>
-  </si>
-  <si>
-    <t>## Équipements de sécurité 
-Exemples d’équipements de sécurité à mettre à jour dès que possible :
-	• Pare-feu réseau, pare-feu applicatif (WAF)
-	• Équipement VPN
-	• Proxy</t>
-  </si>
-  <si>
-    <t>## Serveurs et services d’administration 
-Exemples des serveurs et des services d’administration à mettre à jour dès que possible :
-	• Serveurs d’infrastructures : Windows Server, Active Directory, serveur gestionnaire de mises à jour WSUS, serveur de messagerie (exchange, zimbra, etc.), solution de virtualisation, outil de supervision et de télémaintenance, solution de sauvegarde
-	• Serveurs métiers : base de données, serveur web (Apache, IIS, etc.), serveur d’application, outil de développement et autres applicatifs etc.
-## Mesures complémentaires 
-Mesures complémentaires pouvant être menées pour sécuriser les serveurs obsolètes :
-	• les isoler et les cloisonner du reste du réseau bureautique (ex : déconnecter de l’annuaire centralisée)
-	• ne pas les interconnecter à Internet
-	• mettre en œuvre un outil de protection de type EDR intégrant des règles de sécurité spécifiques aux serveurs obsolètes.</t>
-  </si>
-  <si>
-    <t>## Mécanismes de protection 
-Les mécanismes de protection de mails illégitimes à paramétrer sur le serveur DNS sont :
-	• Sender Policy Framework (SPF) qui permet de spécifier les adresses IP des serveurs autorisés à émettre les mails d’un domaine ;
-	• DomainKeys Identified Mail (DKIM) qui permet l’authentification du domaine de messagerie d’un mail à l’aide d’une signature cryptographique
-	• Domain-based Message Authentication, Reporting and Conformance (DMARC) qui permet notamment à une entité de définir une politique de traitement de ses mails envoyés en fonction des résultats de conformité SPF et DKIM
-Si l’entité (ou son prestataire) ne maitrise pas ces éléments, il est conseillé de se faire accompagner par un prestataire spécialisé.</t>
-  </si>
-  <si>
-    <t>## **ATTAQUE CIBLÉE**
-## Chiffrement de connexion 
-Minimum attendu pour cocher la 4ème réponse :
-	• Mot de passe de 20 caractères minimum ;
-	• Chiffrement robuste de la connexion wifi, a minima WPA2 ;
-	• Pas d'accès au réseau interne pour les visiteurs via le Wi-Fi (SSID différent, sous-réseau différent ou Wi-Fi non accessible au visiteur).</t>
-  </si>
-  <si>
-    <t>## **ATTAQUE CIBLÉE**
-## Accès aux serveurs
-Pour sélectionner “Oui”, l’accès aux serveurs doit être à minima protégé par une porte fermée à clef dont la clef n’est accessible qu’aux personnes légitimes.
-## Référent sûreté de gendarmerie et de police
-Si c’est jugé nécessaire, l’entité peut être mise en relation avec un référent sûreté physique de la gendarmerie et de la police.</t>
-  </si>
-  <si>
-    <t>## Actions de sensibilisation 
-Exemple d'actions de sensibilisation :
-	• Campagne d'affichage, mails d'information, conférence de sensibilisation
-	• Sensibilisation ciblée du CODIR, sensibilisation aux risques d'escroquerie au faux ordre de virement et fraude au président
-	• Sensibilisation en ligne des utilisateurs, ex : https://www.cybermalveillance.gouv.fr/sens-cyber/apprendre
-	• Campagne de faux phishing
-	• Formation en ligne, ex : [https://secnumacademie.gouv.fr](https://secnumacademie.gouv.fr/) , https://pix.fr/actualites/partenariat-pix-anssi-cybermalveillance
-Ressources de sensibilisation gratuites : https://www.cybermalveillance.gouv.fr/tous-nos-contenus/actualites/liste-des-ressources-mises-a-disposition Des actions de sensibilisation gratuites peuvent être menées en sollicitant la police ou la gendarmerie nationales : https://www.masecurite.interieur.gouv.fr/fr</t>
-  </si>
-  <si>
-    <t>## **ATTAQUE CIBLÉE**
-## Passeport de conseils cyber aux voyageurs
-L’ANSSI a publié un guide pour sensibiliser les collaborateurs aux bonnes pratiques de cybersécurité durant les déplacements : https://cyber.gouv.fr/publications/bonnes-pratiques-lusage-des-professionnels-en-deplacement</t>
-  </si>
-  <si>
-    <t>## Entités publiques
-Les entités publiques sont éligibles au service gratuit SILENE de l’ANSSI qui permet d’identifier la surface d’attaque des services exposés sur Internet. Pour y accéder, l’entité est invitée à s'orienter vers le service ANSSI https://club.ssi.gouv.fr/.
-## Suivi des alertes et des vulnérabilités
-Le suivi des alertes et des vulnérabilités consiste à se tenir informé des vulnérabilités techniques de cybersécurité critiques pouvant affecter son système d’information (selon les équipements et les systèmes utilisés). Des services gratuits centralisent et répertorient ces vulnérabilités, par exemple le site du [CERT-FR de l'ANSSI.](https://www.cert.ssi.gouv.fr/)</t>
-  </si>
-  <si>
-    <t>## Jeu de sauvegarde isolé 
-Le jeu de sauvegarde isolé (ou sanctuarisé) peut être réalisé de plusieurs manières :
-	• sur un périphérique de stockage déconnecté du réseau (bandes, disques durs externes, clefs usb),
-	• dans un cloud externe privé, non interconnecté à l'environnement bureautique, via une authentification spécifique,
-	• sur un serveur ou média déconnecté physiquement et/ou logiquement à l’issue de chaque sauvegarde.
-Ce jeu de sauvegarde ne doit donc pas être accessible via l’Active Directory (ou autre service d'annuaire centralisé).
-## Sauvegarde des ressources hébergées en cloud
-Il convient aussi de s’assurer que les mécanismes de sauvegarde mis en œuvre par l’entité (ou par son prestataire) / prennent également en compte les ressources bureautiques et/ou métiers qui sont seulement hébergées dans des environnements cloud.</t>
-  </si>
-  <si>
-    <t>## Organisation de gestion de crise
-Une organisation de gestion de crise doit à minima identifier les priorités métier à rétablir en cas de crise, des fiches réflexes opérationnelles garantissant la continuité d'activité au travers de modes dégradés défini avec les métiers (ex : assurer la paie, poursuivre la production, gestion des agendas, etc.), des moyens et modalités de communication de crise.</t>
   </si>
 </sst>
 </file>
@@ -3196,7 +3196,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>577</v>
+        <v>511</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -3246,7 +3246,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>549</v>
+        <v>483</v>
       </c>
     </row>
   </sheetData>
@@ -3269,10 +3269,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>550</v>
+        <v>484</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>551</v>
+        <v>485</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -3347,7 +3347,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>577</v>
+        <v>511</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -3402,7 +3402,7 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>578</v>
+        <v>512</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>10</v>
@@ -3465,7 +3465,7 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
-        <v>579</v>
+        <v>513</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2" t="s">
@@ -3494,7 +3494,7 @@
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
-        <v>580</v>
+        <v>514</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2" t="s">
@@ -3577,7 +3577,7 @@
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
-        <v>581</v>
+        <v>515</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2" t="s">
@@ -3606,7 +3606,7 @@
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2" t="s">
-        <v>582</v>
+        <v>516</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2" t="s">
@@ -3635,7 +3635,7 @@
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2" t="s">
-        <v>583</v>
+        <v>517</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2" t="s">
@@ -3664,7 +3664,7 @@
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2" t="s">
-        <v>584</v>
+        <v>518</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2" t="s">
@@ -3768,7 +3768,7 @@
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
-        <v>585</v>
+        <v>519</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2" t="s">
@@ -3799,7 +3799,7 @@
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
-        <v>586</v>
+        <v>520</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2" t="s">
@@ -3830,7 +3830,7 @@
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
-        <v>587</v>
+        <v>521</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2" t="s">
@@ -3861,7 +3861,7 @@
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
-        <v>588</v>
+        <v>522</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2" t="s">
@@ -3892,7 +3892,7 @@
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2" t="s">
-        <v>589</v>
+        <v>523</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2" t="s">
@@ -3923,7 +3923,7 @@
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2" t="s">
-        <v>590</v>
+        <v>524</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2" t="s">
@@ -3975,7 +3975,7 @@
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2" t="s">
-        <v>591</v>
+        <v>525</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2" t="s">
@@ -4006,7 +4006,7 @@
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2" t="s">
-        <v>592</v>
+        <v>526</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2" t="s">
@@ -4037,7 +4037,7 @@
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2" t="s">
-        <v>592</v>
+        <v>526</v>
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2" t="s">
@@ -4068,7 +4068,7 @@
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2" t="s">
-        <v>593</v>
+        <v>527</v>
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2" t="s">
@@ -4099,7 +4099,7 @@
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2" t="s">
-        <v>594</v>
+        <v>528</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2" t="s">
@@ -4130,7 +4130,7 @@
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2" t="s">
-        <v>595</v>
+        <v>529</v>
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2" t="s">
@@ -4161,7 +4161,7 @@
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2" t="s">
-        <v>596</v>
+        <v>530</v>
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2" t="s">
@@ -4192,7 +4192,7 @@
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2" t="s">
-        <v>597</v>
+        <v>531</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2" t="s">
@@ -4223,7 +4223,7 @@
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2" t="s">
-        <v>598</v>
+        <v>532</v>
       </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2" t="s">
@@ -4254,7 +4254,7 @@
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2" t="s">
-        <v>599</v>
+        <v>533</v>
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2" t="s">
@@ -4285,7 +4285,7 @@
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="2" t="s">
-        <v>600</v>
+        <v>534</v>
       </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2" t="s">
@@ -4337,7 +4337,7 @@
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2" t="s">
-        <v>601</v>
+        <v>535</v>
       </c>
       <c r="G33" s="2"/>
       <c r="H33" s="2" t="s">
@@ -4368,7 +4368,7 @@
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2" t="s">
-        <v>599</v>
+        <v>533</v>
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2" t="s">
@@ -4399,7 +4399,7 @@
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="2" t="s">
-        <v>602</v>
+        <v>536</v>
       </c>
       <c r="G35" s="2"/>
       <c r="H35" s="2" t="s">
@@ -4430,7 +4430,7 @@
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2" t="s">
-        <v>599</v>
+        <v>533</v>
       </c>
       <c r="G36" s="2"/>
       <c r="H36" s="2" t="s">
@@ -4461,7 +4461,7 @@
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="2" t="s">
-        <v>603</v>
+        <v>537</v>
       </c>
       <c r="G37" s="2"/>
       <c r="H37" s="2" t="s">
@@ -4492,7 +4492,7 @@
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2" t="s">
-        <v>604</v>
+        <v>538</v>
       </c>
       <c r="G38" s="2"/>
       <c r="H38" s="2" t="s">
@@ -4523,7 +4523,7 @@
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="2" t="s">
-        <v>605</v>
+        <v>539</v>
       </c>
       <c r="G39" s="2"/>
       <c r="H39" s="2" t="s">
@@ -4575,7 +4575,7 @@
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="2" t="s">
-        <v>606</v>
+        <v>540</v>
       </c>
       <c r="G41" s="2"/>
       <c r="H41" s="2" t="s">
@@ -4664,7 +4664,7 @@
       </c>
       <c r="E44" s="2"/>
       <c r="F44" s="2" t="s">
-        <v>607</v>
+        <v>541</v>
       </c>
       <c r="G44" s="2"/>
       <c r="H44" s="2" t="s">
@@ -4695,7 +4695,7 @@
       </c>
       <c r="E45" s="2"/>
       <c r="F45" s="2" t="s">
-        <v>608</v>
+        <v>542</v>
       </c>
       <c r="G45" s="2"/>
       <c r="H45" s="2" t="s">
@@ -4726,7 +4726,7 @@
       </c>
       <c r="E46" s="2"/>
       <c r="F46" s="2" t="s">
-        <v>609</v>
+        <v>543</v>
       </c>
       <c r="G46" s="2"/>
       <c r="H46" s="2" t="s">
@@ -4757,7 +4757,7 @@
       </c>
       <c r="E47" s="2"/>
       <c r="F47" s="2" t="s">
-        <v>610</v>
+        <v>544</v>
       </c>
       <c r="G47" s="2"/>
       <c r="H47" s="2" t="s">
@@ -4788,7 +4788,7 @@
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="2" t="s">
-        <v>611</v>
+        <v>545</v>
       </c>
       <c r="G48" s="2"/>
       <c r="H48" s="2" t="s">
@@ -4819,7 +4819,7 @@
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="2" t="s">
-        <v>612</v>
+        <v>546</v>
       </c>
       <c r="G49" s="2"/>
       <c r="H49" s="2" t="s">
@@ -4871,7 +4871,7 @@
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="2" t="s">
-        <v>613</v>
+        <v>547</v>
       </c>
       <c r="G51" s="2"/>
       <c r="H51" s="2" t="s">
@@ -4902,7 +4902,7 @@
       </c>
       <c r="E52" s="2"/>
       <c r="F52" s="2" t="s">
-        <v>614</v>
+        <v>548</v>
       </c>
       <c r="G52" s="2"/>
       <c r="H52" s="2" t="s">
@@ -4983,7 +4983,7 @@
       </c>
       <c r="E55" s="2"/>
       <c r="F55" s="2" t="s">
-        <v>615</v>
+        <v>549</v>
       </c>
       <c r="G55" s="2"/>
       <c r="H55" s="2" t="s">
@@ -5014,7 +5014,7 @@
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="2" t="s">
-        <v>616</v>
+        <v>550</v>
       </c>
       <c r="G56" s="2"/>
       <c r="H56" s="2" t="s">
@@ -5161,7 +5161,7 @@
       </c>
       <c r="E61" s="2"/>
       <c r="F61" s="2" t="s">
-        <v>617</v>
+        <v>551</v>
       </c>
       <c r="G61" s="2"/>
       <c r="H61" s="2" t="s">
@@ -5248,7 +5248,7 @@
         <v>277</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>552</v>
+        <v>486</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -5338,7 +5338,7 @@
         <v>285</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>553</v>
+        <v>487</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -5356,7 +5356,7 @@
         <v>286</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>553</v>
+        <v>487</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -5374,7 +5374,7 @@
         <v>287</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>553</v>
+        <v>487</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
@@ -5404,7 +5404,7 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
-        <v>553</v>
+        <v>487</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -5420,7 +5420,7 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
-        <v>554</v>
+        <v>488</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -5436,7 +5436,7 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
-        <v>555</v>
+        <v>489</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -5452,7 +5452,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
-        <v>556</v>
+        <v>490</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -5468,7 +5468,7 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
-        <v>557</v>
+        <v>491</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -5484,7 +5484,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
-        <v>557</v>
+        <v>491</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -5500,7 +5500,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
-        <v>558</v>
+        <v>492</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -5516,7 +5516,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2" t="s">
-        <v>559</v>
+        <v>493</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
@@ -5532,7 +5532,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2" t="s">
-        <v>556</v>
+        <v>490</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -5548,7 +5548,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2" t="s">
-        <v>556</v>
+        <v>490</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -5564,7 +5564,7 @@
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2" t="s">
-        <v>560</v>
+        <v>494</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -5580,7 +5580,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2" t="s">
-        <v>561</v>
+        <v>495</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -5596,7 +5596,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2" t="s">
-        <v>554</v>
+        <v>488</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -5612,7 +5612,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2" t="s">
-        <v>562</v>
+        <v>496</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -5628,7 +5628,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2" t="s">
-        <v>563</v>
+        <v>497</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -5644,7 +5644,7 @@
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2" t="s">
-        <v>556</v>
+        <v>490</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -5660,7 +5660,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2" t="s">
-        <v>556</v>
+        <v>490</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -5676,7 +5676,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2" t="s">
-        <v>557</v>
+        <v>491</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -5692,7 +5692,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2" t="s">
-        <v>554</v>
+        <v>488</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -5708,7 +5708,7 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2" t="s">
-        <v>556</v>
+        <v>490</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -5724,7 +5724,7 @@
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2" t="s">
-        <v>557</v>
+        <v>491</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -5740,7 +5740,7 @@
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2" t="s">
-        <v>563</v>
+        <v>497</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -5756,7 +5756,7 @@
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2" t="s">
-        <v>553</v>
+        <v>487</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -5772,7 +5772,7 @@
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2" t="s">
-        <v>557</v>
+        <v>491</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -5788,7 +5788,7 @@
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2" t="s">
-        <v>559</v>
+        <v>493</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -5806,7 +5806,7 @@
         <v>312</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>553</v>
+        <v>487</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -5822,7 +5822,7 @@
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2" t="s">
-        <v>557</v>
+        <v>491</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -5838,7 +5838,7 @@
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2" t="s">
-        <v>557</v>
+        <v>491</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -5854,7 +5854,7 @@
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2" t="s">
-        <v>563</v>
+        <v>497</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -5870,7 +5870,7 @@
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2" t="s">
-        <v>564</v>
+        <v>498</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -5886,7 +5886,7 @@
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2" t="s">
-        <v>556</v>
+        <v>490</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -5902,7 +5902,7 @@
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
       <c r="F42" s="2" t="s">
-        <v>563</v>
+        <v>497</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -5918,7 +5918,7 @@
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
       <c r="F43" s="2" t="s">
-        <v>563</v>
+        <v>497</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -5934,7 +5934,7 @@
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
       <c r="F44" s="2" t="s">
-        <v>563</v>
+        <v>497</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -5950,7 +5950,7 @@
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
       <c r="F45" s="2" t="s">
-        <v>557</v>
+        <v>491</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -5966,7 +5966,7 @@
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2" t="s">
-        <v>559</v>
+        <v>493</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -5982,7 +5982,7 @@
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
       <c r="F47" s="2" t="s">
-        <v>557</v>
+        <v>491</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -5998,7 +5998,7 @@
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
       <c r="F48" s="2" t="s">
-        <v>554</v>
+        <v>488</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -6016,7 +6016,7 @@
         <v>324</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>554</v>
+        <v>488</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -6032,7 +6032,7 @@
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
       <c r="F50" s="2" t="s">
-        <v>559</v>
+        <v>493</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -6048,7 +6048,7 @@
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
       <c r="F51" s="2" t="s">
-        <v>559</v>
+        <v>493</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -6064,7 +6064,7 @@
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
       <c r="F52" s="2" t="s">
-        <v>559</v>
+        <v>493</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -6080,7 +6080,7 @@
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
       <c r="F53" s="2" t="s">
-        <v>559</v>
+        <v>493</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -6096,7 +6096,7 @@
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
       <c r="F54" s="2" t="s">
-        <v>557</v>
+        <v>491</v>
       </c>
     </row>
   </sheetData>
@@ -6185,7 +6185,7 @@
         <v>66</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>571</v>
+        <v>505</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -6195,7 +6195,7 @@
         <v>70</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>572</v>
+        <v>506</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -6225,7 +6225,7 @@
         <v>191</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>565</v>
+        <v>499</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -6235,7 +6235,7 @@
         <v>196</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>566</v>
+        <v>500</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -6245,7 +6245,7 @@
         <v>251</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>567</v>
+        <v>501</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -6255,7 +6255,7 @@
         <v>256</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>568</v>
+        <v>502</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -6265,7 +6265,7 @@
         <v>261</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>569</v>
+        <v>503</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -6275,7 +6275,7 @@
         <v>266</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>570</v>
+        <v>504</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -6285,7 +6285,7 @@
         <v>330</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>573</v>
+        <v>507</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -6295,7 +6295,7 @@
         <v>331</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>574</v>
+        <v>508</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -6305,7 +6305,7 @@
         <v>332</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>575</v>
+        <v>509</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -6315,7 +6315,7 @@
         <v>333</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>576</v>
+        <v>510</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -6407,1029 +6407,1029 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>339</v>
+        <v>552</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>340</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>341</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>342</v>
+        <v>553</v>
       </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="216" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>345</v>
+        <v>554</v>
       </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>348</v>
+        <v>555</v>
       </c>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>351</v>
+        <v>556</v>
       </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" ht="144" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>354</v>
+        <v>557</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>357</v>
+        <v>558</v>
       </c>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>357</v>
+        <v>558</v>
       </c>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" ht="144" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>362</v>
+        <v>559</v>
       </c>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" ht="144" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>362</v>
+        <v>559</v>
       </c>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
-        <v>367</v>
+        <v>560</v>
       </c>
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
-        <v>370</v>
+        <v>561</v>
       </c>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
-        <v>373</v>
+        <v>562</v>
       </c>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>374</v>
+        <v>363</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>375</v>
+        <v>364</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
-        <v>376</v>
+        <v>563</v>
       </c>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>377</v>
+        <v>365</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>378</v>
+        <v>366</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>379</v>
+        <v>564</v>
       </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>380</v>
+        <v>367</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>382</v>
+        <v>565</v>
       </c>
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>383</v>
+        <v>369</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>384</v>
+        <v>370</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2" t="s">
-        <v>385</v>
+        <v>566</v>
       </c>
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>386</v>
+        <v>371</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>387</v>
+        <v>372</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2" t="s">
-        <v>388</v>
+        <v>567</v>
       </c>
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>389</v>
+        <v>373</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>390</v>
+        <v>374</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2" t="s">
-        <v>391</v>
+        <v>568</v>
       </c>
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>392</v>
+        <v>375</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>393</v>
+        <v>376</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2" t="s">
-        <v>394</v>
+        <v>569</v>
       </c>
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>395</v>
+        <v>377</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>396</v>
+        <v>378</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2" t="s">
-        <v>397</v>
+        <v>570</v>
       </c>
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>398</v>
+        <v>379</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>399</v>
+        <v>380</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2" t="s">
-        <v>400</v>
+        <v>571</v>
       </c>
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" ht="360" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>401</v>
+        <v>381</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2" t="s">
-        <v>403</v>
+        <v>572</v>
       </c>
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6" ht="216" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>404</v>
+        <v>383</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>405</v>
+        <v>384</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2" t="s">
-        <v>406</v>
+        <v>573</v>
       </c>
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>407</v>
+        <v>385</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>408</v>
+        <v>386</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2" t="s">
-        <v>409</v>
+        <v>574</v>
       </c>
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6" ht="144" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>410</v>
+        <v>387</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>411</v>
+        <v>388</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2" t="s">
-        <v>412</v>
+        <v>575</v>
       </c>
       <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>413</v>
+        <v>389</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>414</v>
+        <v>390</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2" t="s">
-        <v>415</v>
+        <v>576</v>
       </c>
       <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>416</v>
+        <v>391</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>417</v>
+        <v>392</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2" t="s">
-        <v>418</v>
+        <v>577</v>
       </c>
       <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>419</v>
+        <v>393</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>420</v>
+        <v>394</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2" t="s">
-        <v>421</v>
+        <v>578</v>
       </c>
       <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>422</v>
+        <v>395</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>423</v>
+        <v>396</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2" t="s">
-        <v>424</v>
+        <v>579</v>
       </c>
       <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>425</v>
+        <v>397</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>426</v>
+        <v>398</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2" t="s">
-        <v>427</v>
+        <v>580</v>
       </c>
       <c r="F32" s="1"/>
     </row>
     <row r="33" spans="1:6" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>428</v>
+        <v>399</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>429</v>
+        <v>400</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2" t="s">
-        <v>430</v>
+        <v>581</v>
       </c>
       <c r="F33" s="1"/>
     </row>
     <row r="34" spans="1:6" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>431</v>
+        <v>401</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>432</v>
+        <v>402</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2" t="s">
-        <v>433</v>
+        <v>582</v>
       </c>
       <c r="F34" s="1"/>
     </row>
     <row r="35" spans="1:6" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>434</v>
+        <v>403</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>435</v>
+        <v>404</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2" t="s">
-        <v>436</v>
+        <v>583</v>
       </c>
       <c r="F35" s="1"/>
     </row>
     <row r="36" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>437</v>
+        <v>405</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>438</v>
+        <v>406</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2" t="s">
-        <v>439</v>
+        <v>584</v>
       </c>
       <c r="F36" s="1"/>
     </row>
     <row r="37" spans="1:6" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>440</v>
+        <v>407</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>441</v>
+        <v>408</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2" t="s">
-        <v>436</v>
+        <v>583</v>
       </c>
       <c r="F37" s="1"/>
     </row>
     <row r="38" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>442</v>
+        <v>409</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>443</v>
+        <v>410</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2" t="s">
-        <v>439</v>
+        <v>584</v>
       </c>
       <c r="F38" s="1"/>
     </row>
     <row r="39" spans="1:6" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>444</v>
+        <v>411</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>445</v>
+        <v>412</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2" t="s">
-        <v>446</v>
+        <v>585</v>
       </c>
       <c r="F39" s="1"/>
     </row>
     <row r="40" spans="1:6" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>447</v>
+        <v>413</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>448</v>
+        <v>414</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2" t="s">
-        <v>449</v>
+        <v>586</v>
       </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="1:6" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>450</v>
+        <v>415</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>451</v>
+        <v>416</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2" t="s">
-        <v>446</v>
+        <v>585</v>
       </c>
       <c r="F41" s="1"/>
     </row>
     <row r="42" spans="1:6" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>452</v>
+        <v>417</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>453</v>
+        <v>418</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2" t="s">
-        <v>449</v>
+        <v>586</v>
       </c>
       <c r="F42" s="1"/>
     </row>
     <row r="43" spans="1:6" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>454</v>
+        <v>419</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>455</v>
+        <v>420</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2" t="s">
-        <v>456</v>
+        <v>587</v>
       </c>
       <c r="F43" s="1"/>
     </row>
     <row r="44" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>457</v>
+        <v>421</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>458</v>
+        <v>422</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2" t="s">
-        <v>459</v>
+        <v>588</v>
       </c>
       <c r="F44" s="1"/>
     </row>
     <row r="45" spans="1:6" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>460</v>
+        <v>423</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>461</v>
+        <v>424</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2" t="s">
-        <v>462</v>
+        <v>589</v>
       </c>
       <c r="F45" s="1"/>
     </row>
     <row r="46" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>463</v>
+        <v>425</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>464</v>
+        <v>426</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2" t="s">
-        <v>465</v>
+        <v>590</v>
       </c>
       <c r="F46" s="1"/>
     </row>
     <row r="47" spans="1:6" ht="216" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>466</v>
+        <v>427</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>467</v>
+        <v>428</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2" t="s">
-        <v>468</v>
+        <v>591</v>
       </c>
       <c r="F47" s="1"/>
     </row>
     <row r="48" spans="1:6" ht="144" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>469</v>
+        <v>429</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>470</v>
+        <v>430</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2" t="s">
-        <v>471</v>
+        <v>592</v>
       </c>
       <c r="F48" s="1"/>
     </row>
     <row r="49" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>472</v>
+        <v>431</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>473</v>
+        <v>432</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2" t="s">
-        <v>474</v>
+        <v>593</v>
       </c>
       <c r="F49" s="1"/>
     </row>
     <row r="50" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>475</v>
+        <v>433</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>476</v>
+        <v>434</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
       <c r="E50" s="2" t="s">
-        <v>477</v>
+        <v>594</v>
       </c>
       <c r="F50" s="1"/>
     </row>
     <row r="51" spans="1:6" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>478</v>
+        <v>435</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>479</v>
+        <v>436</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
       <c r="E51" s="2" t="s">
-        <v>480</v>
+        <v>595</v>
       </c>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>481</v>
+        <v>437</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>482</v>
+        <v>438</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
       <c r="E52" s="2" t="s">
-        <v>483</v>
+        <v>596</v>
       </c>
       <c r="F52" s="1"/>
     </row>
     <row r="53" spans="1:6" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>484</v>
+        <v>439</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>485</v>
+        <v>440</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
       <c r="E53" s="2" t="s">
-        <v>486</v>
+        <v>597</v>
       </c>
       <c r="F53" s="1"/>
     </row>
     <row r="54" spans="1:6" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>487</v>
+        <v>441</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>488</v>
+        <v>442</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
       <c r="E54" s="2" t="s">
-        <v>489</v>
+        <v>598</v>
       </c>
       <c r="F54" s="1"/>
     </row>
     <row r="55" spans="1:6" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>490</v>
+        <v>443</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>491</v>
+        <v>444</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
       <c r="E55" s="2" t="s">
-        <v>492</v>
+        <v>599</v>
       </c>
       <c r="F55" s="1"/>
     </row>
     <row r="56" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>493</v>
+        <v>445</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>494</v>
+        <v>446</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
       <c r="E56" s="2" t="s">
-        <v>495</v>
+        <v>600</v>
       </c>
       <c r="F56" s="1"/>
     </row>
     <row r="57" spans="1:6" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>496</v>
+        <v>447</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>497</v>
+        <v>448</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
       <c r="E57" s="2" t="s">
-        <v>498</v>
+        <v>601</v>
       </c>
       <c r="F57" s="1"/>
     </row>
     <row r="58" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>499</v>
+        <v>449</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>500</v>
+        <v>450</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
       <c r="E58" s="2" t="s">
-        <v>501</v>
+        <v>602</v>
       </c>
       <c r="F58" s="1"/>
     </row>
     <row r="59" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>502</v>
+        <v>451</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>503</v>
+        <v>452</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
       <c r="E59" s="2" t="s">
-        <v>504</v>
+        <v>603</v>
       </c>
       <c r="F59" s="1"/>
     </row>
     <row r="60" spans="1:6" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>505</v>
+        <v>453</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>506</v>
+        <v>454</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
       <c r="E60" s="2" t="s">
-        <v>507</v>
+        <v>604</v>
       </c>
       <c r="F60" s="1"/>
     </row>
     <row r="61" spans="1:6" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>508</v>
+        <v>455</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>509</v>
+        <v>456</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
       <c r="E61" s="2" t="s">
-        <v>510</v>
+        <v>605</v>
       </c>
       <c r="F61" s="1"/>
     </row>
     <row r="62" spans="1:6" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>511</v>
+        <v>457</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>512</v>
+        <v>458</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
       <c r="E62" s="2" t="s">
-        <v>513</v>
+        <v>606</v>
       </c>
       <c r="F62" s="1"/>
     </row>
     <row r="63" spans="1:6" ht="216" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
-        <v>514</v>
+        <v>459</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>515</v>
+        <v>460</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
       <c r="E63" s="2" t="s">
-        <v>516</v>
+        <v>607</v>
       </c>
       <c r="F63" s="1"/>
     </row>
     <row r="64" spans="1:6" ht="144" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
-        <v>517</v>
+        <v>461</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>518</v>
+        <v>462</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
       <c r="E64" s="2" t="s">
-        <v>519</v>
+        <v>608</v>
       </c>
       <c r="F64" s="1"/>
     </row>
     <row r="65" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
-        <v>520</v>
+        <v>463</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>521</v>
+        <v>464</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
       <c r="E65" s="2" t="s">
-        <v>522</v>
+        <v>609</v>
       </c>
       <c r="F65" s="1"/>
     </row>
     <row r="66" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
-        <v>523</v>
+        <v>465</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>524</v>
+        <v>466</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
       <c r="E66" s="2" t="s">
-        <v>525</v>
+        <v>610</v>
       </c>
       <c r="F66" s="1"/>
     </row>
     <row r="67" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
-        <v>526</v>
+        <v>467</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>527</v>
+        <v>468</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
       <c r="E67" s="2" t="s">
-        <v>528</v>
+        <v>611</v>
       </c>
       <c r="F67" s="1"/>
     </row>
     <row r="68" spans="1:6" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
-        <v>529</v>
+        <v>469</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>530</v>
+        <v>470</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
       <c r="E68" s="2" t="s">
-        <v>531</v>
+        <v>612</v>
       </c>
       <c r="F68" s="1"/>
     </row>
     <row r="69" spans="1:6" ht="144" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
-        <v>532</v>
+        <v>471</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>533</v>
+        <v>472</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
       <c r="E69" s="2" t="s">
-        <v>534</v>
+        <v>613</v>
       </c>
       <c r="F69" s="1"/>
     </row>
     <row r="70" spans="1:6" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
-        <v>535</v>
+        <v>473</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>536</v>
+        <v>474</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
       <c r="E70" s="2" t="s">
-        <v>537</v>
+        <v>614</v>
       </c>
       <c r="F70" s="1"/>
     </row>
     <row r="71" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
-        <v>538</v>
+        <v>475</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>539</v>
+        <v>476</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
       <c r="E71" s="2" t="s">
-        <v>540</v>
+        <v>615</v>
       </c>
       <c r="F71" s="1"/>
     </row>
     <row r="72" spans="1:6" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
-        <v>541</v>
+        <v>477</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>536</v>
+        <v>474</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
       <c r="E72" s="2" t="s">
-        <v>537</v>
+        <v>614</v>
       </c>
       <c r="F72" s="1"/>
     </row>
     <row r="73" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
-        <v>542</v>
+        <v>478</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>539</v>
+        <v>476</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
       <c r="E73" s="2" t="s">
-        <v>540</v>
+        <v>615</v>
       </c>
       <c r="F73" s="1"/>
     </row>
     <row r="74" spans="1:6" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
-        <v>543</v>
+        <v>479</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>544</v>
+        <v>480</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
       <c r="E74" s="2" t="s">
-        <v>545</v>
+        <v>616</v>
       </c>
       <c r="F74" s="1"/>
     </row>
     <row r="75" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
-        <v>546</v>
+        <v>481</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>547</v>
+        <v>482</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
       <c r="E75" s="2" t="s">
-        <v>548</v>
+        <v>617</v>
       </c>
       <c r="F75" s="1"/>
     </row>

</xml_diff>

<commit_message>
[Excel] Fix "depth" for Sub-Questions
</commit_message>
<xml_diff>
--- a/tools/excel/anssi/anssi-mon-aide-cyber.xlsx
+++ b/tools/excel/anssi/anssi-mon-aide-cyber.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\tarkadia\projects\intuitem\ciso-assistant-community\tools\excel\anssi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD7F9F2-1504-411D-BE51-3CCB6D213F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA5DC1F-7048-45D8-BC42-7A2D195158A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1485" yWindow="-15870" windowWidth="25440" windowHeight="15990" tabRatio="882" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="-15750" windowWidth="12810" windowHeight="15855" tabRatio="882" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_meta" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="619">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="620">
   <si>
     <t>type</t>
   </si>
@@ -2794,6 +2794,9 @@
     http://www.apache.org/licenses/LICENSE-2.0
 Unless required by applicable law or agreed to in writing, software distributed under the License is distributed on an "AS IS" BASIS, WITHOUT WARRANTIES OR CONDITIONS OF ANY KIND, either express or implied.
 See the License for the specific language governing permissions and limitations under the License.</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
 </sst>
 </file>
@@ -3142,7 +3145,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -3384,7 +3387,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -3407,7 +3410,7 @@
       <c r="A1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -3440,7 +3443,7 @@
     </row>
     <row r="2" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -3463,7 +3466,7 @@
       <c r="A3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -3492,7 +3495,7 @@
       <c r="A4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -3521,7 +3524,7 @@
       <c r="A5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -3548,7 +3551,7 @@
       <c r="A6" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -3575,7 +3578,7 @@
       <c r="A7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -3604,7 +3607,7 @@
       <c r="A8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -3633,7 +3636,7 @@
       <c r="A9" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -3662,7 +3665,7 @@
       <c r="A10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -3691,8 +3694,8 @@
       <c r="A11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>38</v>
+      <c r="B11" s="1" t="s">
+        <v>619</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>64</v>
@@ -3718,8 +3721,8 @@
       <c r="A12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>38</v>
+      <c r="B12" s="1" t="s">
+        <v>619</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>68</v>
@@ -3743,7 +3746,7 @@
     </row>
     <row r="13" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -3766,7 +3769,7 @@
       <c r="A14" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -3797,7 +3800,7 @@
       <c r="A15" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -3828,7 +3831,7 @@
       <c r="A16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -3859,7 +3862,7 @@
       <c r="A17" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -3890,7 +3893,7 @@
       <c r="A18" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -3921,7 +3924,7 @@
       <c r="A19" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -3950,7 +3953,7 @@
     </row>
     <row r="20" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -3973,7 +3976,7 @@
       <c r="A21" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -4004,7 +4007,7 @@
       <c r="A22" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C22" s="2" t="s">
@@ -4035,7 +4038,7 @@
       <c r="A23" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C23" s="2" t="s">
@@ -4066,7 +4069,7 @@
       <c r="A24" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C24" s="2" t="s">
@@ -4097,7 +4100,7 @@
       <c r="A25" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C25" s="2" t="s">
@@ -4128,7 +4131,7 @@
       <c r="A26" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C26" s="2" t="s">
@@ -4159,7 +4162,7 @@
       <c r="A27" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C27" s="2" t="s">
@@ -4190,7 +4193,7 @@
       <c r="A28" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C28" s="2" t="s">
@@ -4221,7 +4224,7 @@
       <c r="A29" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C29" s="2" t="s">
@@ -4252,7 +4255,7 @@
       <c r="A30" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C30" s="2" t="s">
@@ -4283,7 +4286,7 @@
       <c r="A31" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C31" s="2" t="s">
@@ -4312,7 +4315,7 @@
     </row>
     <row r="32" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C32" s="2" t="s">
@@ -4335,7 +4338,7 @@
       <c r="A33" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C33" s="2" t="s">
@@ -4366,7 +4369,7 @@
       <c r="A34" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C34" s="2" t="s">
@@ -4397,7 +4400,7 @@
       <c r="A35" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C35" s="2" t="s">
@@ -4428,7 +4431,7 @@
       <c r="A36" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C36" s="2" t="s">
@@ -4459,7 +4462,7 @@
       <c r="A37" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C37" s="2" t="s">
@@ -4490,7 +4493,7 @@
       <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C38" s="2" t="s">
@@ -4521,7 +4524,7 @@
       <c r="A39" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C39" s="2" t="s">
@@ -4550,7 +4553,7 @@
     </row>
     <row r="40" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C40" s="2" t="s">
@@ -4573,7 +4576,7 @@
       <c r="A41" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C41" s="2" t="s">
@@ -4604,8 +4607,8 @@
       <c r="A42" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>38</v>
+      <c r="B42" s="1" t="s">
+        <v>619</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>189</v>
@@ -4633,8 +4636,8 @@
       <c r="A43" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>38</v>
+      <c r="B43" s="1" t="s">
+        <v>619</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>194</v>
@@ -4662,7 +4665,7 @@
       <c r="A44" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C44" s="2" t="s">
@@ -4693,7 +4696,7 @@
       <c r="A45" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C45" s="2" t="s">
@@ -4724,7 +4727,7 @@
       <c r="A46" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C46" s="2" t="s">
@@ -4755,7 +4758,7 @@
       <c r="A47" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C47" s="2" t="s">
@@ -4786,7 +4789,7 @@
       <c r="A48" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C48" s="2" t="s">
@@ -4817,7 +4820,7 @@
       <c r="A49" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C49" s="2" t="s">
@@ -4846,7 +4849,7 @@
     </row>
     <row r="50" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A50" s="2"/>
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C50" s="2" t="s">
@@ -4869,7 +4872,7 @@
       <c r="A51" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C51" s="2" t="s">
@@ -4900,7 +4903,7 @@
       <c r="A52" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B52" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C52" s="2" t="s">
@@ -4931,7 +4934,7 @@
       <c r="A53" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C53" s="2" t="s">
@@ -4958,7 +4961,7 @@
     </row>
     <row r="54" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A54" s="2"/>
-      <c r="B54" s="2" t="s">
+      <c r="B54" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C54" s="2" t="s">
@@ -4981,7 +4984,7 @@
       <c r="A55" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B55" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C55" s="2" t="s">
@@ -5012,7 +5015,7 @@
       <c r="A56" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B56" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C56" s="2" t="s">
@@ -5043,8 +5046,8 @@
       <c r="A57" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B57" s="2" t="s">
-        <v>38</v>
+      <c r="B57" s="1" t="s">
+        <v>619</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>249</v>
@@ -5072,8 +5075,8 @@
       <c r="A58" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B58" s="2" t="s">
-        <v>38</v>
+      <c r="B58" s="1" t="s">
+        <v>619</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>254</v>
@@ -5101,8 +5104,8 @@
       <c r="A59" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B59" s="2" t="s">
-        <v>38</v>
+      <c r="B59" s="1" t="s">
+        <v>619</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>259</v>
@@ -5130,8 +5133,8 @@
       <c r="A60" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B60" s="2" t="s">
-        <v>38</v>
+      <c r="B60" s="1" t="s">
+        <v>619</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>264</v>
@@ -5159,7 +5162,7 @@
       <c r="A61" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B61" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C61" s="2" t="s">

</xml_diff>

<commit_message>
[Excel + Script] Add "_dev_info" column
Informational column in order to ease future updates of the questionnaire
</commit_message>
<xml_diff>
--- a/tools/excel/anssi/anssi-mon-aide-cyber.xlsx
+++ b/tools/excel/anssi/anssi-mon-aide-cyber.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\tarkadia\projects\intuitem\ciso-assistant-community\tools\excel\anssi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A292B865-27C4-4701-9127-405463A536C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42DB6B3C-31CB-44A6-BCD4-EAB5DE2615C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="-15750" windowWidth="16365" windowHeight="15855" tabRatio="882" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1485" yWindow="-15870" windowWidth="25440" windowHeight="15990" tabRatio="882" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_meta" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="977" uniqueCount="567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="621">
   <si>
     <t>type</t>
   </si>
@@ -2639,6 +2639,168 @@
   <si>
     <t>3</t>
   </si>
+  <si>
+    <t>_dev_info</t>
+  </si>
+  <si>
+    <t>Question 1</t>
+  </si>
+  <si>
+    <t>Question 2</t>
+  </si>
+  <si>
+    <t>Question 3</t>
+  </si>
+  <si>
+    <t>Question 4</t>
+  </si>
+  <si>
+    <t>Question 5</t>
+  </si>
+  <si>
+    <t>Question 6</t>
+  </si>
+  <si>
+    <t>Question 7</t>
+  </si>
+  <si>
+    <t>Question 8</t>
+  </si>
+  <si>
+    <t>Question 8.1</t>
+  </si>
+  <si>
+    <t>Question 8.2</t>
+  </si>
+  <si>
+    <t>Question 9</t>
+  </si>
+  <si>
+    <t>Question 10</t>
+  </si>
+  <si>
+    <t>Question 11</t>
+  </si>
+  <si>
+    <t>Question 12</t>
+  </si>
+  <si>
+    <t>Question 13</t>
+  </si>
+  <si>
+    <t>Question 14</t>
+  </si>
+  <si>
+    <t>Question 15</t>
+  </si>
+  <si>
+    <t>Question 16</t>
+  </si>
+  <si>
+    <t>Question 17</t>
+  </si>
+  <si>
+    <t>Question 18</t>
+  </si>
+  <si>
+    <t>Question 19</t>
+  </si>
+  <si>
+    <t>Question 20</t>
+  </si>
+  <si>
+    <t>Question 21</t>
+  </si>
+  <si>
+    <t>Question 22</t>
+  </si>
+  <si>
+    <t>Question 23</t>
+  </si>
+  <si>
+    <t>Question 24</t>
+  </si>
+  <si>
+    <t>Question 25</t>
+  </si>
+  <si>
+    <t>Question 26</t>
+  </si>
+  <si>
+    <t>Question 27</t>
+  </si>
+  <si>
+    <t>Question 28</t>
+  </si>
+  <si>
+    <t>Question 29</t>
+  </si>
+  <si>
+    <t>Question 30</t>
+  </si>
+  <si>
+    <t>Question 31</t>
+  </si>
+  <si>
+    <t>Question 32</t>
+  </si>
+  <si>
+    <t>Question 33</t>
+  </si>
+  <si>
+    <t>Question 33.1</t>
+  </si>
+  <si>
+    <t>Question 33.2</t>
+  </si>
+  <si>
+    <t>Question 34</t>
+  </si>
+  <si>
+    <t>Question 35</t>
+  </si>
+  <si>
+    <t>Question 36</t>
+  </si>
+  <si>
+    <t>Question 37</t>
+  </si>
+  <si>
+    <t>Question 38</t>
+  </si>
+  <si>
+    <t>Question 39</t>
+  </si>
+  <si>
+    <t>Question 40</t>
+  </si>
+  <si>
+    <t>Question 41</t>
+  </si>
+  <si>
+    <t>Question 42</t>
+  </si>
+  <si>
+    <t>Question 43</t>
+  </si>
+  <si>
+    <t>Question 44</t>
+  </si>
+  <si>
+    <t>Question 44.1</t>
+  </si>
+  <si>
+    <t>Question 44.2</t>
+  </si>
+  <si>
+    <t>Question 44.3</t>
+  </si>
+  <si>
+    <t>Question 44.4</t>
+  </si>
+  <si>
+    <t>Question 45</t>
+  </si>
 </sst>
 </file>
 
@@ -2673,7 +2835,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -2682,6 +2844,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2986,7 +3149,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -3226,9 +3389,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K61"/>
+  <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -3245,9 +3408,10 @@
     <col min="9" max="9" width="152.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="95.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="117.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>26</v>
       </c>
@@ -3281,8 +3445,11 @@
       <c r="K1" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="L1" s="4" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -3302,8 +3469,9 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
-    </row>
-    <row r="3" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="L2" s="4"/>
+    </row>
+    <row r="3" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>37</v>
       </c>
@@ -3329,8 +3497,11 @@
         <v>39</v>
       </c>
       <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="L3" s="4" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>37</v>
       </c>
@@ -3356,8 +3527,11 @@
         <v>42</v>
       </c>
       <c r="K4" s="2"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L4" s="4" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>37</v>
       </c>
@@ -3381,8 +3555,11 @@
         <v>44</v>
       </c>
       <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L5" s="4" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>37</v>
       </c>
@@ -3406,8 +3583,11 @@
         <v>46</v>
       </c>
       <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="L6" s="4" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>37</v>
       </c>
@@ -3433,8 +3613,11 @@
         <v>48</v>
       </c>
       <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="L7" s="4" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>37</v>
       </c>
@@ -3460,8 +3643,11 @@
         <v>50</v>
       </c>
       <c r="K8" s="2"/>
-    </row>
-    <row r="9" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="L8" s="4" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>37</v>
       </c>
@@ -3487,8 +3673,11 @@
         <v>52</v>
       </c>
       <c r="K9" s="2"/>
-    </row>
-    <row r="10" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="L9" s="4" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>37</v>
       </c>
@@ -3514,8 +3703,11 @@
         <v>54</v>
       </c>
       <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L10" s="4" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>37</v>
       </c>
@@ -3539,8 +3731,11 @@
         <v>56</v>
       </c>
       <c r="K11" s="2"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L11" s="4" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>37</v>
       </c>
@@ -3564,8 +3759,11 @@
         <v>59</v>
       </c>
       <c r="K12" s="2"/>
-    </row>
-    <row r="13" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="L12" s="4" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="1" t="s">
         <v>5</v>
@@ -3585,8 +3783,9 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
-    </row>
-    <row r="14" spans="1:11" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="L13" s="4"/>
+    </row>
+    <row r="14" spans="1:12" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>37</v>
       </c>
@@ -3614,8 +3813,11 @@
       <c r="K14" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="L14" s="4" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>37</v>
       </c>
@@ -3643,8 +3845,11 @@
       <c r="K15" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="L15" s="4" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>37</v>
       </c>
@@ -3672,8 +3877,11 @@
       <c r="K16" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="L16" s="4" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>37</v>
       </c>
@@ -3701,8 +3909,11 @@
       <c r="K17" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="L17" s="4" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>37</v>
       </c>
@@ -3730,8 +3941,11 @@
       <c r="K18" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="L18" s="4" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>37</v>
       </c>
@@ -3759,8 +3973,11 @@
       <c r="K19" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="L19" s="4" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="1" t="s">
         <v>5</v>
@@ -3780,8 +3997,9 @@
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
-    </row>
-    <row r="21" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="L20" s="4"/>
+    </row>
+    <row r="21" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>37</v>
       </c>
@@ -3809,8 +4027,11 @@
       <c r="K21" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="L21" s="4" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>37</v>
       </c>
@@ -3838,8 +4059,11 @@
       <c r="K22" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="L22" s="4" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>37</v>
       </c>
@@ -3867,8 +4091,11 @@
       <c r="K23" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="L23" s="4" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>37</v>
       </c>
@@ -3896,8 +4123,11 @@
       <c r="K24" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="L24" s="4" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>37</v>
       </c>
@@ -3925,8 +4155,11 @@
       <c r="K25" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="L25" s="4" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>37</v>
       </c>
@@ -3954,8 +4187,11 @@
       <c r="K26" s="2" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" ht="144" x14ac:dyDescent="0.3">
+      <c r="L26" s="4" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="144" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>37</v>
       </c>
@@ -3983,8 +4219,11 @@
       <c r="K27" s="2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="L27" s="4" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>37</v>
       </c>
@@ -4012,8 +4251,11 @@
       <c r="K28" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="L28" s="4" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>37</v>
       </c>
@@ -4041,8 +4283,11 @@
       <c r="K29" s="2" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="L29" s="4" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>37</v>
       </c>
@@ -4070,8 +4315,11 @@
       <c r="K30" s="2" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="L30" s="4" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>37</v>
       </c>
@@ -4099,8 +4347,11 @@
       <c r="K31" s="2" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="L31" s="4" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="1" t="s">
         <v>5</v>
@@ -4120,8 +4371,9 @@
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
-    </row>
-    <row r="33" spans="1:11" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="L32" s="4"/>
+    </row>
+    <row r="33" spans="1:12" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>37</v>
       </c>
@@ -4149,8 +4401,11 @@
       <c r="K33" s="2" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="L33" s="4" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>37</v>
       </c>
@@ -4178,8 +4433,11 @@
       <c r="K34" s="2" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="L34" s="4" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>37</v>
       </c>
@@ -4207,8 +4465,11 @@
       <c r="K35" s="2" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="L35" s="4" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>37</v>
       </c>
@@ -4236,8 +4497,11 @@
       <c r="K36" s="2" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="L36" s="4" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>37</v>
       </c>
@@ -4265,8 +4529,11 @@
       <c r="K37" s="2" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="L37" s="4" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
@@ -4294,8 +4561,11 @@
       <c r="K38" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" ht="216" x14ac:dyDescent="0.3">
+      <c r="L38" s="4" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="216" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>37</v>
       </c>
@@ -4323,8 +4593,11 @@
       <c r="K39" s="2" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="L39" s="4" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
       <c r="B40" s="1" t="s">
         <v>5</v>
@@ -4344,8 +4617,9 @@
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
-    </row>
-    <row r="41" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="L40" s="4"/>
+    </row>
+    <row r="41" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>37</v>
       </c>
@@ -4373,8 +4647,11 @@
       <c r="K41" s="2" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="L41" s="4" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>37</v>
       </c>
@@ -4400,8 +4677,11 @@
       <c r="K42" s="2" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L42" s="4" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>37</v>
       </c>
@@ -4427,8 +4707,11 @@
       <c r="K43" s="2" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="L43" s="4" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>37</v>
       </c>
@@ -4456,8 +4739,11 @@
       <c r="K44" s="2" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="L44" s="4" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>37</v>
       </c>
@@ -4485,8 +4771,11 @@
       <c r="K45" s="2" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="L45" s="4" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>37</v>
       </c>
@@ -4514,8 +4803,11 @@
       <c r="K46" s="2" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="L46" s="4" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>37</v>
       </c>
@@ -4543,8 +4835,11 @@
       <c r="K47" s="2" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="L47" s="4" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>37</v>
       </c>
@@ -4572,8 +4867,11 @@
       <c r="K48" s="2" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" ht="144" x14ac:dyDescent="0.3">
+      <c r="L48" s="4" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="144" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>37</v>
       </c>
@@ -4601,8 +4899,11 @@
       <c r="K49" s="2" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="L49" s="4" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A50" s="2"/>
       <c r="B50" s="1" t="s">
         <v>5</v>
@@ -4622,8 +4923,9 @@
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
-    </row>
-    <row r="51" spans="1:11" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="L50" s="4"/>
+    </row>
+    <row r="51" spans="1:12" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>37</v>
       </c>
@@ -4651,8 +4953,11 @@
       <c r="K51" s="2" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="L51" s="4" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>37</v>
       </c>
@@ -4680,8 +4985,11 @@
       <c r="K52" s="2" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="L52" s="4" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>37</v>
       </c>
@@ -4707,8 +5015,11 @@
       <c r="K53" s="2" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="L53" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A54" s="2"/>
       <c r="B54" s="1" t="s">
         <v>5</v>
@@ -4728,8 +5039,9 @@
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
-    </row>
-    <row r="55" spans="1:11" ht="144" x14ac:dyDescent="0.3">
+      <c r="L54" s="4"/>
+    </row>
+    <row r="55" spans="1:12" ht="144" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>37</v>
       </c>
@@ -4757,8 +5069,11 @@
       <c r="K55" s="2" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="L55" s="4" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>37</v>
       </c>
@@ -4786,8 +5101,11 @@
       <c r="K56" s="2" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L56" s="4" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>37</v>
       </c>
@@ -4813,8 +5131,11 @@
       <c r="K57" s="2" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L57" s="4" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>37</v>
       </c>
@@ -4840,8 +5161,11 @@
       <c r="K58" s="2" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L58" s="4" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>37</v>
       </c>
@@ -4867,8 +5191,11 @@
       <c r="K59" s="2" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L59" s="4" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>37</v>
       </c>
@@ -4894,8 +5221,11 @@
       <c r="K60" s="2" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="L60" s="4" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>37</v>
       </c>
@@ -4922,6 +5252,9 @@
       </c>
       <c r="K61" s="2" t="s">
         <v>219</v>
+      </c>
+      <c r="L61" s="4" t="s">
+        <v>620</v>
       </c>
     </row>
   </sheetData>

</xml_diff>